<commit_message>
[schedule] Modifying Time Estimations
</commit_message>
<xml_diff>
--- a/schedules/Time Estimations.xlsx
+++ b/schedules/Time Estimations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dalia\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Freelance\FantasyLeague\Project\lagartija\schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="599" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="599" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Schedule" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="138">
   <si>
     <t>Página</t>
   </si>
@@ -435,6 +435,12 @@
   </si>
   <si>
     <t xml:space="preserve">Subject to Prizing Definitions </t>
+  </si>
+  <si>
+    <t>getNotifications(Start Date, End Date)</t>
+  </si>
+  <si>
+    <t>getNotifications/getNotifications(StartDate,EndDate)</t>
   </si>
 </sst>
 </file>
@@ -513,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -656,14 +662,134 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -674,150 +800,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1101,7 +1122,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,37 +1136,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="63" t="s">
+      <c r="B1" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="102" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="63"/>
-      <c r="F1" s="66" t="s">
+      <c r="E1" s="102"/>
+      <c r="F1" s="104" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
+      <c r="A2" s="103"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
       <c r="D2" s="29" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="67"/>
+      <c r="F2" s="105"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="89" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1165,7 +1186,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
+      <c r="A4" s="95"/>
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1181,12 +1202,12 @@
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
+      <c r="A5" s="95"/>
       <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>9</v>
+        <v>137</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>34</v>
@@ -1197,7 +1218,7 @@
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
+      <c r="A6" s="95"/>
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
@@ -1213,7 +1234,7 @@
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
+      <c r="A7" s="95"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
@@ -1229,7 +1250,7 @@
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="62"/>
+      <c r="A8" s="95"/>
       <c r="B8" s="8" t="s">
         <v>116</v>
       </c>
@@ -1243,7 +1264,7 @@
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="89" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -1252,7 +1273,7 @@
       <c r="C9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="88" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="33">
@@ -1263,14 +1284,14 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
+      <c r="A10" s="95"/>
       <c r="B10" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="60"/>
+      <c r="D10" s="85"/>
       <c r="E10" s="33">
         <v>0.3</v>
       </c>
@@ -1279,14 +1300,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="65"/>
+      <c r="A11" s="91"/>
       <c r="B11" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="56"/>
+      <c r="D11" s="87"/>
       <c r="E11" s="32" t="s">
         <v>24</v>
       </c>
@@ -1329,47 +1350,47 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="89" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="75" t="s">
+      <c r="C14" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="54">
+      <c r="E14" s="86">
         <v>0.5</v>
       </c>
-      <c r="F14" s="57" t="s">
+      <c r="F14" s="99" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
+      <c r="A15" s="95"/>
       <c r="B15" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="76"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="58"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="100"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="65"/>
+      <c r="A16" s="91"/>
       <c r="B16" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="77"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="59"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="101"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="89" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1378,7 +1399,7 @@
       <c r="C17" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="D17" s="86" t="s">
         <v>34</v>
       </c>
       <c r="E17" s="33">
@@ -1389,53 +1410,53 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="74"/>
+      <c r="A18" s="90"/>
       <c r="B18" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="55"/>
+      <c r="D18" s="88"/>
       <c r="E18" s="33" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="74"/>
+      <c r="A19" s="90"/>
       <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C19" t="s">
         <v>129</v>
       </c>
-      <c r="D19" s="55"/>
+      <c r="D19" s="88"/>
       <c r="E19" s="33">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="74"/>
+      <c r="A20" s="90"/>
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C20" t="s">
         <v>130</v>
       </c>
-      <c r="D20" s="55"/>
+      <c r="D20" s="88"/>
       <c r="E20" s="33">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="91"/>
       <c r="B21" s="19" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="56"/>
+      <c r="D21" s="87"/>
       <c r="E21" s="32" t="s">
         <v>24</v>
       </c>
@@ -1498,7 +1519,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="68" t="s">
+      <c r="A25" s="82" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1507,7 +1528,7 @@
       <c r="C25" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="54" t="s">
+      <c r="D25" s="86" t="s">
         <v>34</v>
       </c>
       <c r="E25" s="33">
@@ -1518,27 +1539,27 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="70"/>
+      <c r="A26" s="83"/>
       <c r="B26" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="60"/>
+      <c r="D26" s="85"/>
       <c r="E26" s="33">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="69"/>
+      <c r="A27" s="84"/>
       <c r="B27" s="19" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="56"/>
+      <c r="D27" s="87"/>
       <c r="E27" s="32">
         <v>2</v>
       </c>
@@ -1565,7 +1586,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="68" t="s">
+      <c r="A29" s="82" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1582,7 +1603,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="73"/>
+      <c r="A30" s="98"/>
       <c r="B30" s="3" t="s">
         <v>63</v>
       </c>
@@ -1597,14 +1618,14 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="73"/>
-      <c r="B31" s="71" t="s">
+      <c r="A31" s="98"/>
+      <c r="B31" s="96" t="s">
         <v>64</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="60">
+      <c r="D31" s="85">
         <v>3</v>
       </c>
       <c r="E31" s="33">
@@ -1615,25 +1636,25 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="73"/>
-      <c r="B32" s="71"/>
+      <c r="A32" s="98"/>
+      <c r="B32" s="96"/>
       <c r="C32" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="60"/>
+      <c r="D32" s="85"/>
       <c r="E32" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="73"/>
-      <c r="B33" s="71" t="s">
+      <c r="A33" s="98"/>
+      <c r="B33" s="96" t="s">
         <v>65</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="60">
+      <c r="D33" s="85">
         <v>3</v>
       </c>
       <c r="E33" s="33">
@@ -1644,12 +1665,12 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="73"/>
-      <c r="B34" s="71"/>
+      <c r="A34" s="98"/>
+      <c r="B34" s="96"/>
       <c r="C34" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="60"/>
+      <c r="D34" s="85"/>
       <c r="E34" s="33">
         <v>1</v>
       </c>
@@ -1658,7 +1679,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="69"/>
+      <c r="A35" s="84"/>
       <c r="B35" s="9" t="s">
         <v>59</v>
       </c>
@@ -1696,7 +1717,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="68" t="s">
+      <c r="A37" s="82" t="s">
         <v>76</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1716,7 +1737,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="70"/>
+      <c r="A38" s="83"/>
       <c r="B38" s="3" t="s">
         <v>78</v>
       </c>
@@ -1731,7 +1752,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="70"/>
+      <c r="A39" s="83"/>
       <c r="B39" s="3" t="s">
         <v>79</v>
       </c>
@@ -1746,8 +1767,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="70"/>
-      <c r="B40" s="71" t="s">
+      <c r="A40" s="83"/>
+      <c r="B40" s="96" t="s">
         <v>80</v>
       </c>
       <c r="C40" t="s">
@@ -1761,8 +1782,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="69"/>
-      <c r="B41" s="72"/>
+      <c r="A41" s="84"/>
+      <c r="B41" s="97"/>
       <c r="C41" s="9" t="s">
         <v>84</v>
       </c>
@@ -1793,7 +1814,7 @@
       <c r="F42" s="15"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="68" t="s">
+      <c r="A43" s="82" t="s">
         <v>92</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -1802,7 +1823,7 @@
       <c r="C43" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="54" t="s">
+      <c r="D43" s="86" t="s">
         <v>34</v>
       </c>
       <c r="E43" s="33">
@@ -1813,14 +1834,14 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="69"/>
+      <c r="A44" s="84"/>
       <c r="B44" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="56"/>
+      <c r="D44" s="87"/>
       <c r="E44" s="32" t="s">
         <v>24</v>
       </c>
@@ -1829,7 +1850,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="68" t="s">
+      <c r="A45" s="82" t="s">
         <v>93</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -1838,7 +1859,7 @@
       <c r="C45" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D45" s="54" t="s">
+      <c r="D45" s="86" t="s">
         <v>34</v>
       </c>
       <c r="E45" s="33">
@@ -1846,56 +1867,56 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="70"/>
+      <c r="A46" s="83"/>
       <c r="B46" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60" t="s">
+      <c r="D46" s="85"/>
+      <c r="E46" s="85" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="70"/>
+      <c r="A47" s="83"/>
       <c r="B47" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
+      <c r="D47" s="85"/>
+      <c r="E47" s="85"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="70"/>
+      <c r="A48" s="83"/>
       <c r="B48" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="60"/>
-      <c r="E48" s="60"/>
+      <c r="D48" s="85"/>
+      <c r="E48" s="85"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="69"/>
+      <c r="A49" s="84"/>
       <c r="B49" s="9" t="s">
         <v>86</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D49" s="56"/>
+      <c r="D49" s="87"/>
       <c r="E49" s="32">
         <v>3</v>
       </c>
       <c r="F49" s="9"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="68" t="s">
+      <c r="A50" s="82" t="s">
         <v>97</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -1904,7 +1925,7 @@
       <c r="C50" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D50" s="54" t="s">
+      <c r="D50" s="86" t="s">
         <v>34</v>
       </c>
       <c r="E50" s="33">
@@ -1912,27 +1933,27 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="70"/>
+      <c r="A51" s="83"/>
       <c r="B51" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D51" s="60"/>
+      <c r="D51" s="85"/>
       <c r="E51" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="69"/>
+      <c r="A52" s="84"/>
       <c r="B52" s="8" t="s">
         <v>98</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D52" s="56"/>
+      <c r="D52" s="87"/>
       <c r="E52" s="32">
         <v>2</v>
       </c>
@@ -2013,27 +2034,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D45:D49"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="D17:D21"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="A37:A41"/>
     <mergeCell ref="E14:E16"/>
     <mergeCell ref="F14:F16"/>
     <mergeCell ref="D9:D11"/>
@@ -2044,6 +2044,27 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D45:D49"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2052,10 +2073,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,54 +2085,54 @@
     <col min="2" max="2" width="29.85546875" style="53" customWidth="1"/>
     <col min="3" max="3" width="14" style="45" customWidth="1"/>
     <col min="4" max="5" width="11.42578125" style="50"/>
-    <col min="6" max="6" width="13.42578125" style="102" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="76" customWidth="1"/>
     <col min="7" max="8" width="11.42578125" style="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="100" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="100" t="s">
         <v>121</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="114" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="81"/>
-      <c r="F1" s="102" t="s">
+      <c r="E1" s="114"/>
+      <c r="F1" s="76" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="G1" s="114" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="81"/>
+      <c r="H1" s="114"/>
       <c r="I1" s="47" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="59"/>
-      <c r="B2" s="59"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
       <c r="C2" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="79" t="s">
+      <c r="E2" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="103" t="s">
+      <c r="F2" s="77" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="79" t="s">
+      <c r="G2" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="H2" s="79" t="s">
+      <c r="H2" s="58" t="s">
         <v>128</v>
       </c>
       <c r="I2" s="48" t="s">
@@ -2119,1492 +2140,1502 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C3" s="44"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="98">
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="113">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
+      <c r="A4" s="100"/>
       <c r="B4" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C4" s="49"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="62"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="95"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
+      <c r="A5" s="100"/>
       <c r="B5" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C5" s="49"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="62"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="95"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="59"/>
+      <c r="A6" s="101"/>
       <c r="B6" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C6" s="46"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="65"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="91"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C7" s="44">
         <v>1</v>
       </c>
-      <c r="D7" s="84">
+      <c r="D7" s="62">
         <v>43118</v>
       </c>
-      <c r="E7" s="84">
+      <c r="E7" s="62">
         <v>42753</v>
       </c>
-      <c r="F7" s="102">
-        <v>1</v>
-      </c>
-      <c r="G7" s="100">
+      <c r="F7" s="76">
+        <v>1</v>
+      </c>
+      <c r="G7" s="74">
         <v>43118</v>
       </c>
-      <c r="H7" s="94">
+      <c r="H7" s="69">
         <v>43118</v>
       </c>
-      <c r="I7" s="62"/>
+      <c r="I7" s="95"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="58"/>
+      <c r="A8" s="100"/>
       <c r="B8" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C8" s="49"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="95"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
+      <c r="A9" s="100"/>
       <c r="B9" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C9" s="49"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="89"/>
-      <c r="I9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="95"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="59"/>
+      <c r="A10" s="101"/>
       <c r="B10" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C10" s="46"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="103"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="65"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="91"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="86" t="s">
+      <c r="A11" s="99" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="80" t="s">
         <v>119</v>
       </c>
-      <c r="C11" s="44">
-        <v>1</v>
-      </c>
-      <c r="D11" s="84">
+      <c r="C11" s="54">
+        <v>1</v>
+      </c>
+      <c r="D11" s="62">
         <v>43118</v>
       </c>
-      <c r="E11" s="84">
+      <c r="E11" s="62">
+        <v>42753</v>
+      </c>
+      <c r="F11" s="76">
+        <v>1</v>
+      </c>
+      <c r="G11" s="74">
         <v>43118</v>
       </c>
-      <c r="F11" s="102">
-        <v>1</v>
-      </c>
-      <c r="G11" s="100">
+      <c r="H11" s="69">
         <v>43118</v>
       </c>
-      <c r="H11" s="94">
-        <v>43118</v>
-      </c>
-      <c r="I11" s="62"/>
+      <c r="I11" s="95"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="58"/>
-      <c r="B12" s="52" t="s">
+      <c r="A12" s="100"/>
+      <c r="B12" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="G12" s="101"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="62"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="95"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="58"/>
-      <c r="B13" s="52" t="s">
+      <c r="A13" s="100"/>
+      <c r="B13" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="G13" s="101"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="62"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="95"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="59"/>
+      <c r="A14" s="101"/>
       <c r="B14" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="95"/>
-      <c r="F14" s="103"/>
-      <c r="G14" s="99"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="65"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="91"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="86" t="s">
+      <c r="A15" s="99" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C15" s="44">
         <v>1</v>
       </c>
-      <c r="D15" s="94">
+      <c r="D15" s="62">
         <v>43118</v>
       </c>
-      <c r="E15" s="94">
+      <c r="E15" s="62">
         <v>43118</v>
       </c>
-      <c r="F15" s="102">
-        <v>1</v>
-      </c>
-      <c r="G15" s="100">
+      <c r="F15" s="76">
+        <v>1</v>
+      </c>
+      <c r="G15" s="74">
         <v>43118</v>
       </c>
-      <c r="H15" s="94">
+      <c r="H15" s="69">
         <v>43118</v>
       </c>
-      <c r="I15" s="62"/>
+      <c r="I15" s="95"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="58"/>
+      <c r="A16" s="100"/>
       <c r="B16" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C16" s="49"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="84"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="82"/>
-      <c r="I16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="95"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="58"/>
+      <c r="A17" s="100"/>
       <c r="B17" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C17" s="49"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="84"/>
-      <c r="G17" s="101"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="95"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="59"/>
+      <c r="A18" s="101"/>
       <c r="B18" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C18" s="46"/>
-      <c r="D18" s="95"/>
-      <c r="E18" s="95"/>
-      <c r="F18" s="103"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="79"/>
-      <c r="I18" s="65"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="91"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="86" t="s">
+      <c r="A19" s="99" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C19" s="44">
         <v>1</v>
       </c>
-      <c r="D19" s="94">
-        <v>43119</v>
-      </c>
-      <c r="E19" s="94">
-        <v>43119</v>
-      </c>
-      <c r="F19" s="102">
-        <v>1</v>
-      </c>
-      <c r="G19" s="100">
-        <v>43119</v>
-      </c>
-      <c r="H19" s="94">
-        <v>43119</v>
-      </c>
-      <c r="I19" s="62"/>
+      <c r="D19" s="69">
+        <v>43118</v>
+      </c>
+      <c r="E19" s="69">
+        <v>43118</v>
+      </c>
+      <c r="F19" s="76">
+        <v>1</v>
+      </c>
+      <c r="G19" s="74">
+        <v>43118</v>
+      </c>
+      <c r="H19" s="69">
+        <v>43118</v>
+      </c>
+      <c r="I19" s="95"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="58"/>
+      <c r="A20" s="100"/>
       <c r="B20" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C20" s="49"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="78"/>
-      <c r="G20" s="101"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="95"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
+      <c r="A21" s="100"/>
       <c r="B21" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C21" s="49"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="78"/>
-      <c r="G21" s="101"/>
-      <c r="H21" s="82"/>
-      <c r="I21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="95"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="59"/>
+      <c r="A22" s="101"/>
       <c r="B22" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C22" s="46"/>
-      <c r="D22" s="93"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="103"/>
-      <c r="G22" s="99"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="65"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="91"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="91" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="86" t="s">
+      <c r="A23" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C23" s="44">
         <v>1</v>
       </c>
-      <c r="D23" s="94">
+      <c r="D23" s="69">
         <v>43119</v>
       </c>
-      <c r="E23" s="94">
+      <c r="E23" s="69">
         <v>43119</v>
       </c>
-      <c r="F23" s="102">
-        <v>1</v>
-      </c>
-      <c r="G23" s="100">
+      <c r="F23" s="76">
+        <v>1</v>
+      </c>
+      <c r="G23" s="74">
         <v>43119</v>
       </c>
-      <c r="H23" s="94">
+      <c r="H23" s="69">
         <v>43119</v>
       </c>
-      <c r="I23" s="62"/>
+      <c r="I23" s="95"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="85"/>
+      <c r="A24" s="100"/>
       <c r="B24" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C24" s="49"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="105"/>
-      <c r="G24" s="82"/>
-      <c r="H24" s="82"/>
-      <c r="I24" s="62"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="95"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="85"/>
+      <c r="A25" s="100"/>
       <c r="B25" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C25" s="49"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="105"/>
-      <c r="G25" s="82"/>
-      <c r="H25" s="82"/>
-      <c r="I25" s="62"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="95"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="92"/>
+      <c r="A26" s="101"/>
       <c r="B26" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C26" s="46"/>
-      <c r="D26" s="93"/>
-      <c r="E26" s="93"/>
-      <c r="F26" s="103"/>
-      <c r="G26" s="79"/>
-      <c r="H26" s="79"/>
-      <c r="I26" s="65"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="91"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="61" t="s">
-        <v>129</v>
-      </c>
-      <c r="B27" s="86" t="s">
+      <c r="A27" s="110" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C27" s="44">
         <v>1</v>
       </c>
-      <c r="D27" s="94">
-        <v>43120</v>
-      </c>
-      <c r="E27" s="94">
-        <v>43120</v>
-      </c>
-      <c r="F27" s="102">
-        <v>1</v>
-      </c>
-      <c r="G27" s="100">
-        <v>43120</v>
-      </c>
-      <c r="H27" s="88">
-        <v>43120</v>
-      </c>
-      <c r="I27" s="62"/>
+      <c r="D27" s="69">
+        <v>43119</v>
+      </c>
+      <c r="E27" s="69">
+        <v>43119</v>
+      </c>
+      <c r="F27" s="76">
+        <v>1</v>
+      </c>
+      <c r="G27" s="74">
+        <v>43119</v>
+      </c>
+      <c r="H27" s="69">
+        <v>43119</v>
+      </c>
+      <c r="I27" s="95"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="62"/>
+      <c r="A28" s="111"/>
       <c r="B28" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C28" s="49"/>
-      <c r="D28" s="96"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="105"/>
-      <c r="G28" s="82"/>
-      <c r="H28" s="82"/>
-      <c r="I28" s="62"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="95"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="62"/>
+      <c r="A29" s="111"/>
       <c r="B29" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C29" s="49"/>
-      <c r="D29" s="96"/>
-      <c r="E29" s="82"/>
-      <c r="F29" s="105"/>
-      <c r="G29" s="82"/>
-      <c r="H29" s="82"/>
-      <c r="I29" s="62"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="95"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
+      <c r="A30" s="112"/>
       <c r="B30" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C30" s="46"/>
-      <c r="D30" s="97"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="103"/>
-      <c r="G30" s="79"/>
-      <c r="H30" s="79"/>
-      <c r="I30" s="65"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="91"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="61" t="s">
-        <v>130</v>
-      </c>
-      <c r="B31" s="86" t="s">
+      <c r="A31" s="89" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C31" s="44">
         <v>1</v>
       </c>
-      <c r="D31" s="94">
+      <c r="D31" s="69">
         <v>43120</v>
       </c>
-      <c r="E31" s="94">
+      <c r="E31" s="69">
         <v>43120</v>
       </c>
-      <c r="F31" s="102">
-        <v>1</v>
-      </c>
-      <c r="G31" s="100">
+      <c r="F31" s="76">
+        <v>1</v>
+      </c>
+      <c r="G31" s="74">
         <v>43120</v>
       </c>
-      <c r="H31" s="88">
+      <c r="H31" s="65">
         <v>43120</v>
       </c>
-      <c r="I31" s="62"/>
+      <c r="I31" s="95"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="62"/>
+      <c r="A32" s="95"/>
       <c r="B32" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C32" s="49"/>
-      <c r="D32" s="96"/>
-      <c r="E32" s="82"/>
-      <c r="F32" s="105"/>
-      <c r="G32" s="82"/>
-      <c r="H32" s="82"/>
-      <c r="I32" s="62"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="95"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="62"/>
+      <c r="A33" s="95"/>
       <c r="B33" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C33" s="49"/>
-      <c r="D33" s="96"/>
-      <c r="E33" s="82"/>
-      <c r="F33" s="105"/>
-      <c r="G33" s="82"/>
-      <c r="H33" s="82"/>
-      <c r="I33" s="62"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="95"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="65"/>
+      <c r="A34" s="91"/>
       <c r="B34" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C34" s="46"/>
-      <c r="D34" s="97"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="103"/>
-      <c r="G34" s="79"/>
-      <c r="H34" s="79"/>
-      <c r="I34" s="65"/>
+      <c r="D34" s="72"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="91"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="91" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="86" t="s">
+      <c r="A35" s="89" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C35" s="44">
         <v>1</v>
       </c>
-      <c r="D35" s="94">
+      <c r="D35" s="69">
         <v>43120</v>
       </c>
-      <c r="E35" s="94">
+      <c r="E35" s="69">
         <v>43120</v>
       </c>
-      <c r="F35" s="102">
-        <v>1</v>
-      </c>
-      <c r="G35" s="100">
+      <c r="F35" s="76">
+        <v>1</v>
+      </c>
+      <c r="G35" s="74">
         <v>43120</v>
       </c>
-      <c r="H35" s="88">
+      <c r="H35" s="65">
         <v>43120</v>
       </c>
-      <c r="I35" s="62"/>
+      <c r="I35" s="95"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="85"/>
+      <c r="A36" s="95"/>
       <c r="B36" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C36" s="49"/>
-      <c r="D36" s="82"/>
-      <c r="E36" s="82"/>
-      <c r="F36" s="105"/>
-      <c r="G36" s="82"/>
-      <c r="H36" s="82"/>
-      <c r="I36" s="62"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="79"/>
+      <c r="G36" s="60"/>
+      <c r="H36" s="60"/>
+      <c r="I36" s="95"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="85"/>
+      <c r="A37" s="95"/>
       <c r="B37" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C37" s="49"/>
-      <c r="D37" s="82"/>
-      <c r="E37" s="82"/>
-      <c r="F37" s="105"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="82"/>
-      <c r="I37" s="62"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="79"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="95"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="92"/>
+      <c r="A38" s="91"/>
       <c r="B38" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C38" s="46"/>
-      <c r="D38" s="79"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="103"/>
-      <c r="G38" s="79"/>
-      <c r="H38" s="79"/>
-      <c r="I38" s="65"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="77"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="91"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="91" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" s="86" t="s">
+      <c r="A39" s="110" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C39" s="44">
         <v>1</v>
       </c>
-      <c r="D39" s="94">
-        <v>43121</v>
-      </c>
-      <c r="E39" s="94">
-        <v>43121</v>
-      </c>
-      <c r="F39" s="104">
-        <v>1</v>
-      </c>
-      <c r="G39" s="94">
-        <v>43121</v>
-      </c>
-      <c r="H39" s="94">
-        <v>43121</v>
-      </c>
-      <c r="I39" s="62"/>
+      <c r="D39" s="69">
+        <v>43120</v>
+      </c>
+      <c r="E39" s="69">
+        <v>43120</v>
+      </c>
+      <c r="F39" s="76">
+        <v>1</v>
+      </c>
+      <c r="G39" s="74">
+        <v>43120</v>
+      </c>
+      <c r="H39" s="65">
+        <v>43120</v>
+      </c>
+      <c r="I39" s="95"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="85"/>
+      <c r="A40" s="111"/>
       <c r="B40" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C40" s="49"/>
-      <c r="D40" s="96"/>
-      <c r="E40" s="82"/>
-      <c r="F40" s="105"/>
-      <c r="G40" s="82"/>
-      <c r="H40" s="82"/>
-      <c r="I40" s="62"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="60"/>
+      <c r="F40" s="79"/>
+      <c r="G40" s="60"/>
+      <c r="H40" s="60"/>
+      <c r="I40" s="95"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="85"/>
+      <c r="A41" s="111"/>
       <c r="B41" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C41" s="49"/>
-      <c r="D41" s="96"/>
-      <c r="E41" s="82"/>
-      <c r="F41" s="105"/>
-      <c r="G41" s="82"/>
-      <c r="H41" s="82"/>
-      <c r="I41" s="62"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="79"/>
+      <c r="G41" s="60"/>
+      <c r="H41" s="60"/>
+      <c r="I41" s="95"/>
     </row>
     <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="92"/>
+      <c r="A42" s="112"/>
       <c r="B42" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C42" s="46"/>
-      <c r="D42" s="97"/>
-      <c r="E42" s="79"/>
-      <c r="F42" s="103"/>
-      <c r="G42" s="79"/>
-      <c r="H42" s="79"/>
-      <c r="I42" s="65"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="77"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="91"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="91" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" s="86" t="s">
+      <c r="A43" s="110" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C43" s="44">
         <v>1</v>
       </c>
-      <c r="D43" s="94">
-        <v>43122</v>
-      </c>
-      <c r="E43" s="94">
-        <v>43122</v>
-      </c>
-      <c r="F43" s="104">
-        <v>1</v>
-      </c>
-      <c r="G43" s="94">
-        <v>43122</v>
-      </c>
-      <c r="H43" s="94">
-        <v>43122</v>
-      </c>
-      <c r="I43" s="62"/>
+      <c r="D43" s="69">
+        <v>43121</v>
+      </c>
+      <c r="E43" s="69">
+        <v>43121</v>
+      </c>
+      <c r="F43" s="78">
+        <v>1</v>
+      </c>
+      <c r="G43" s="69">
+        <v>43121</v>
+      </c>
+      <c r="H43" s="69">
+        <v>43121</v>
+      </c>
+      <c r="I43" s="95"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="85"/>
+      <c r="A44" s="111"/>
       <c r="B44" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C44" s="49"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="105"/>
-      <c r="G44" s="82"/>
-      <c r="H44" s="82"/>
-      <c r="I44" s="62"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="60"/>
+      <c r="F44" s="79"/>
+      <c r="G44" s="60"/>
+      <c r="H44" s="60"/>
+      <c r="I44" s="95"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="85"/>
+      <c r="A45" s="111"/>
       <c r="B45" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C45" s="49"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="82"/>
-      <c r="F45" s="105"/>
-      <c r="G45" s="82"/>
-      <c r="H45" s="82"/>
-      <c r="I45" s="62"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="60"/>
+      <c r="F45" s="79"/>
+      <c r="G45" s="60"/>
+      <c r="H45" s="60"/>
+      <c r="I45" s="95"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="92"/>
+      <c r="A46" s="112"/>
       <c r="B46" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C46" s="46"/>
-      <c r="D46" s="79"/>
-      <c r="E46" s="79"/>
-      <c r="F46" s="103"/>
-      <c r="G46" s="79"/>
-      <c r="H46" s="79"/>
-      <c r="I46" s="65"/>
+      <c r="D46" s="72"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="77"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="91"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="91" t="s">
-        <v>85</v>
-      </c>
-      <c r="B47" s="86" t="s">
+      <c r="A47" s="110" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C47" s="44">
         <v>1</v>
       </c>
-      <c r="D47" s="94">
+      <c r="D47" s="69">
         <v>43122</v>
       </c>
-      <c r="E47" s="94">
+      <c r="E47" s="69">
         <v>43122</v>
       </c>
-      <c r="F47" s="104">
-        <v>1</v>
-      </c>
-      <c r="G47" s="94">
+      <c r="F47" s="78">
+        <v>1</v>
+      </c>
+      <c r="G47" s="69">
         <v>43122</v>
       </c>
-      <c r="H47" s="94">
+      <c r="H47" s="69">
         <v>43122</v>
       </c>
-      <c r="I47" s="62"/>
+      <c r="I47" s="95"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="85"/>
+      <c r="A48" s="111"/>
       <c r="B48" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C48" s="49"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="82"/>
-      <c r="F48" s="105"/>
-      <c r="G48" s="82"/>
-      <c r="H48" s="82"/>
-      <c r="I48" s="62"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="60"/>
+      <c r="F48" s="79"/>
+      <c r="G48" s="60"/>
+      <c r="H48" s="60"/>
+      <c r="I48" s="95"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="85"/>
+      <c r="A49" s="111"/>
       <c r="B49" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C49" s="49"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="105"/>
-      <c r="G49" s="82"/>
-      <c r="H49" s="82"/>
-      <c r="I49" s="62"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="60"/>
+      <c r="F49" s="79"/>
+      <c r="G49" s="60"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="95"/>
     </row>
     <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="92"/>
+      <c r="A50" s="112"/>
       <c r="B50" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C50" s="46"/>
-      <c r="D50" s="79"/>
-      <c r="E50" s="79"/>
-      <c r="F50" s="103"/>
-      <c r="G50" s="79"/>
-      <c r="H50" s="79"/>
-      <c r="I50" s="65"/>
+      <c r="D50" s="58"/>
+      <c r="E50" s="58"/>
+      <c r="F50" s="77"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="58"/>
+      <c r="I50" s="91"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="57" t="s">
-        <v>62</v>
-      </c>
-      <c r="B51" s="86" t="s">
+      <c r="A51" s="110" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C51" s="44">
         <v>1</v>
       </c>
-      <c r="D51" s="94">
+      <c r="D51" s="69">
         <v>43122</v>
       </c>
-      <c r="E51" s="94">
+      <c r="E51" s="69">
         <v>43122</v>
       </c>
-      <c r="F51" s="104">
-        <v>1</v>
-      </c>
-      <c r="G51" s="94">
+      <c r="F51" s="78">
+        <v>1</v>
+      </c>
+      <c r="G51" s="69">
         <v>43122</v>
       </c>
-      <c r="H51" s="94">
+      <c r="H51" s="69">
         <v>43122</v>
       </c>
-      <c r="I51" s="62"/>
+      <c r="I51" s="95"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="58"/>
+      <c r="A52" s="111"/>
       <c r="B52" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C52" s="49"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="82"/>
-      <c r="F52" s="105"/>
-      <c r="G52" s="82"/>
-      <c r="H52" s="82"/>
-      <c r="I52" s="62"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="60"/>
+      <c r="F52" s="79"/>
+      <c r="G52" s="60"/>
+      <c r="H52" s="60"/>
+      <c r="I52" s="95"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="58"/>
+      <c r="A53" s="111"/>
       <c r="B53" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C53" s="49"/>
-      <c r="D53" s="82"/>
-      <c r="E53" s="82"/>
-      <c r="F53" s="105"/>
-      <c r="G53" s="82"/>
-      <c r="H53" s="82"/>
-      <c r="I53" s="62"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="60"/>
+      <c r="F53" s="79"/>
+      <c r="G53" s="60"/>
+      <c r="H53" s="60"/>
+      <c r="I53" s="95"/>
     </row>
     <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="59"/>
+      <c r="A54" s="112"/>
       <c r="B54" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C54" s="46"/>
-      <c r="D54" s="79"/>
-      <c r="E54" s="79"/>
-      <c r="F54" s="103"/>
-      <c r="G54" s="79"/>
-      <c r="H54" s="79"/>
-      <c r="I54" s="65"/>
+      <c r="D54" s="58"/>
+      <c r="E54" s="58"/>
+      <c r="F54" s="77"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="I54" s="91"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="57" t="s">
-        <v>66</v>
-      </c>
-      <c r="B55" s="86" t="s">
+      <c r="A55" s="99" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C55" s="44">
         <v>1</v>
       </c>
-      <c r="D55" s="94">
-        <v>43123</v>
-      </c>
-      <c r="E55" s="94">
-        <v>43123</v>
-      </c>
-      <c r="F55" s="104">
-        <v>1</v>
-      </c>
-      <c r="G55" s="94">
-        <v>43123</v>
-      </c>
-      <c r="H55" s="94">
-        <v>43123</v>
-      </c>
-      <c r="I55" s="62"/>
+      <c r="D55" s="69">
+        <v>43122</v>
+      </c>
+      <c r="E55" s="69">
+        <v>43122</v>
+      </c>
+      <c r="F55" s="78">
+        <v>1</v>
+      </c>
+      <c r="G55" s="69">
+        <v>43122</v>
+      </c>
+      <c r="H55" s="69">
+        <v>43122</v>
+      </c>
+      <c r="I55" s="95"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="58"/>
+      <c r="A56" s="100"/>
       <c r="B56" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C56" s="49"/>
-      <c r="D56" s="82"/>
-      <c r="E56" s="82"/>
-      <c r="F56" s="105"/>
-      <c r="G56" s="82"/>
-      <c r="H56" s="82"/>
-      <c r="I56" s="62"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="60"/>
+      <c r="F56" s="79"/>
+      <c r="G56" s="60"/>
+      <c r="H56" s="60"/>
+      <c r="I56" s="95"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="58"/>
+      <c r="A57" s="100"/>
       <c r="B57" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C57" s="49"/>
-      <c r="D57" s="82"/>
-      <c r="E57" s="82"/>
-      <c r="F57" s="105"/>
-      <c r="G57" s="82"/>
-      <c r="H57" s="82"/>
-      <c r="I57" s="62"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="60"/>
+      <c r="F57" s="79"/>
+      <c r="G57" s="60"/>
+      <c r="H57" s="60"/>
+      <c r="I57" s="95"/>
     </row>
     <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="59"/>
+      <c r="A58" s="101"/>
       <c r="B58" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C58" s="46"/>
-      <c r="D58" s="79"/>
-      <c r="E58" s="79"/>
-      <c r="F58" s="103"/>
-      <c r="G58" s="79"/>
-      <c r="H58" s="79"/>
-      <c r="I58" s="65"/>
+      <c r="D58" s="58"/>
+      <c r="E58" s="58"/>
+      <c r="F58" s="77"/>
+      <c r="G58" s="58"/>
+      <c r="H58" s="58"/>
+      <c r="I58" s="91"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="57" t="s">
-        <v>67</v>
-      </c>
-      <c r="B59" s="86" t="s">
+      <c r="A59" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C59" s="44">
         <v>1</v>
       </c>
-      <c r="D59" s="94">
+      <c r="D59" s="69">
         <v>43123</v>
       </c>
-      <c r="E59" s="94">
+      <c r="E59" s="69">
         <v>43123</v>
       </c>
-      <c r="F59" s="104">
-        <v>1</v>
-      </c>
-      <c r="G59" s="94">
+      <c r="F59" s="78">
+        <v>1</v>
+      </c>
+      <c r="G59" s="69">
         <v>43123</v>
       </c>
-      <c r="H59" s="94">
+      <c r="H59" s="69">
         <v>43123</v>
       </c>
-      <c r="I59" s="62"/>
+      <c r="I59" s="95"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="58"/>
+      <c r="A60" s="100"/>
       <c r="B60" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C60" s="49"/>
-      <c r="D60" s="82"/>
-      <c r="E60" s="82"/>
-      <c r="F60" s="105"/>
-      <c r="G60" s="82"/>
-      <c r="H60" s="82"/>
-      <c r="I60" s="62"/>
+      <c r="D60" s="60"/>
+      <c r="E60" s="60"/>
+      <c r="F60" s="79"/>
+      <c r="G60" s="60"/>
+      <c r="H60" s="60"/>
+      <c r="I60" s="95"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="58"/>
+      <c r="A61" s="100"/>
       <c r="B61" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C61" s="49"/>
-      <c r="D61" s="82"/>
-      <c r="E61" s="82"/>
-      <c r="F61" s="105"/>
-      <c r="G61" s="82"/>
-      <c r="H61" s="82"/>
-      <c r="I61" s="62"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="60"/>
+      <c r="F61" s="79"/>
+      <c r="G61" s="60"/>
+      <c r="H61" s="60"/>
+      <c r="I61" s="95"/>
     </row>
     <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="59"/>
+      <c r="A62" s="101"/>
       <c r="B62" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C62" s="46"/>
-      <c r="D62" s="79"/>
-      <c r="E62" s="79"/>
-      <c r="F62" s="103"/>
-      <c r="G62" s="79"/>
-      <c r="H62" s="79"/>
-      <c r="I62" s="65"/>
+      <c r="D62" s="58"/>
+      <c r="E62" s="58"/>
+      <c r="F62" s="77"/>
+      <c r="G62" s="58"/>
+      <c r="H62" s="58"/>
+      <c r="I62" s="91"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="91" t="s">
-        <v>68</v>
-      </c>
-      <c r="B63" s="86" t="s">
+      <c r="A63" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C63" s="44">
         <v>1</v>
       </c>
-      <c r="D63" s="94">
-        <v>43124</v>
-      </c>
-      <c r="E63" s="94">
-        <v>43124</v>
-      </c>
-      <c r="F63" s="104">
-        <v>1</v>
-      </c>
-      <c r="G63" s="94">
-        <v>43124</v>
-      </c>
-      <c r="H63" s="94">
-        <v>43124</v>
-      </c>
-      <c r="I63" s="62"/>
+      <c r="D63" s="69">
+        <v>43123</v>
+      </c>
+      <c r="E63" s="69">
+        <v>43123</v>
+      </c>
+      <c r="F63" s="78">
+        <v>1</v>
+      </c>
+      <c r="G63" s="69">
+        <v>43123</v>
+      </c>
+      <c r="H63" s="69">
+        <v>43123</v>
+      </c>
+      <c r="I63" s="95"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="85"/>
+      <c r="A64" s="100"/>
       <c r="B64" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C64" s="49"/>
-      <c r="D64" s="82"/>
-      <c r="E64" s="82"/>
-      <c r="F64" s="105"/>
-      <c r="G64" s="82"/>
-      <c r="H64" s="82"/>
-      <c r="I64" s="62"/>
+      <c r="D64" s="60"/>
+      <c r="E64" s="60"/>
+      <c r="F64" s="79"/>
+      <c r="G64" s="60"/>
+      <c r="H64" s="60"/>
+      <c r="I64" s="95"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="85"/>
+      <c r="A65" s="100"/>
       <c r="B65" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C65" s="49"/>
-      <c r="D65" s="82"/>
-      <c r="E65" s="82"/>
-      <c r="F65" s="105"/>
-      <c r="G65" s="82"/>
-      <c r="H65" s="82"/>
-      <c r="I65" s="62"/>
+      <c r="D65" s="60"/>
+      <c r="E65" s="60"/>
+      <c r="F65" s="79"/>
+      <c r="G65" s="60"/>
+      <c r="H65" s="60"/>
+      <c r="I65" s="95"/>
     </row>
     <row r="66" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="92"/>
+      <c r="A66" s="101"/>
       <c r="B66" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C66" s="46"/>
-      <c r="D66" s="79"/>
-      <c r="E66" s="79"/>
-      <c r="F66" s="103"/>
-      <c r="G66" s="79"/>
-      <c r="H66" s="79"/>
-      <c r="I66" s="65"/>
+      <c r="D66" s="58"/>
+      <c r="E66" s="58"/>
+      <c r="F66" s="77"/>
+      <c r="G66" s="58"/>
+      <c r="H66" s="58"/>
+      <c r="I66" s="91"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="91" t="s">
-        <v>69</v>
-      </c>
-      <c r="B67" s="86" t="s">
+      <c r="A67" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C67" s="44">
         <v>1</v>
       </c>
-      <c r="D67" s="94">
+      <c r="D67" s="69">
         <v>43124</v>
       </c>
-      <c r="E67" s="94">
+      <c r="E67" s="69">
         <v>43124</v>
       </c>
-      <c r="F67" s="104">
-        <v>1</v>
-      </c>
-      <c r="G67" s="94">
+      <c r="F67" s="78">
+        <v>1</v>
+      </c>
+      <c r="G67" s="69">
         <v>43124</v>
       </c>
-      <c r="H67" s="94">
+      <c r="H67" s="69">
         <v>43124</v>
       </c>
-      <c r="I67" s="62"/>
+      <c r="I67" s="95"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="85"/>
+      <c r="A68" s="111"/>
       <c r="B68" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C68" s="49"/>
-      <c r="D68" s="82"/>
-      <c r="E68" s="82"/>
-      <c r="F68" s="105"/>
-      <c r="G68" s="82"/>
-      <c r="H68" s="82"/>
-      <c r="I68" s="62"/>
+      <c r="D68" s="60"/>
+      <c r="E68" s="60"/>
+      <c r="F68" s="79"/>
+      <c r="G68" s="60"/>
+      <c r="H68" s="60"/>
+      <c r="I68" s="95"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="85"/>
+      <c r="A69" s="111"/>
       <c r="B69" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C69" s="49"/>
-      <c r="D69" s="82"/>
-      <c r="E69" s="82"/>
-      <c r="F69" s="105"/>
-      <c r="G69" s="82"/>
-      <c r="H69" s="82"/>
-      <c r="I69" s="62"/>
+      <c r="D69" s="60"/>
+      <c r="E69" s="60"/>
+      <c r="F69" s="79"/>
+      <c r="G69" s="60"/>
+      <c r="H69" s="60"/>
+      <c r="I69" s="95"/>
     </row>
     <row r="70" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="92"/>
+      <c r="A70" s="112"/>
       <c r="B70" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C70" s="46"/>
-      <c r="D70" s="79"/>
-      <c r="E70" s="79"/>
-      <c r="F70" s="103"/>
-      <c r="G70" s="79"/>
-      <c r="H70" s="79"/>
-      <c r="I70" s="65"/>
+      <c r="D70" s="58"/>
+      <c r="E70" s="58"/>
+      <c r="F70" s="77"/>
+      <c r="G70" s="58"/>
+      <c r="H70" s="58"/>
+      <c r="I70" s="91"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="57" t="s">
-        <v>15</v>
-      </c>
-      <c r="B71" s="86" t="s">
+      <c r="A71" s="110" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C71" s="44">
         <v>1</v>
       </c>
-      <c r="D71" s="94">
-        <v>43125</v>
-      </c>
-      <c r="E71" s="94">
-        <v>43125</v>
-      </c>
-      <c r="F71" s="104">
-        <v>1</v>
-      </c>
-      <c r="G71" s="94">
-        <v>43125</v>
-      </c>
-      <c r="H71" s="94">
-        <v>43125</v>
-      </c>
-      <c r="I71" s="62"/>
+      <c r="D71" s="69">
+        <v>43124</v>
+      </c>
+      <c r="E71" s="69">
+        <v>43124</v>
+      </c>
+      <c r="F71" s="78">
+        <v>1</v>
+      </c>
+      <c r="G71" s="69">
+        <v>43124</v>
+      </c>
+      <c r="H71" s="69">
+        <v>43124</v>
+      </c>
+      <c r="I71" s="95"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="58"/>
+      <c r="A72" s="111"/>
       <c r="B72" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C72" s="49"/>
-      <c r="D72" s="82"/>
-      <c r="E72" s="82"/>
-      <c r="F72" s="105"/>
-      <c r="G72" s="82"/>
-      <c r="H72" s="82"/>
-      <c r="I72" s="62"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="60"/>
+      <c r="F72" s="79"/>
+      <c r="G72" s="60"/>
+      <c r="H72" s="60"/>
+      <c r="I72" s="95"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="58"/>
+      <c r="A73" s="111"/>
       <c r="B73" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C73" s="49"/>
-      <c r="D73" s="82"/>
-      <c r="E73" s="82"/>
-      <c r="F73" s="105"/>
-      <c r="G73" s="82"/>
-      <c r="H73" s="82"/>
-      <c r="I73" s="62"/>
+      <c r="D73" s="60"/>
+      <c r="E73" s="60"/>
+      <c r="F73" s="79"/>
+      <c r="G73" s="60"/>
+      <c r="H73" s="60"/>
+      <c r="I73" s="95"/>
     </row>
     <row r="74" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="59"/>
+      <c r="A74" s="112"/>
       <c r="B74" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C74" s="46"/>
-      <c r="D74" s="79"/>
-      <c r="E74" s="79"/>
-      <c r="F74" s="103"/>
-      <c r="G74" s="79"/>
-      <c r="H74" s="79"/>
-      <c r="I74" s="65"/>
+      <c r="D74" s="58"/>
+      <c r="E74" s="58"/>
+      <c r="F74" s="77"/>
+      <c r="G74" s="58"/>
+      <c r="H74" s="58"/>
+      <c r="I74" s="91"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="B75" s="86" t="s">
+      <c r="A75" s="99" t="s">
+        <v>15</v>
+      </c>
+      <c r="B75" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C75" s="44">
         <v>1</v>
       </c>
-      <c r="D75" s="94">
+      <c r="D75" s="69">
         <v>43125</v>
       </c>
-      <c r="E75" s="94">
+      <c r="E75" s="69">
         <v>43125</v>
       </c>
-      <c r="F75" s="104">
-        <v>1</v>
-      </c>
-      <c r="G75" s="94">
+      <c r="F75" s="78">
+        <v>1</v>
+      </c>
+      <c r="G75" s="69">
         <v>43125</v>
       </c>
-      <c r="H75" s="94">
+      <c r="H75" s="69">
         <v>43125</v>
       </c>
-      <c r="I75" s="62"/>
+      <c r="I75" s="95"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="58"/>
+      <c r="A76" s="100"/>
       <c r="B76" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C76" s="49"/>
-      <c r="D76" s="82"/>
-      <c r="E76" s="82"/>
-      <c r="F76" s="105"/>
-      <c r="G76" s="82"/>
-      <c r="I76" s="62"/>
+      <c r="D76" s="60"/>
+      <c r="E76" s="60"/>
+      <c r="F76" s="79"/>
+      <c r="G76" s="60"/>
+      <c r="H76" s="60"/>
+      <c r="I76" s="95"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="58"/>
+      <c r="A77" s="100"/>
       <c r="B77" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C77" s="49"/>
-      <c r="D77" s="82"/>
-      <c r="E77" s="82"/>
-      <c r="F77" s="105"/>
-      <c r="G77" s="82"/>
-      <c r="I77" s="62"/>
+      <c r="D77" s="60"/>
+      <c r="E77" s="60"/>
+      <c r="F77" s="79"/>
+      <c r="G77" s="60"/>
+      <c r="H77" s="60"/>
+      <c r="I77" s="95"/>
     </row>
     <row r="78" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="59"/>
+      <c r="A78" s="101"/>
       <c r="B78" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C78" s="46"/>
-      <c r="D78" s="79"/>
-      <c r="E78" s="79"/>
-      <c r="F78" s="103"/>
-      <c r="G78" s="79"/>
-      <c r="H78" s="79"/>
-      <c r="I78" s="65"/>
+      <c r="D78" s="58"/>
+      <c r="E78" s="58"/>
+      <c r="F78" s="77"/>
+      <c r="G78" s="58"/>
+      <c r="H78" s="58"/>
+      <c r="I78" s="91"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="57" t="s">
-        <v>82</v>
-      </c>
-      <c r="B79" s="86" t="s">
+      <c r="A79" s="99" t="s">
+        <v>56</v>
+      </c>
+      <c r="B79" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C79" s="44">
         <v>1</v>
       </c>
-      <c r="D79" s="94">
-        <v>43126</v>
-      </c>
-      <c r="E79" s="94">
-        <v>43126</v>
-      </c>
-      <c r="F79" s="104">
-        <v>1</v>
-      </c>
-      <c r="G79" s="94">
-        <v>43126</v>
-      </c>
-      <c r="H79" s="94">
-        <v>43126</v>
-      </c>
-      <c r="I79" s="62"/>
+      <c r="D79" s="69">
+        <v>43125</v>
+      </c>
+      <c r="E79" s="69">
+        <v>43125</v>
+      </c>
+      <c r="F79" s="78">
+        <v>1</v>
+      </c>
+      <c r="G79" s="69">
+        <v>43125</v>
+      </c>
+      <c r="H79" s="69">
+        <v>43125</v>
+      </c>
+      <c r="I79" s="95"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="58"/>
+      <c r="A80" s="100"/>
       <c r="B80" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C80" s="49"/>
-      <c r="D80" s="82"/>
-      <c r="E80" s="82"/>
-      <c r="F80" s="105"/>
-      <c r="G80" s="82"/>
-      <c r="H80" s="82"/>
-      <c r="I80" s="62"/>
+      <c r="D80" s="60"/>
+      <c r="E80" s="60"/>
+      <c r="F80" s="79"/>
+      <c r="G80" s="60"/>
+      <c r="I80" s="95"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="58"/>
+      <c r="A81" s="100"/>
       <c r="B81" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C81" s="49"/>
-      <c r="D81" s="82"/>
-      <c r="E81" s="82"/>
-      <c r="F81" s="105"/>
-      <c r="G81" s="82"/>
-      <c r="H81" s="82"/>
-      <c r="I81" s="62"/>
+      <c r="D81" s="60"/>
+      <c r="E81" s="60"/>
+      <c r="F81" s="79"/>
+      <c r="G81" s="60"/>
+      <c r="I81" s="95"/>
     </row>
     <row r="82" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="59"/>
+      <c r="A82" s="101"/>
       <c r="B82" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C82" s="46"/>
-      <c r="D82" s="79"/>
-      <c r="E82" s="79"/>
-      <c r="F82" s="103"/>
-      <c r="G82" s="79"/>
-      <c r="H82" s="79"/>
-      <c r="I82" s="65"/>
+      <c r="D82" s="58"/>
+      <c r="E82" s="58"/>
+      <c r="F82" s="77"/>
+      <c r="G82" s="58"/>
+      <c r="H82" s="58"/>
+      <c r="I82" s="91"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="57" t="s">
-        <v>83</v>
-      </c>
-      <c r="B83" s="86" t="s">
+      <c r="A83" s="99" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C83" s="44">
         <v>1</v>
       </c>
-      <c r="D83" s="94">
+      <c r="D83" s="69">
         <v>43126</v>
       </c>
-      <c r="E83" s="94">
+      <c r="E83" s="69">
         <v>43126</v>
       </c>
-      <c r="F83" s="104">
-        <v>1</v>
-      </c>
-      <c r="G83" s="94">
+      <c r="F83" s="78">
+        <v>1</v>
+      </c>
+      <c r="G83" s="69">
         <v>43126</v>
       </c>
-      <c r="H83" s="94">
+      <c r="H83" s="69">
         <v>43126</v>
       </c>
-      <c r="I83" s="62"/>
+      <c r="I83" s="95"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="58"/>
+      <c r="A84" s="100"/>
       <c r="B84" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C84" s="49"/>
-      <c r="D84" s="82"/>
-      <c r="E84" s="82"/>
-      <c r="F84" s="105"/>
-      <c r="G84" s="82"/>
-      <c r="H84" s="82"/>
-      <c r="I84" s="62"/>
+      <c r="D84" s="60"/>
+      <c r="E84" s="60"/>
+      <c r="F84" s="79"/>
+      <c r="G84" s="60"/>
+      <c r="H84" s="60"/>
+      <c r="I84" s="95"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="58"/>
+      <c r="A85" s="100"/>
       <c r="B85" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C85" s="49"/>
-      <c r="D85" s="82"/>
-      <c r="E85" s="82"/>
-      <c r="F85" s="105"/>
-      <c r="G85" s="82"/>
-      <c r="H85" s="82"/>
-      <c r="I85" s="62"/>
+      <c r="D85" s="60"/>
+      <c r="E85" s="60"/>
+      <c r="F85" s="79"/>
+      <c r="G85" s="60"/>
+      <c r="H85" s="60"/>
+      <c r="I85" s="95"/>
     </row>
     <row r="86" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="59"/>
+      <c r="A86" s="101"/>
       <c r="B86" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C86" s="46"/>
-      <c r="D86" s="79"/>
-      <c r="E86" s="79"/>
-      <c r="F86" s="103"/>
-      <c r="G86" s="79"/>
-      <c r="H86" s="79"/>
-      <c r="I86" s="65"/>
+      <c r="D86" s="58"/>
+      <c r="E86" s="58"/>
+      <c r="F86" s="77"/>
+      <c r="G86" s="58"/>
+      <c r="H86" s="58"/>
+      <c r="I86" s="91"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="91" t="s">
-        <v>101</v>
-      </c>
-      <c r="B87" s="86" t="s">
+      <c r="A87" s="99" t="s">
+        <v>83</v>
+      </c>
+      <c r="B87" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C87" s="44">
         <v>1</v>
       </c>
-      <c r="D87" s="94">
-        <v>43127</v>
-      </c>
-      <c r="E87" s="94">
-        <v>43127</v>
-      </c>
-      <c r="F87" s="104">
-        <v>1</v>
-      </c>
-      <c r="G87" s="94">
-        <v>43127</v>
-      </c>
-      <c r="H87" s="94">
-        <v>43127</v>
-      </c>
-      <c r="I87" s="62"/>
+      <c r="D87" s="69">
+        <v>43126</v>
+      </c>
+      <c r="E87" s="69">
+        <v>43126</v>
+      </c>
+      <c r="F87" s="78">
+        <v>1</v>
+      </c>
+      <c r="G87" s="69">
+        <v>43126</v>
+      </c>
+      <c r="H87" s="69">
+        <v>43126</v>
+      </c>
+      <c r="I87" s="95"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="85"/>
+      <c r="A88" s="100"/>
       <c r="B88" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C88" s="49"/>
-      <c r="D88" s="82"/>
-      <c r="E88" s="82"/>
-      <c r="F88" s="105"/>
-      <c r="G88" s="82"/>
-      <c r="I88" s="62"/>
+      <c r="D88" s="60"/>
+      <c r="E88" s="60"/>
+      <c r="F88" s="79"/>
+      <c r="G88" s="60"/>
+      <c r="H88" s="60"/>
+      <c r="I88" s="95"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="85"/>
+      <c r="A89" s="100"/>
       <c r="B89" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C89" s="49"/>
-      <c r="D89" s="82"/>
-      <c r="E89" s="82"/>
-      <c r="F89" s="105"/>
-      <c r="G89" s="82"/>
-      <c r="I89" s="62"/>
+      <c r="D89" s="60"/>
+      <c r="E89" s="60"/>
+      <c r="F89" s="79"/>
+      <c r="G89" s="60"/>
+      <c r="H89" s="60"/>
+      <c r="I89" s="95"/>
     </row>
     <row r="90" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="92"/>
+      <c r="A90" s="101"/>
       <c r="B90" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C90" s="46"/>
-      <c r="D90" s="79"/>
-      <c r="E90" s="79"/>
-      <c r="F90" s="103"/>
-      <c r="G90" s="79"/>
-      <c r="H90" s="79"/>
-      <c r="I90" s="65"/>
+      <c r="D90" s="58"/>
+      <c r="E90" s="58"/>
+      <c r="F90" s="77"/>
+      <c r="G90" s="58"/>
+      <c r="H90" s="58"/>
+      <c r="I90" s="91"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="91" t="s">
-        <v>109</v>
-      </c>
-      <c r="B91" s="52" t="s">
+      <c r="A91" s="110" t="s">
+        <v>101</v>
+      </c>
+      <c r="B91" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C91" s="44">
         <v>1</v>
       </c>
-      <c r="D91" s="94">
+      <c r="D91" s="69">
         <v>43127</v>
       </c>
-      <c r="E91" s="94">
+      <c r="E91" s="69">
         <v>43127</v>
       </c>
-      <c r="F91" s="104">
-        <v>1</v>
-      </c>
-      <c r="G91" s="94">
+      <c r="F91" s="78">
+        <v>1</v>
+      </c>
+      <c r="G91" s="69">
         <v>43127</v>
       </c>
-      <c r="H91" s="94">
+      <c r="H91" s="69">
         <v>43127</v>
       </c>
-      <c r="I91" s="61"/>
+      <c r="I91" s="95"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="85"/>
+      <c r="A92" s="111"/>
       <c r="B92" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="I92" s="62"/>
+      <c r="C92" s="49"/>
+      <c r="D92" s="60"/>
+      <c r="E92" s="60"/>
+      <c r="F92" s="79"/>
+      <c r="G92" s="60"/>
+      <c r="I92" s="95"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="85"/>
+      <c r="A93" s="111"/>
       <c r="B93" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="I93" s="62"/>
+      <c r="C93" s="49"/>
+      <c r="D93" s="60"/>
+      <c r="E93" s="60"/>
+      <c r="F93" s="79"/>
+      <c r="G93" s="60"/>
+      <c r="I93" s="95"/>
     </row>
     <row r="94" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="92"/>
+      <c r="A94" s="112"/>
       <c r="B94" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C94" s="46"/>
-      <c r="D94" s="79"/>
-      <c r="E94" s="79"/>
-      <c r="F94" s="103"/>
-      <c r="G94" s="79"/>
-      <c r="H94" s="79"/>
-      <c r="I94" s="65"/>
+      <c r="D94" s="58"/>
+      <c r="E94" s="58"/>
+      <c r="F94" s="77"/>
+      <c r="G94" s="58"/>
+      <c r="H94" s="58"/>
+      <c r="I94" s="91"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="91" t="s">
-        <v>102</v>
+      <c r="A95" s="110" t="s">
+        <v>109</v>
       </c>
       <c r="B95" s="52" t="s">
         <v>119</v>
@@ -3612,53 +3643,53 @@
       <c r="C95" s="44">
         <v>1</v>
       </c>
-      <c r="D95" s="94">
+      <c r="D95" s="69">
         <v>43127</v>
       </c>
-      <c r="E95" s="94">
+      <c r="E95" s="69">
         <v>43127</v>
       </c>
-      <c r="F95" s="104">
-        <v>1</v>
-      </c>
-      <c r="G95" s="94">
+      <c r="F95" s="78">
+        <v>1</v>
+      </c>
+      <c r="G95" s="69">
         <v>43127</v>
       </c>
-      <c r="H95" s="94">
+      <c r="H95" s="69">
         <v>43127</v>
       </c>
-      <c r="I95" s="62"/>
+      <c r="I95" s="89"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="85"/>
+      <c r="A96" s="111"/>
       <c r="B96" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="I96" s="62"/>
+      <c r="I96" s="95"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="85"/>
+      <c r="A97" s="111"/>
       <c r="B97" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="I97" s="62"/>
+      <c r="I97" s="95"/>
     </row>
     <row r="98" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="92"/>
+      <c r="A98" s="112"/>
       <c r="B98" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C98" s="46"/>
-      <c r="D98" s="79"/>
-      <c r="E98" s="79"/>
-      <c r="F98" s="103"/>
-      <c r="G98" s="79"/>
-      <c r="H98" s="79"/>
-      <c r="I98" s="65"/>
+      <c r="D98" s="58"/>
+      <c r="E98" s="58"/>
+      <c r="F98" s="77"/>
+      <c r="G98" s="58"/>
+      <c r="H98" s="58"/>
+      <c r="I98" s="91"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="91" t="s">
-        <v>104</v>
+      <c r="A99" s="110" t="s">
+        <v>102</v>
       </c>
       <c r="B99" s="52" t="s">
         <v>119</v>
@@ -3666,173 +3697,173 @@
       <c r="C99" s="44">
         <v>1</v>
       </c>
-      <c r="D99" s="94">
-        <v>43128</v>
-      </c>
-      <c r="E99" s="94">
-        <v>43128</v>
-      </c>
-      <c r="F99" s="104">
-        <v>1</v>
-      </c>
-      <c r="G99" s="94">
-        <v>43128</v>
-      </c>
-      <c r="H99" s="94">
-        <v>43128</v>
-      </c>
-      <c r="I99" s="62"/>
+      <c r="D99" s="69">
+        <v>43127</v>
+      </c>
+      <c r="E99" s="69">
+        <v>43127</v>
+      </c>
+      <c r="F99" s="78">
+        <v>1</v>
+      </c>
+      <c r="G99" s="69">
+        <v>43127</v>
+      </c>
+      <c r="H99" s="69">
+        <v>43127</v>
+      </c>
+      <c r="I99" s="95"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="85"/>
+      <c r="A100" s="111"/>
       <c r="B100" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="I100" s="62"/>
+      <c r="I100" s="95"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="85"/>
+      <c r="A101" s="111"/>
       <c r="B101" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="I101" s="62"/>
+      <c r="I101" s="95"/>
     </row>
     <row r="102" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="92"/>
+      <c r="A102" s="112"/>
       <c r="B102" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C102" s="46"/>
-      <c r="D102" s="79"/>
-      <c r="E102" s="79"/>
-      <c r="F102" s="103"/>
-      <c r="G102" s="79"/>
-      <c r="H102" s="79"/>
-      <c r="I102" s="65"/>
+      <c r="D102" s="58"/>
+      <c r="E102" s="58"/>
+      <c r="F102" s="77"/>
+      <c r="G102" s="58"/>
+      <c r="H102" s="58"/>
+      <c r="I102" s="91"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="57" t="s">
-        <v>103</v>
-      </c>
-      <c r="B103" s="86" t="s">
+      <c r="A103" s="110" t="s">
+        <v>104</v>
+      </c>
+      <c r="B103" s="52" t="s">
         <v>119</v>
       </c>
       <c r="C103" s="44">
         <v>1</v>
       </c>
-      <c r="D103" s="94">
+      <c r="D103" s="69">
         <v>43128</v>
       </c>
-      <c r="E103" s="94">
+      <c r="E103" s="69">
         <v>43128</v>
       </c>
-      <c r="F103" s="104">
-        <v>1</v>
-      </c>
-      <c r="G103" s="94">
+      <c r="F103" s="78">
+        <v>1</v>
+      </c>
+      <c r="G103" s="69">
         <v>43128</v>
       </c>
-      <c r="H103" s="94">
+      <c r="H103" s="69">
         <v>43128</v>
       </c>
-      <c r="I103" s="62"/>
+      <c r="I103" s="95"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="58"/>
+      <c r="A104" s="111"/>
       <c r="B104" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="C104" s="49"/>
-      <c r="D104" s="82"/>
-      <c r="E104" s="82"/>
-      <c r="F104" s="105"/>
-      <c r="G104" s="82"/>
-      <c r="H104" s="82"/>
-      <c r="I104" s="62"/>
+      <c r="I104" s="95"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="58"/>
+      <c r="A105" s="111"/>
       <c r="B105" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="C105" s="49"/>
-      <c r="D105" s="82"/>
-      <c r="E105" s="82"/>
-      <c r="F105" s="105"/>
-      <c r="G105" s="82"/>
-      <c r="H105" s="82"/>
-      <c r="I105" s="62"/>
+      <c r="I105" s="95"/>
     </row>
     <row r="106" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="59"/>
+      <c r="A106" s="112"/>
       <c r="B106" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C106" s="46"/>
-      <c r="D106" s="79"/>
-      <c r="E106" s="79"/>
-      <c r="F106" s="103"/>
-      <c r="G106" s="79"/>
-      <c r="H106" s="79"/>
-      <c r="I106" s="65"/>
+      <c r="D106" s="58"/>
+      <c r="E106" s="58"/>
+      <c r="F106" s="77"/>
+      <c r="G106" s="58"/>
+      <c r="H106" s="58"/>
+      <c r="I106" s="91"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="57" t="s">
-        <v>105</v>
-      </c>
-      <c r="B107" s="52" t="s">
+      <c r="A107" s="99" t="s">
+        <v>103</v>
+      </c>
+      <c r="B107" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C107" s="44">
         <v>1</v>
       </c>
-      <c r="D107" s="94">
-        <v>43129</v>
-      </c>
-      <c r="E107" s="94">
-        <v>43129</v>
-      </c>
-      <c r="F107" s="104">
-        <v>1</v>
-      </c>
-      <c r="G107" s="94">
-        <v>43129</v>
-      </c>
-      <c r="H107" s="94">
-        <v>43129</v>
-      </c>
-      <c r="I107" s="62"/>
+      <c r="D107" s="69">
+        <v>43128</v>
+      </c>
+      <c r="E107" s="69">
+        <v>43128</v>
+      </c>
+      <c r="F107" s="78">
+        <v>1</v>
+      </c>
+      <c r="G107" s="69">
+        <v>43128</v>
+      </c>
+      <c r="H107" s="69">
+        <v>43128</v>
+      </c>
+      <c r="I107" s="95"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="58"/>
+      <c r="A108" s="100"/>
       <c r="B108" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="I108" s="62"/>
+      <c r="C108" s="49"/>
+      <c r="D108" s="60"/>
+      <c r="E108" s="60"/>
+      <c r="F108" s="79"/>
+      <c r="G108" s="60"/>
+      <c r="H108" s="60"/>
+      <c r="I108" s="95"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="58"/>
+      <c r="A109" s="100"/>
       <c r="B109" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="I109" s="62"/>
+      <c r="C109" s="49"/>
+      <c r="D109" s="60"/>
+      <c r="E109" s="60"/>
+      <c r="F109" s="79"/>
+      <c r="G109" s="60"/>
+      <c r="H109" s="60"/>
+      <c r="I109" s="95"/>
     </row>
     <row r="110" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="59"/>
+      <c r="A110" s="101"/>
       <c r="B110" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C110" s="46"/>
-      <c r="D110" s="79"/>
-      <c r="E110" s="79"/>
-      <c r="F110" s="103"/>
-      <c r="G110" s="79"/>
-      <c r="H110" s="79"/>
-      <c r="I110" s="65"/>
+      <c r="D110" s="58"/>
+      <c r="E110" s="58"/>
+      <c r="F110" s="77"/>
+      <c r="G110" s="58"/>
+      <c r="H110" s="58"/>
+      <c r="I110" s="91"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="57" t="s">
-        <v>108</v>
+      <c r="A111" s="99" t="s">
+        <v>105</v>
       </c>
       <c r="B111" s="52" t="s">
         <v>119</v>
@@ -3840,398 +3871,454 @@
       <c r="C111" s="44">
         <v>1</v>
       </c>
-      <c r="D111" s="94">
+      <c r="D111" s="69">
         <v>43129</v>
       </c>
-      <c r="E111" s="94">
+      <c r="E111" s="69">
         <v>43129</v>
       </c>
-      <c r="F111" s="104">
-        <v>1</v>
-      </c>
-      <c r="G111" s="94">
+      <c r="F111" s="78">
+        <v>1</v>
+      </c>
+      <c r="G111" s="69">
         <v>43129</v>
       </c>
-      <c r="H111" s="94">
+      <c r="H111" s="69">
         <v>43129</v>
       </c>
-      <c r="I111" s="62"/>
+      <c r="I111" s="95"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="58"/>
+      <c r="A112" s="100"/>
       <c r="B112" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="I112" s="62"/>
+      <c r="I112" s="95"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="58"/>
+      <c r="A113" s="100"/>
       <c r="B113" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="I113" s="62"/>
+      <c r="I113" s="95"/>
     </row>
     <row r="114" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="59"/>
+      <c r="A114" s="101"/>
       <c r="B114" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C114" s="46"/>
-      <c r="D114" s="79"/>
-      <c r="E114" s="79"/>
-      <c r="F114" s="103"/>
-      <c r="G114" s="79"/>
-      <c r="H114" s="79"/>
-      <c r="I114" s="65"/>
-    </row>
-    <row r="115" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="57" t="s">
+      <c r="D114" s="58"/>
+      <c r="E114" s="58"/>
+      <c r="F114" s="77"/>
+      <c r="G114" s="58"/>
+      <c r="H114" s="58"/>
+      <c r="I114" s="91"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="99" t="s">
+        <v>108</v>
+      </c>
+      <c r="B115" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="C115" s="44">
+        <v>1</v>
+      </c>
+      <c r="D115" s="69">
+        <v>43129</v>
+      </c>
+      <c r="E115" s="69">
+        <v>43129</v>
+      </c>
+      <c r="F115" s="78">
+        <v>1</v>
+      </c>
+      <c r="G115" s="69">
+        <v>43129</v>
+      </c>
+      <c r="H115" s="69">
+        <v>43129</v>
+      </c>
+      <c r="I115" s="95"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="100"/>
+      <c r="B116" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="I116" s="95"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="100"/>
+      <c r="B117" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="I117" s="95"/>
+    </row>
+    <row r="118" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="101"/>
+      <c r="B118" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="C118" s="46"/>
+      <c r="D118" s="58"/>
+      <c r="E118" s="58"/>
+      <c r="F118" s="77"/>
+      <c r="G118" s="58"/>
+      <c r="H118" s="58"/>
+      <c r="I118" s="91"/>
+    </row>
+    <row r="119" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="B115" s="86" t="s">
+      <c r="B119" s="63" t="s">
         <v>122</v>
       </c>
-      <c r="C115" s="44"/>
-      <c r="D115" s="94"/>
-      <c r="E115" s="94"/>
-      <c r="F115" s="83"/>
-      <c r="G115" s="100"/>
-      <c r="H115" s="100"/>
-      <c r="I115" s="62"/>
-    </row>
-    <row r="116" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="58"/>
-      <c r="B116" s="52" t="s">
+      <c r="C119" s="44"/>
+      <c r="D119" s="69"/>
+      <c r="E119" s="69"/>
+      <c r="F119" s="61"/>
+      <c r="G119" s="74"/>
+      <c r="H119" s="74"/>
+      <c r="I119" s="95"/>
+    </row>
+    <row r="120" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="100"/>
+      <c r="B120" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="C116" s="49"/>
-      <c r="D116" s="78"/>
-      <c r="E116" s="84"/>
-      <c r="F116" s="83"/>
-      <c r="G116" s="101"/>
-      <c r="H116" s="82"/>
-      <c r="I116" s="62"/>
-    </row>
-    <row r="117" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="58"/>
-      <c r="B117" s="52" t="s">
+      <c r="C120" s="49"/>
+      <c r="D120" s="57"/>
+      <c r="E120" s="62"/>
+      <c r="F120" s="61"/>
+      <c r="G120" s="75"/>
+      <c r="H120" s="60"/>
+      <c r="I120" s="95"/>
+    </row>
+    <row r="121" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="100"/>
+      <c r="B121" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="C117" s="49"/>
-      <c r="D117" s="78"/>
-      <c r="E117" s="84"/>
-      <c r="F117" s="83"/>
-      <c r="G117" s="101"/>
-      <c r="H117" s="82"/>
-      <c r="I117" s="62"/>
-    </row>
-    <row r="118" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="59"/>
-      <c r="B118" s="51" t="s">
+      <c r="C121" s="49"/>
+      <c r="D121" s="57"/>
+      <c r="E121" s="62"/>
+      <c r="F121" s="61"/>
+      <c r="G121" s="75"/>
+      <c r="H121" s="60"/>
+      <c r="I121" s="95"/>
+    </row>
+    <row r="122" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="101"/>
+      <c r="B122" s="51" t="s">
         <v>119</v>
       </c>
-      <c r="C118" s="46"/>
-      <c r="D118" s="93"/>
-      <c r="E118" s="95"/>
-      <c r="F118" s="103"/>
-      <c r="G118" s="99"/>
-      <c r="H118" s="79"/>
-      <c r="I118" s="65"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="91" t="s">
+      <c r="C122" s="46"/>
+      <c r="D122" s="68"/>
+      <c r="E122" s="70"/>
+      <c r="F122" s="77"/>
+      <c r="G122" s="73"/>
+      <c r="H122" s="58"/>
+      <c r="I122" s="91"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="110" t="s">
         <v>54</v>
       </c>
-      <c r="B119" s="86" t="s">
+      <c r="B123" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="C119" s="44"/>
-      <c r="D119" s="94"/>
-      <c r="E119" s="94"/>
-      <c r="F119" s="104"/>
-      <c r="G119" s="94"/>
-      <c r="H119" s="94"/>
-      <c r="I119" s="62"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="85"/>
-      <c r="B120" s="52" t="s">
-        <v>118</v>
-      </c>
-      <c r="C120" s="49"/>
-      <c r="D120" s="82"/>
-      <c r="E120" s="82"/>
-      <c r="F120" s="105"/>
-      <c r="G120" s="82"/>
-      <c r="H120" s="82"/>
-      <c r="I120" s="62"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="85"/>
-      <c r="B121" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="C121" s="49"/>
-      <c r="D121" s="82"/>
-      <c r="E121" s="82"/>
-      <c r="F121" s="105"/>
-      <c r="G121" s="82"/>
-      <c r="H121" s="82"/>
-      <c r="I121" s="62"/>
-    </row>
-    <row r="122" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="92"/>
-      <c r="B122" s="51" t="s">
-        <v>122</v>
-      </c>
-      <c r="C122" s="46"/>
-      <c r="D122" s="79"/>
-      <c r="E122" s="79"/>
-      <c r="F122" s="103"/>
-      <c r="G122" s="79"/>
-      <c r="H122" s="79"/>
-      <c r="I122" s="65"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="B123" s="86" t="s">
-        <v>119</v>
-      </c>
       <c r="C123" s="44"/>
-      <c r="D123" s="94"/>
-      <c r="E123" s="94"/>
-      <c r="F123" s="104"/>
-      <c r="G123" s="94"/>
-      <c r="H123" s="94"/>
-      <c r="I123" s="62"/>
+      <c r="D123" s="69"/>
+      <c r="E123" s="69"/>
+      <c r="F123" s="78"/>
+      <c r="G123" s="69"/>
+      <c r="H123" s="69"/>
+      <c r="I123" s="95"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="58"/>
+      <c r="A124" s="111"/>
       <c r="B124" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C124" s="49"/>
-      <c r="D124" s="82"/>
-      <c r="E124" s="82"/>
-      <c r="F124" s="105"/>
-      <c r="G124" s="82"/>
-      <c r="H124" s="82"/>
-      <c r="I124" s="62"/>
+      <c r="D124" s="60"/>
+      <c r="E124" s="60"/>
+      <c r="F124" s="79"/>
+      <c r="G124" s="60"/>
+      <c r="H124" s="60"/>
+      <c r="I124" s="95"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="58"/>
+      <c r="A125" s="111"/>
       <c r="B125" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C125" s="49"/>
-      <c r="D125" s="82"/>
-      <c r="E125" s="82"/>
-      <c r="F125" s="105"/>
-      <c r="G125" s="82"/>
-      <c r="H125" s="82"/>
-      <c r="I125" s="62"/>
+      <c r="D125" s="60"/>
+      <c r="E125" s="60"/>
+      <c r="F125" s="79"/>
+      <c r="G125" s="60"/>
+      <c r="H125" s="60"/>
+      <c r="I125" s="95"/>
     </row>
     <row r="126" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="59"/>
+      <c r="A126" s="112"/>
       <c r="B126" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C126" s="46"/>
-      <c r="D126" s="79"/>
-      <c r="E126" s="79"/>
-      <c r="F126" s="103"/>
-      <c r="G126" s="79"/>
-      <c r="H126" s="79"/>
-      <c r="I126" s="65"/>
+      <c r="D126" s="58"/>
+      <c r="E126" s="58"/>
+      <c r="F126" s="77"/>
+      <c r="G126" s="58"/>
+      <c r="H126" s="58"/>
+      <c r="I126" s="91"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" s="108" t="s">
-        <v>84</v>
-      </c>
-      <c r="B127" s="86" t="s">
+      <c r="A127" s="99" t="s">
+        <v>55</v>
+      </c>
+      <c r="B127" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C127" s="44"/>
-      <c r="D127" s="94"/>
-      <c r="E127" s="94"/>
-      <c r="F127" s="104"/>
-      <c r="G127" s="94"/>
-      <c r="H127" s="94"/>
-      <c r="I127" s="62"/>
+      <c r="D127" s="69"/>
+      <c r="E127" s="69"/>
+      <c r="F127" s="78"/>
+      <c r="G127" s="69"/>
+      <c r="H127" s="69"/>
+      <c r="I127" s="95"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" s="80"/>
+      <c r="A128" s="100"/>
       <c r="B128" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C128" s="49"/>
-      <c r="D128" s="82"/>
-      <c r="E128" s="82"/>
-      <c r="F128" s="105"/>
-      <c r="G128" s="82"/>
-      <c r="H128" s="82"/>
-      <c r="I128" s="62"/>
+      <c r="D128" s="60"/>
+      <c r="E128" s="60"/>
+      <c r="F128" s="79"/>
+      <c r="G128" s="60"/>
+      <c r="H128" s="60"/>
+      <c r="I128" s="95"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="106" t="s">
-        <v>135</v>
-      </c>
+      <c r="A129" s="100"/>
       <c r="B129" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C129" s="49"/>
-      <c r="D129" s="82"/>
-      <c r="E129" s="82"/>
-      <c r="F129" s="105"/>
-      <c r="G129" s="82"/>
-      <c r="H129" s="82"/>
-      <c r="I129" s="62"/>
+      <c r="D129" s="60"/>
+      <c r="E129" s="60"/>
+      <c r="F129" s="79"/>
+      <c r="G129" s="60"/>
+      <c r="H129" s="60"/>
+      <c r="I129" s="95"/>
     </row>
     <row r="130" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="107"/>
+      <c r="A130" s="101"/>
       <c r="B130" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C130" s="46"/>
-      <c r="D130" s="79"/>
-      <c r="E130" s="79"/>
-      <c r="F130" s="103"/>
-      <c r="G130" s="79"/>
-      <c r="H130" s="79"/>
-      <c r="I130" s="65"/>
+      <c r="D130" s="58"/>
+      <c r="E130" s="58"/>
+      <c r="F130" s="77"/>
+      <c r="G130" s="58"/>
+      <c r="H130" s="58"/>
+      <c r="I130" s="91"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="108" t="s">
-        <v>43</v>
-      </c>
-      <c r="B131" s="86" t="s">
+      <c r="A131" s="106" t="s">
+        <v>84</v>
+      </c>
+      <c r="B131" s="63" t="s">
         <v>119</v>
       </c>
       <c r="C131" s="44"/>
-      <c r="D131" s="94"/>
-      <c r="E131" s="94"/>
-      <c r="F131" s="104"/>
-      <c r="G131" s="94"/>
-      <c r="H131" s="94"/>
-      <c r="I131" s="62"/>
+      <c r="D131" s="69"/>
+      <c r="E131" s="69"/>
+      <c r="F131" s="78"/>
+      <c r="G131" s="69"/>
+      <c r="H131" s="69"/>
+      <c r="I131" s="95"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="80"/>
+      <c r="A132" s="107"/>
       <c r="B132" s="52" t="s">
         <v>118</v>
       </c>
       <c r="C132" s="49"/>
-      <c r="D132" s="82"/>
-      <c r="E132" s="82"/>
-      <c r="F132" s="105"/>
-      <c r="G132" s="82"/>
-      <c r="H132" s="82"/>
-      <c r="I132" s="62"/>
+      <c r="D132" s="60"/>
+      <c r="E132" s="60"/>
+      <c r="F132" s="79"/>
+      <c r="G132" s="60"/>
+      <c r="H132" s="60"/>
+      <c r="I132" s="95"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="106" t="s">
+      <c r="A133" s="108" t="s">
         <v>135</v>
       </c>
       <c r="B133" s="52" t="s">
         <v>120</v>
       </c>
       <c r="C133" s="49"/>
-      <c r="D133" s="82"/>
-      <c r="E133" s="82"/>
-      <c r="F133" s="105"/>
-      <c r="G133" s="82"/>
-      <c r="H133" s="82"/>
-      <c r="I133" s="62"/>
+      <c r="D133" s="60"/>
+      <c r="E133" s="60"/>
+      <c r="F133" s="79"/>
+      <c r="G133" s="60"/>
+      <c r="H133" s="60"/>
+      <c r="I133" s="95"/>
     </row>
     <row r="134" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="107"/>
+      <c r="A134" s="109"/>
       <c r="B134" s="51" t="s">
         <v>122</v>
       </c>
       <c r="C134" s="46"/>
-      <c r="D134" s="79"/>
-      <c r="E134" s="79"/>
-      <c r="F134" s="103"/>
-      <c r="G134" s="79"/>
-      <c r="H134" s="79"/>
-      <c r="I134" s="65"/>
+      <c r="D134" s="58"/>
+      <c r="E134" s="58"/>
+      <c r="F134" s="77"/>
+      <c r="G134" s="58"/>
+      <c r="H134" s="58"/>
+      <c r="I134" s="91"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="106" t="s">
+        <v>43</v>
+      </c>
+      <c r="B135" s="63" t="s">
+        <v>119</v>
+      </c>
+      <c r="C135" s="44"/>
+      <c r="D135" s="69"/>
+      <c r="E135" s="69"/>
+      <c r="F135" s="78"/>
+      <c r="G135" s="69"/>
+      <c r="H135" s="69"/>
+      <c r="I135" s="95"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="107"/>
+      <c r="B136" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="C136" s="49"/>
+      <c r="D136" s="60"/>
+      <c r="E136" s="60"/>
+      <c r="F136" s="79"/>
+      <c r="G136" s="60"/>
+      <c r="H136" s="60"/>
+      <c r="I136" s="95"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" s="108" t="s">
+        <v>135</v>
+      </c>
+      <c r="B137" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="C137" s="49"/>
+      <c r="D137" s="60"/>
+      <c r="E137" s="60"/>
+      <c r="F137" s="79"/>
+      <c r="G137" s="60"/>
+      <c r="H137" s="60"/>
+      <c r="I137" s="95"/>
+    </row>
+    <row r="138" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="109"/>
+      <c r="B138" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="C138" s="46"/>
+      <c r="D138" s="58"/>
+      <c r="E138" s="58"/>
+      <c r="F138" s="77"/>
+      <c r="G138" s="58"/>
+      <c r="H138" s="58"/>
+      <c r="I138" s="91"/>
     </row>
   </sheetData>
-  <mergeCells count="72">
-    <mergeCell ref="I107:I110"/>
-    <mergeCell ref="I111:I114"/>
-    <mergeCell ref="I91:I94"/>
-    <mergeCell ref="A131:A132"/>
-    <mergeCell ref="A133:A134"/>
-    <mergeCell ref="A107:A110"/>
-    <mergeCell ref="A111:A114"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="I47:I50"/>
-    <mergeCell ref="I87:I90"/>
-    <mergeCell ref="I103:I106"/>
-    <mergeCell ref="I95:I98"/>
-    <mergeCell ref="I99:I102"/>
-    <mergeCell ref="I71:I74"/>
-    <mergeCell ref="I75:I78"/>
-    <mergeCell ref="I79:I82"/>
-    <mergeCell ref="I83:I86"/>
-    <mergeCell ref="I127:I130"/>
-    <mergeCell ref="I51:I54"/>
-    <mergeCell ref="I55:I58"/>
-    <mergeCell ref="I59:I62"/>
-    <mergeCell ref="I63:I66"/>
-    <mergeCell ref="I67:I70"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="I3:I6"/>
-    <mergeCell ref="I7:I10"/>
+  <mergeCells count="74">
     <mergeCell ref="I11:I14"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="I19:I22"/>
-    <mergeCell ref="I115:I118"/>
-    <mergeCell ref="I23:I26"/>
-    <mergeCell ref="I131:I134"/>
-    <mergeCell ref="I27:I30"/>
-    <mergeCell ref="I31:I34"/>
-    <mergeCell ref="I35:I38"/>
-    <mergeCell ref="I39:I42"/>
-    <mergeCell ref="I119:I122"/>
-    <mergeCell ref="I123:I126"/>
-    <mergeCell ref="I43:I46"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="A123:A126"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A103:A106"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A119:A122"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A115:A118"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A119:A122"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A123:A126"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="A127:A130"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="A107:A110"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="A103:A106"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="I3:I6"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="I19:I22"/>
+    <mergeCell ref="I23:I26"/>
+    <mergeCell ref="I27:I30"/>
+    <mergeCell ref="I31:I34"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="I43:I46"/>
+    <mergeCell ref="I47:I50"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="I51:I54"/>
+    <mergeCell ref="I91:I94"/>
+    <mergeCell ref="I107:I110"/>
+    <mergeCell ref="I99:I102"/>
+    <mergeCell ref="I103:I106"/>
+    <mergeCell ref="I75:I78"/>
+    <mergeCell ref="I79:I82"/>
+    <mergeCell ref="I83:I86"/>
+    <mergeCell ref="I87:I90"/>
+    <mergeCell ref="I55:I58"/>
+    <mergeCell ref="I59:I62"/>
+    <mergeCell ref="I63:I66"/>
+    <mergeCell ref="I67:I70"/>
+    <mergeCell ref="I71:I74"/>
+    <mergeCell ref="I111:I114"/>
+    <mergeCell ref="I115:I118"/>
+    <mergeCell ref="I95:I98"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A111:A114"/>
+    <mergeCell ref="A115:A118"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="I131:I134"/>
+    <mergeCell ref="I119:I122"/>
+    <mergeCell ref="I135:I138"/>
+    <mergeCell ref="I123:I126"/>
+    <mergeCell ref="I127:I130"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="A133:A134"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4241,7 +4328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -4253,33 +4340,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="102" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="114" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="81"/>
+      <c r="E1" s="114"/>
       <c r="F1" s="47" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
+      <c r="A2" s="103"/>
+      <c r="B2" s="103"/>
       <c r="C2" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="79" t="s">
+      <c r="E2" s="58" t="s">
         <v>128</v>
       </c>
       <c r="F2" s="48" t="s">
@@ -4287,7 +4374,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="89" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -4296,15 +4383,15 @@
       <c r="C3" s="30">
         <v>10</v>
       </c>
-      <c r="D3" s="109">
+      <c r="D3" s="81">
         <v>43118</v>
       </c>
-      <c r="E3" s="109">
+      <c r="E3" s="81">
         <v>43128</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
+      <c r="A4" s="95"/>
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
@@ -4313,7 +4400,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
+      <c r="A5" s="95"/>
       <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
@@ -4322,7 +4409,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
+      <c r="A6" s="95"/>
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
@@ -4331,7 +4418,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
+      <c r="A7" s="95"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
@@ -4340,7 +4427,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="62"/>
+      <c r="A8" s="95"/>
       <c r="B8" s="8" t="s">
         <v>116</v>
       </c>
@@ -4352,7 +4439,7 @@
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="89" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -4360,13 +4447,13 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
+      <c r="A10" s="95"/>
       <c r="B10" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="65"/>
+      <c r="A11" s="91"/>
       <c r="B11" s="12" t="s">
         <v>20</v>
       </c>
@@ -4396,7 +4483,7 @@
       <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="89" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="42" t="s">
@@ -4404,13 +4491,13 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
+      <c r="A15" s="95"/>
       <c r="B15" s="42" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="65"/>
+      <c r="A16" s="91"/>
       <c r="B16" s="43" t="s">
         <v>32</v>
       </c>
@@ -4420,7 +4507,7 @@
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="89" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -4428,25 +4515,25 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="74"/>
+      <c r="A18" s="90"/>
       <c r="B18" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="74"/>
+      <c r="A19" s="90"/>
       <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="74"/>
+      <c r="A20" s="90"/>
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="91"/>
       <c r="B21" s="19" t="s">
         <v>40</v>
       </c>
@@ -4492,7 +4579,7 @@
       <c r="F24" s="15"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="68" t="s">
+      <c r="A25" s="82" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -4500,13 +4587,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="70"/>
+      <c r="A26" s="83"/>
       <c r="B26" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="69"/>
+      <c r="A27" s="84"/>
       <c r="B27" s="19" t="s">
         <v>53</v>
       </c>
@@ -4528,7 +4615,7 @@
       <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="68" t="s">
+      <c r="A29" s="82" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -4536,33 +4623,33 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="73"/>
+      <c r="A30" s="98"/>
       <c r="B30" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="73"/>
-      <c r="B31" s="71" t="s">
+      <c r="A31" s="98"/>
+      <c r="B31" s="96" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="73"/>
-      <c r="B32" s="71"/>
+      <c r="A32" s="98"/>
+      <c r="B32" s="96"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="73"/>
-      <c r="B33" s="71" t="s">
+      <c r="A33" s="98"/>
+      <c r="B33" s="96" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="73"/>
-      <c r="B34" s="71"/>
+      <c r="A34" s="98"/>
+      <c r="B34" s="96"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="69"/>
+      <c r="A35" s="84"/>
       <c r="B35" s="9" t="s">
         <v>59</v>
       </c>
@@ -4584,7 +4671,7 @@
       <c r="F36" s="15"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="68" t="s">
+      <c r="A37" s="82" t="s">
         <v>76</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -4592,19 +4679,19 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="70"/>
+      <c r="A38" s="83"/>
       <c r="B38" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="70"/>
+      <c r="A39" s="83"/>
       <c r="B39" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="70"/>
+      <c r="A40" s="83"/>
       <c r="B40" s="3" t="s">
         <v>80</v>
       </c>
@@ -4626,7 +4713,7 @@
       <c r="F41" s="15"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="68" t="s">
+      <c r="A42" s="82" t="s">
         <v>92</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -4634,7 +4721,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="69"/>
+      <c r="A43" s="84"/>
       <c r="B43" s="8" t="s">
         <v>87</v>
       </c>
@@ -4644,7 +4731,7 @@
       <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="68" t="s">
+      <c r="A44" s="82" t="s">
         <v>93</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -4652,25 +4739,25 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="70"/>
+      <c r="A45" s="83"/>
       <c r="B45" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="70"/>
+      <c r="A46" s="83"/>
       <c r="B46" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="70"/>
+      <c r="A47" s="83"/>
       <c r="B47" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="69"/>
+      <c r="A48" s="84"/>
       <c r="B48" s="9" t="s">
         <v>86</v>
       </c>
@@ -4680,7 +4767,7 @@
       <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="68" t="s">
+      <c r="A49" s="82" t="s">
         <v>97</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -4688,13 +4775,13 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="70"/>
+      <c r="A50" s="83"/>
       <c r="B50" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="69"/>
+      <c r="A51" s="84"/>
       <c r="B51" s="8" t="s">
         <v>98</v>
       </c>
@@ -4729,6 +4816,10 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A49:A51"/>
@@ -4740,10 +4831,6 @@
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[DataAccess] GetLineupsofContest task 89
</commit_message>
<xml_diff>
--- a/schedules/Time Estimations.xlsx
+++ b/schedules/Time Estimations.xlsx
@@ -862,105 +862,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -971,9 +872,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1012,23 +910,125 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1332,37 +1332,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="113" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="113" t="s">
+      <c r="B1" s="127" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="127" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="113" t="s">
+      <c r="D1" s="127" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="113"/>
-      <c r="F1" s="115" t="s">
+      <c r="E1" s="127"/>
+      <c r="F1" s="130" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="114"/>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
+      <c r="A2" s="128"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
       <c r="D2" s="29" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="116"/>
+      <c r="F2" s="131"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="125" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1382,7 +1382,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="106"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="106"/>
+      <c r="A5" s="126"/>
       <c r="B5" s="6" t="s">
         <v>139</v>
       </c>
@@ -1414,7 +1414,7 @@
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="106"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
@@ -1430,7 +1430,7 @@
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="106"/>
+      <c r="A7" s="126"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="106"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="8" t="s">
         <v>115</v>
       </c>
@@ -1460,7 +1460,7 @@
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="125" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -1469,7 +1469,7 @@
       <c r="C9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="99" t="s">
+      <c r="D9" s="119" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="33">
@@ -1480,27 +1480,27 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="106"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="96"/>
+      <c r="D10" s="124"/>
       <c r="E10" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="102"/>
+      <c r="A11" s="129"/>
       <c r="B11" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="98"/>
+      <c r="D11" s="120"/>
       <c r="E11" s="32" t="s">
         <v>24</v>
       </c>
@@ -1543,47 +1543,47 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="125" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="103" t="s">
+      <c r="C14" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="97" t="s">
+      <c r="D14" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="97">
+      <c r="E14" s="118">
         <v>0.5</v>
       </c>
-      <c r="F14" s="110" t="s">
+      <c r="F14" s="121" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="106"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="99"/>
-      <c r="E15" s="99"/>
-      <c r="F15" s="111"/>
+      <c r="C15" s="140"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="122"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="102"/>
+      <c r="A16" s="129"/>
       <c r="B16" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="105"/>
-      <c r="D16" s="98"/>
-      <c r="E16" s="98"/>
-      <c r="F16" s="112"/>
+      <c r="C16" s="141"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="123"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="100" t="s">
+      <c r="A17" s="125" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1592,7 +1592,7 @@
       <c r="C17" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="97" t="s">
+      <c r="D17" s="118" t="s">
         <v>34</v>
       </c>
       <c r="E17" s="33">
@@ -1603,53 +1603,53 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="101"/>
+      <c r="A18" s="138"/>
       <c r="B18" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="99"/>
+      <c r="D18" s="119"/>
       <c r="E18" s="33" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="101"/>
+      <c r="A19" s="138"/>
       <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C19" t="s">
         <v>128</v>
       </c>
-      <c r="D19" s="99"/>
+      <c r="D19" s="119"/>
       <c r="E19" s="33">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="101"/>
+      <c r="A20" s="138"/>
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C20" t="s">
         <v>129</v>
       </c>
-      <c r="D20" s="99"/>
+      <c r="D20" s="119"/>
       <c r="E20" s="33">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="102"/>
+      <c r="A21" s="129"/>
       <c r="B21" s="19" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="98"/>
+      <c r="D21" s="120"/>
       <c r="E21" s="32" t="s">
         <v>24</v>
       </c>
@@ -1712,7 +1712,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="93" t="s">
+      <c r="A25" s="134" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1721,7 +1721,7 @@
       <c r="C25" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="97" t="s">
+      <c r="D25" s="118" t="s">
         <v>34</v>
       </c>
       <c r="E25" s="33">
@@ -1732,27 +1732,27 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="94"/>
+      <c r="A26" s="135"/>
       <c r="B26" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="96"/>
+      <c r="D26" s="124"/>
       <c r="E26" s="33">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="95"/>
+      <c r="A27" s="136"/>
       <c r="B27" s="19" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="98"/>
+      <c r="D27" s="120"/>
       <c r="E27" s="32">
         <v>2</v>
       </c>
@@ -1779,7 +1779,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="93" t="s">
+      <c r="A29" s="134" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1796,7 +1796,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="109"/>
+      <c r="A30" s="137"/>
       <c r="B30" s="3" t="s">
         <v>63</v>
       </c>
@@ -1811,14 +1811,14 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="109"/>
-      <c r="B31" s="107" t="s">
+      <c r="A31" s="137"/>
+      <c r="B31" s="132" t="s">
         <v>64</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="96">
+      <c r="D31" s="124">
         <v>3</v>
       </c>
       <c r="E31" s="33">
@@ -1829,25 +1829,25 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="109"/>
-      <c r="B32" s="107"/>
+      <c r="A32" s="137"/>
+      <c r="B32" s="132"/>
       <c r="C32" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="96"/>
+      <c r="D32" s="124"/>
       <c r="E32" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="109"/>
-      <c r="B33" s="107" t="s">
+      <c r="A33" s="137"/>
+      <c r="B33" s="132" t="s">
         <v>65</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="96">
+      <c r="D33" s="124">
         <v>3</v>
       </c>
       <c r="E33" s="33">
@@ -1858,12 +1858,12 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="109"/>
-      <c r="B34" s="107"/>
+      <c r="A34" s="137"/>
+      <c r="B34" s="132"/>
       <c r="C34" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="96"/>
+      <c r="D34" s="124"/>
       <c r="E34" s="33">
         <v>1</v>
       </c>
@@ -1872,7 +1872,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="95"/>
+      <c r="A35" s="136"/>
       <c r="B35" s="9" t="s">
         <v>59</v>
       </c>
@@ -1910,7 +1910,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="93" t="s">
+      <c r="A37" s="134" t="s">
         <v>76</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1930,7 +1930,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="94"/>
+      <c r="A38" s="135"/>
       <c r="B38" s="3" t="s">
         <v>78</v>
       </c>
@@ -1945,7 +1945,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="94"/>
+      <c r="A39" s="135"/>
       <c r="B39" s="3" t="s">
         <v>79</v>
       </c>
@@ -1960,8 +1960,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="94"/>
-      <c r="B40" s="107" t="s">
+      <c r="A40" s="135"/>
+      <c r="B40" s="132" t="s">
         <v>80</v>
       </c>
       <c r="C40" t="s">
@@ -1975,8 +1975,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="95"/>
-      <c r="B41" s="108"/>
+      <c r="A41" s="136"/>
+      <c r="B41" s="133"/>
       <c r="C41" s="9" t="s">
         <v>84</v>
       </c>
@@ -2007,7 +2007,7 @@
       <c r="F42" s="15"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="93" t="s">
+      <c r="A43" s="134" t="s">
         <v>92</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2016,7 +2016,7 @@
       <c r="C43" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="97" t="s">
+      <c r="D43" s="118" t="s">
         <v>34</v>
       </c>
       <c r="E43" s="33">
@@ -2027,14 +2027,14 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="95"/>
+      <c r="A44" s="136"/>
       <c r="B44" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="98"/>
+      <c r="D44" s="120"/>
       <c r="E44" s="32" t="s">
         <v>24</v>
       </c>
@@ -2043,7 +2043,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="93" t="s">
+      <c r="A45" s="134" t="s">
         <v>93</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -2052,7 +2052,7 @@
       <c r="C45" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D45" s="97" t="s">
+      <c r="D45" s="118" t="s">
         <v>34</v>
       </c>
       <c r="E45" s="33">
@@ -2060,56 +2060,56 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="94"/>
+      <c r="A46" s="135"/>
       <c r="B46" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="96"/>
-      <c r="E46" s="96" t="s">
+      <c r="D46" s="124"/>
+      <c r="E46" s="124" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="94"/>
+      <c r="A47" s="135"/>
       <c r="B47" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D47" s="96"/>
-      <c r="E47" s="96"/>
+      <c r="D47" s="124"/>
+      <c r="E47" s="124"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="94"/>
+      <c r="A48" s="135"/>
       <c r="B48" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="96"/>
-      <c r="E48" s="96"/>
+      <c r="D48" s="124"/>
+      <c r="E48" s="124"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="95"/>
+      <c r="A49" s="136"/>
       <c r="B49" s="9" t="s">
         <v>86</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D49" s="98"/>
+      <c r="D49" s="120"/>
       <c r="E49" s="32">
         <v>3</v>
       </c>
       <c r="F49" s="9"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="93" t="s">
+      <c r="A50" s="134" t="s">
         <v>97</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -2118,7 +2118,7 @@
       <c r="C50" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D50" s="97" t="s">
+      <c r="D50" s="118" t="s">
         <v>34</v>
       </c>
       <c r="E50" s="33">
@@ -2126,27 +2126,27 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="94"/>
+      <c r="A51" s="135"/>
       <c r="B51" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D51" s="96"/>
+      <c r="D51" s="124"/>
       <c r="E51" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="95"/>
+      <c r="A52" s="136"/>
       <c r="B52" s="8" t="s">
         <v>98</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D52" s="98"/>
+      <c r="D52" s="120"/>
       <c r="E52" s="32">
         <v>2</v>
       </c>
@@ -2227,6 +2227,27 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D45:D49"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="A37:A41"/>
     <mergeCell ref="E14:E16"/>
     <mergeCell ref="F14:F16"/>
     <mergeCell ref="D9:D11"/>
@@ -2237,27 +2258,6 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="D17:D21"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D45:D49"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2268,8 +2268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J91" sqref="J91:J114"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91:B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2281,7 +2281,7 @@
     <col min="5" max="6" width="11.42578125" style="50"/>
     <col min="7" max="7" width="13.42578125" style="72" customWidth="1"/>
     <col min="8" max="9" width="11.42578125" style="50"/>
-    <col min="11" max="11" width="21.28515625" style="133" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" style="99" customWidth="1"/>
     <col min="12" max="12" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2289,37 +2289,37 @@
       <c r="A1" s="147" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="111" t="s">
+      <c r="B1" s="122" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="111" t="s">
+      <c r="C1" s="122" t="s">
         <v>120</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="125" t="s">
+      <c r="E1" s="148" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="125"/>
+      <c r="F1" s="148"/>
       <c r="G1" s="72" t="s">
         <v>124</v>
       </c>
-      <c r="H1" s="125" t="s">
+      <c r="H1" s="148" t="s">
         <v>125</v>
       </c>
-      <c r="I1" s="125"/>
+      <c r="I1" s="148"/>
       <c r="J1" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="K1" s="130" t="s">
+      <c r="K1" s="142" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="147"/>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
       <c r="D2" s="46" t="s">
         <v>122</v>
       </c>
@@ -2341,13 +2341,13 @@
       <c r="J2" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="K2" s="130"/>
+      <c r="K2" s="142"/>
     </row>
     <row r="3" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="148">
-        <v>1</v>
-      </c>
-      <c r="B3" s="110" t="s">
+      <c r="A3" s="113">
+        <v>1</v>
+      </c>
+      <c r="B3" s="121" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="59" t="s">
@@ -2359,16 +2359,16 @@
       <c r="G3" s="74"/>
       <c r="H3" s="60"/>
       <c r="I3" s="60"/>
-      <c r="J3" s="117">
-        <v>1</v>
-      </c>
-      <c r="K3" s="131"/>
+      <c r="J3" s="146">
+        <v>1</v>
+      </c>
+      <c r="K3" s="97"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="149">
+      <c r="A4" s="114">
         <v>2</v>
       </c>
-      <c r="B4" s="111"/>
+      <c r="B4" s="122"/>
       <c r="C4" s="52" t="s">
         <v>117</v>
       </c>
@@ -2378,14 +2378,14 @@
       <c r="G4" s="75"/>
       <c r="H4" s="56"/>
       <c r="I4" s="56"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="132"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="98"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="149">
+      <c r="A5" s="114">
         <v>3</v>
       </c>
-      <c r="B5" s="111"/>
+      <c r="B5" s="122"/>
       <c r="C5" s="52" t="s">
         <v>119</v>
       </c>
@@ -2395,14 +2395,14 @@
       <c r="G5" s="75"/>
       <c r="H5" s="56"/>
       <c r="I5" s="56"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="132"/>
+      <c r="J5" s="126"/>
+      <c r="K5" s="98"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="150">
+      <c r="A6" s="115">
         <v>4</v>
       </c>
-      <c r="B6" s="112"/>
+      <c r="B6" s="123"/>
       <c r="C6" s="51" t="s">
         <v>121</v>
       </c>
@@ -2412,14 +2412,14 @@
       <c r="G6" s="73"/>
       <c r="H6" s="55"/>
       <c r="I6" s="55"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="132"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="98"/>
     </row>
     <row r="7" spans="1:11" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="148">
+      <c r="A7" s="113">
         <v>5</v>
       </c>
-      <c r="B7" s="110" t="s">
+      <c r="B7" s="121" t="s">
         <v>141</v>
       </c>
       <c r="C7" s="86" t="s">
@@ -2443,16 +2443,16 @@
       <c r="I7" s="61">
         <v>43121</v>
       </c>
-      <c r="J7" s="117">
+      <c r="J7" s="146">
         <v>0.25</v>
       </c>
-      <c r="K7" s="131"/>
+      <c r="K7" s="97"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="149">
+      <c r="A8" s="114">
         <v>6</v>
       </c>
-      <c r="B8" s="111"/>
+      <c r="B8" s="122"/>
       <c r="C8" s="87" t="s">
         <v>117</v>
       </c>
@@ -2462,13 +2462,13 @@
       <c r="G8" s="75"/>
       <c r="H8" s="56"/>
       <c r="I8" s="56"/>
-      <c r="J8" s="106"/>
+      <c r="J8" s="126"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="149">
+      <c r="A9" s="114">
         <v>7</v>
       </c>
-      <c r="B9" s="111"/>
+      <c r="B9" s="122"/>
       <c r="C9" s="87" t="s">
         <v>119</v>
       </c>
@@ -2478,13 +2478,13 @@
       <c r="G9" s="75"/>
       <c r="H9" s="56"/>
       <c r="I9" s="56"/>
-      <c r="J9" s="106"/>
+      <c r="J9" s="126"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="150">
+      <c r="A10" s="115">
         <v>8</v>
       </c>
-      <c r="B10" s="112"/>
+      <c r="B10" s="123"/>
       <c r="C10" s="51" t="s">
         <v>121</v>
       </c>
@@ -2494,13 +2494,13 @@
       <c r="G10" s="73"/>
       <c r="H10" s="55"/>
       <c r="I10" s="55"/>
-      <c r="J10" s="102"/>
+      <c r="J10" s="129"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="148">
+      <c r="A11" s="113">
         <v>9</v>
       </c>
-      <c r="B11" s="110" t="s">
+      <c r="B11" s="121" t="s">
         <v>137</v>
       </c>
       <c r="C11" s="59" t="s">
@@ -2524,16 +2524,16 @@
       <c r="I11" s="65">
         <v>43118</v>
       </c>
-      <c r="J11" s="117">
+      <c r="J11" s="146">
         <v>0.25</v>
       </c>
-      <c r="K11" s="132"/>
+      <c r="K11" s="98"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="149">
+      <c r="A12" s="114">
         <v>10</v>
       </c>
-      <c r="B12" s="111"/>
+      <c r="B12" s="122"/>
       <c r="C12" s="52" t="s">
         <v>117</v>
       </c>
@@ -2542,13 +2542,13 @@
       <c r="F12" s="58"/>
       <c r="H12" s="71"/>
       <c r="I12" s="58"/>
-      <c r="J12" s="106"/>
+      <c r="J12" s="126"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="149">
+      <c r="A13" s="114">
         <v>11</v>
       </c>
-      <c r="B13" s="111"/>
+      <c r="B13" s="122"/>
       <c r="C13" s="52" t="s">
         <v>119</v>
       </c>
@@ -2557,13 +2557,13 @@
       <c r="F13" s="58"/>
       <c r="H13" s="71"/>
       <c r="I13" s="62"/>
-      <c r="J13" s="106"/>
+      <c r="J13" s="126"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="150">
+      <c r="A14" s="115">
         <v>12</v>
       </c>
-      <c r="B14" s="112"/>
+      <c r="B14" s="123"/>
       <c r="C14" s="51" t="s">
         <v>121</v>
       </c>
@@ -2573,13 +2573,13 @@
       <c r="G14" s="73"/>
       <c r="H14" s="69"/>
       <c r="I14" s="63"/>
-      <c r="J14" s="102"/>
+      <c r="J14" s="129"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="148">
+      <c r="A15" s="113">
         <v>13</v>
       </c>
-      <c r="B15" s="110" t="s">
+      <c r="B15" s="121" t="s">
         <v>138</v>
       </c>
       <c r="C15" s="80" t="s">
@@ -2603,16 +2603,16 @@
       <c r="I15" s="65">
         <v>43118</v>
       </c>
-      <c r="J15" s="117">
+      <c r="J15" s="146">
         <v>0.25</v>
       </c>
-      <c r="K15" s="132"/>
+      <c r="K15" s="98"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="149">
+      <c r="A16" s="114">
         <v>14</v>
       </c>
-      <c r="B16" s="111"/>
+      <c r="B16" s="122"/>
       <c r="C16" s="81" t="s">
         <v>117</v>
       </c>
@@ -2621,13 +2621,13 @@
       <c r="F16" s="58"/>
       <c r="H16" s="71"/>
       <c r="I16" s="58"/>
-      <c r="J16" s="106"/>
+      <c r="J16" s="126"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="149">
+      <c r="A17" s="114">
         <v>15</v>
       </c>
-      <c r="B17" s="111"/>
+      <c r="B17" s="122"/>
       <c r="C17" s="81" t="s">
         <v>119</v>
       </c>
@@ -2636,13 +2636,13 @@
       <c r="F17" s="58"/>
       <c r="H17" s="71"/>
       <c r="I17" s="62"/>
-      <c r="J17" s="106"/>
+      <c r="J17" s="126"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="150">
+      <c r="A18" s="115">
         <v>16</v>
       </c>
-      <c r="B18" s="112"/>
+      <c r="B18" s="123"/>
       <c r="C18" s="51" t="s">
         <v>121</v>
       </c>
@@ -2652,13 +2652,13 @@
       <c r="G18" s="73"/>
       <c r="H18" s="69"/>
       <c r="I18" s="63"/>
-      <c r="J18" s="102"/>
+      <c r="J18" s="129"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="148">
+      <c r="A19" s="113">
         <v>17</v>
       </c>
-      <c r="B19" s="110" t="s">
+      <c r="B19" s="121" t="s">
         <v>135</v>
       </c>
       <c r="C19" s="80" t="s">
@@ -2682,16 +2682,16 @@
       <c r="I19" s="65">
         <v>43118</v>
       </c>
-      <c r="J19" s="117">
+      <c r="J19" s="146">
         <v>0.25</v>
       </c>
-      <c r="K19" s="132"/>
+      <c r="K19" s="98"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="149">
+      <c r="A20" s="114">
         <v>18</v>
       </c>
-      <c r="B20" s="111"/>
+      <c r="B20" s="122"/>
       <c r="C20" s="81" t="s">
         <v>117</v>
       </c>
@@ -2700,13 +2700,13 @@
       <c r="F20" s="58"/>
       <c r="H20" s="71"/>
       <c r="I20" s="58"/>
-      <c r="J20" s="106"/>
+      <c r="J20" s="126"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="149">
+      <c r="A21" s="114">
         <v>19</v>
       </c>
-      <c r="B21" s="111"/>
+      <c r="B21" s="122"/>
       <c r="C21" s="81" t="s">
         <v>119</v>
       </c>
@@ -2715,13 +2715,13 @@
       <c r="F21" s="58"/>
       <c r="H21" s="71"/>
       <c r="I21" s="62"/>
-      <c r="J21" s="106"/>
+      <c r="J21" s="126"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="150">
+      <c r="A22" s="115">
         <v>20</v>
       </c>
-      <c r="B22" s="112"/>
+      <c r="B22" s="123"/>
       <c r="C22" s="51" t="s">
         <v>121</v>
       </c>
@@ -2731,13 +2731,13 @@
       <c r="G22" s="73"/>
       <c r="H22" s="69"/>
       <c r="I22" s="63"/>
-      <c r="J22" s="102"/>
+      <c r="J22" s="129"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="148">
+      <c r="A23" s="113">
         <v>21</v>
       </c>
-      <c r="B23" s="110" t="s">
+      <c r="B23" s="121" t="s">
         <v>136</v>
       </c>
       <c r="C23" s="80" t="s">
@@ -2761,16 +2761,16 @@
       <c r="I23" s="65">
         <v>43118</v>
       </c>
-      <c r="J23" s="117">
+      <c r="J23" s="146">
         <v>0.25</v>
       </c>
-      <c r="K23" s="132"/>
+      <c r="K23" s="98"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="149">
+      <c r="A24" s="114">
         <v>22</v>
       </c>
-      <c r="B24" s="111"/>
+      <c r="B24" s="122"/>
       <c r="C24" s="81" t="s">
         <v>117</v>
       </c>
@@ -2779,13 +2779,13 @@
       <c r="F24" s="58"/>
       <c r="H24" s="71"/>
       <c r="I24" s="58"/>
-      <c r="J24" s="106"/>
+      <c r="J24" s="126"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="149">
+      <c r="A25" s="114">
         <v>23</v>
       </c>
-      <c r="B25" s="111"/>
+      <c r="B25" s="122"/>
       <c r="C25" s="81" t="s">
         <v>119</v>
       </c>
@@ -2794,13 +2794,13 @@
       <c r="F25" s="58"/>
       <c r="H25" s="71"/>
       <c r="I25" s="62"/>
-      <c r="J25" s="106"/>
+      <c r="J25" s="126"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="150">
+      <c r="A26" s="115">
         <v>24</v>
       </c>
-      <c r="B26" s="112"/>
+      <c r="B26" s="123"/>
       <c r="C26" s="51" t="s">
         <v>121</v>
       </c>
@@ -2810,13 +2810,13 @@
       <c r="G26" s="73"/>
       <c r="H26" s="69"/>
       <c r="I26" s="63"/>
-      <c r="J26" s="102"/>
+      <c r="J26" s="129"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="148">
+      <c r="A27" s="113">
         <v>25</v>
       </c>
-      <c r="B27" s="110" t="s">
+      <c r="B27" s="121" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="59" t="s">
@@ -2840,16 +2840,16 @@
       <c r="I27" s="65">
         <v>43121</v>
       </c>
-      <c r="J27" s="117">
+      <c r="J27" s="146">
         <v>0.25</v>
       </c>
-      <c r="K27" s="132"/>
+      <c r="K27" s="98"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="149">
+      <c r="A28" s="114">
         <v>26</v>
       </c>
-      <c r="B28" s="111"/>
+      <c r="B28" s="122"/>
       <c r="C28" s="52" t="s">
         <v>117</v>
       </c>
@@ -2858,13 +2858,13 @@
       <c r="F28" s="58"/>
       <c r="H28" s="71"/>
       <c r="I28" s="56"/>
-      <c r="J28" s="106"/>
+      <c r="J28" s="126"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="149">
+      <c r="A29" s="114">
         <v>27</v>
       </c>
-      <c r="B29" s="111"/>
+      <c r="B29" s="122"/>
       <c r="C29" s="52" t="s">
         <v>119</v>
       </c>
@@ -2873,13 +2873,13 @@
       <c r="F29" s="58"/>
       <c r="H29" s="71"/>
       <c r="I29" s="56"/>
-      <c r="J29" s="106"/>
+      <c r="J29" s="126"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="150">
+      <c r="A30" s="115">
         <v>28</v>
       </c>
-      <c r="B30" s="112"/>
+      <c r="B30" s="123"/>
       <c r="C30" s="51" t="s">
         <v>121</v>
       </c>
@@ -2889,13 +2889,13 @@
       <c r="G30" s="73"/>
       <c r="H30" s="69"/>
       <c r="I30" s="55"/>
-      <c r="J30" s="102"/>
+      <c r="J30" s="129"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="148">
+      <c r="A31" s="113">
         <v>29</v>
       </c>
-      <c r="B31" s="110" t="s">
+      <c r="B31" s="121" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="59" t="s">
@@ -2919,16 +2919,16 @@
       <c r="I31" s="65">
         <v>43121</v>
       </c>
-      <c r="J31" s="117">
+      <c r="J31" s="146">
         <v>0.25</v>
       </c>
-      <c r="K31" s="132"/>
+      <c r="K31" s="98"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="149">
+      <c r="A32" s="114">
         <v>30</v>
       </c>
-      <c r="B32" s="111"/>
+      <c r="B32" s="122"/>
       <c r="C32" s="52" t="s">
         <v>117</v>
       </c>
@@ -2937,13 +2937,13 @@
       <c r="F32" s="58"/>
       <c r="H32" s="71"/>
       <c r="I32" s="56"/>
-      <c r="J32" s="106"/>
+      <c r="J32" s="126"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="149">
+      <c r="A33" s="114">
         <v>31</v>
       </c>
-      <c r="B33" s="111"/>
+      <c r="B33" s="122"/>
       <c r="C33" s="52" t="s">
         <v>119</v>
       </c>
@@ -2952,13 +2952,13 @@
       <c r="F33" s="58"/>
       <c r="H33" s="71"/>
       <c r="I33" s="56"/>
-      <c r="J33" s="106"/>
+      <c r="J33" s="126"/>
     </row>
     <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="150">
+      <c r="A34" s="115">
         <v>32</v>
       </c>
-      <c r="B34" s="112"/>
+      <c r="B34" s="123"/>
       <c r="C34" s="51" t="s">
         <v>121</v>
       </c>
@@ -2968,13 +2968,13 @@
       <c r="G34" s="73"/>
       <c r="H34" s="69"/>
       <c r="I34" s="55"/>
-      <c r="J34" s="102"/>
+      <c r="J34" s="129"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="148">
+      <c r="A35" s="113">
         <v>33</v>
       </c>
-      <c r="B35" s="110" t="s">
+      <c r="B35" s="121" t="s">
         <v>14</v>
       </c>
       <c r="C35" s="59" t="s">
@@ -2992,25 +2992,25 @@
       <c r="G35" s="72">
         <v>1</v>
       </c>
-      <c r="H35" s="126">
+      <c r="H35" s="93">
         <v>43121</v>
       </c>
-      <c r="I35" s="127">
+      <c r="I35" s="94">
         <v>43121</v>
       </c>
-      <c r="J35" s="117">
+      <c r="J35" s="146">
         <v>0.25</v>
       </c>
-      <c r="K35" s="132"/>
-      <c r="L35" s="134" t="s">
+      <c r="K35" s="98"/>
+      <c r="L35" s="100" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="149">
+      <c r="A36" s="114">
         <v>34</v>
       </c>
-      <c r="B36" s="111"/>
+      <c r="B36" s="122"/>
       <c r="C36" s="52" t="s">
         <v>117</v>
       </c>
@@ -3019,16 +3019,16 @@
       <c r="F36" s="54"/>
       <c r="H36" s="71"/>
       <c r="I36" s="56"/>
-      <c r="J36" s="106"/>
-      <c r="L36" s="134" t="s">
+      <c r="J36" s="126"/>
+      <c r="L36" s="100" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="149">
+      <c r="A37" s="114">
         <v>35</v>
       </c>
-      <c r="B37" s="111"/>
+      <c r="B37" s="122"/>
       <c r="C37" s="52" t="s">
         <v>119</v>
       </c>
@@ -3037,14 +3037,14 @@
       <c r="F37" s="54"/>
       <c r="H37" s="71"/>
       <c r="I37" s="56"/>
-      <c r="J37" s="106"/>
-      <c r="K37" s="135"/>
+      <c r="J37" s="126"/>
+      <c r="K37" s="101"/>
     </row>
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="150">
+      <c r="A38" s="115">
         <v>36</v>
       </c>
-      <c r="B38" s="112"/>
+      <c r="B38" s="123"/>
       <c r="C38" s="51" t="s">
         <v>121</v>
       </c>
@@ -3054,14 +3054,14 @@
       <c r="G38" s="73"/>
       <c r="H38" s="69"/>
       <c r="I38" s="55"/>
-      <c r="J38" s="102"/>
-      <c r="K38" s="135"/>
+      <c r="J38" s="129"/>
+      <c r="K38" s="101"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="148">
+      <c r="A39" s="113">
         <v>37</v>
       </c>
-      <c r="B39" s="120" t="s">
+      <c r="B39" s="143" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="59" t="s">
@@ -3079,22 +3079,22 @@
       <c r="G39" s="72">
         <v>1</v>
       </c>
-      <c r="H39" s="126">
+      <c r="H39" s="93">
         <v>43121</v>
       </c>
-      <c r="I39" s="127">
+      <c r="I39" s="94">
         <v>43121</v>
       </c>
-      <c r="J39" s="117">
+      <c r="J39" s="146">
         <v>0.25</v>
       </c>
-      <c r="K39" s="132"/>
+      <c r="K39" s="98"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="149">
+      <c r="A40" s="114">
         <v>38</v>
       </c>
-      <c r="B40" s="121"/>
+      <c r="B40" s="144"/>
       <c r="C40" s="52" t="s">
         <v>117</v>
       </c>
@@ -3104,13 +3104,13 @@
       <c r="G40" s="75"/>
       <c r="H40" s="56"/>
       <c r="I40" s="56"/>
-      <c r="J40" s="106"/>
+      <c r="J40" s="126"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="149">
+      <c r="A41" s="114">
         <v>39</v>
       </c>
-      <c r="B41" s="121"/>
+      <c r="B41" s="144"/>
       <c r="C41" s="52" t="s">
         <v>119</v>
       </c>
@@ -3120,13 +3120,13 @@
       <c r="G41" s="75"/>
       <c r="H41" s="56"/>
       <c r="I41" s="56"/>
-      <c r="J41" s="106"/>
+      <c r="J41" s="126"/>
     </row>
     <row r="42" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="150">
+      <c r="A42" s="115">
         <v>40</v>
       </c>
-      <c r="B42" s="122"/>
+      <c r="B42" s="145"/>
       <c r="C42" s="51" t="s">
         <v>121</v>
       </c>
@@ -3136,13 +3136,13 @@
       <c r="G42" s="73"/>
       <c r="H42" s="55"/>
       <c r="I42" s="55"/>
-      <c r="J42" s="102"/>
+      <c r="J42" s="129"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="148">
+      <c r="A43" s="113">
         <v>41</v>
       </c>
-      <c r="B43" s="110" t="s">
+      <c r="B43" s="121" t="s">
         <v>128</v>
       </c>
       <c r="C43" s="59" t="s">
@@ -3160,22 +3160,22 @@
       <c r="G43" s="72">
         <v>1</v>
       </c>
-      <c r="H43" s="126">
+      <c r="H43" s="93">
         <v>43121</v>
       </c>
-      <c r="I43" s="127">
+      <c r="I43" s="94">
         <v>43121</v>
       </c>
-      <c r="J43" s="117">
+      <c r="J43" s="146">
         <v>0.25</v>
       </c>
-      <c r="K43" s="132"/>
+      <c r="K43" s="98"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="149">
+      <c r="A44" s="114">
         <v>42</v>
       </c>
-      <c r="B44" s="111"/>
+      <c r="B44" s="122"/>
       <c r="C44" s="52" t="s">
         <v>117</v>
       </c>
@@ -3185,13 +3185,13 @@
       <c r="G44" s="75"/>
       <c r="H44" s="56"/>
       <c r="I44" s="56"/>
-      <c r="J44" s="106"/>
+      <c r="J44" s="126"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="149">
+      <c r="A45" s="114">
         <v>43</v>
       </c>
-      <c r="B45" s="111"/>
+      <c r="B45" s="122"/>
       <c r="C45" s="52" t="s">
         <v>119</v>
       </c>
@@ -3201,13 +3201,13 @@
       <c r="G45" s="75"/>
       <c r="H45" s="56"/>
       <c r="I45" s="56"/>
-      <c r="J45" s="106"/>
+      <c r="J45" s="126"/>
     </row>
     <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="150">
+      <c r="A46" s="115">
         <v>44</v>
       </c>
-      <c r="B46" s="112"/>
+      <c r="B46" s="123"/>
       <c r="C46" s="51" t="s">
         <v>121</v>
       </c>
@@ -3217,13 +3217,13 @@
       <c r="G46" s="73"/>
       <c r="H46" s="55"/>
       <c r="I46" s="55"/>
-      <c r="J46" s="102"/>
+      <c r="J46" s="129"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="148">
+      <c r="A47" s="113">
         <v>45</v>
       </c>
-      <c r="B47" s="110" t="s">
+      <c r="B47" s="121" t="s">
         <v>129</v>
       </c>
       <c r="C47" s="59" t="s">
@@ -3241,22 +3241,22 @@
       <c r="G47" s="72">
         <v>1</v>
       </c>
-      <c r="H47" s="126">
+      <c r="H47" s="93">
         <v>43121</v>
       </c>
-      <c r="I47" s="127">
+      <c r="I47" s="94">
         <v>43121</v>
       </c>
-      <c r="J47" s="117">
+      <c r="J47" s="146">
         <v>0.25</v>
       </c>
-      <c r="K47" s="132"/>
+      <c r="K47" s="98"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="149">
+      <c r="A48" s="114">
         <v>46</v>
       </c>
-      <c r="B48" s="111"/>
+      <c r="B48" s="122"/>
       <c r="C48" s="52" t="s">
         <v>117</v>
       </c>
@@ -3266,13 +3266,13 @@
       <c r="G48" s="75"/>
       <c r="H48" s="56"/>
       <c r="I48" s="56"/>
-      <c r="J48" s="106"/>
+      <c r="J48" s="126"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="149">
+      <c r="A49" s="114">
         <v>47</v>
       </c>
-      <c r="B49" s="111"/>
+      <c r="B49" s="122"/>
       <c r="C49" s="52" t="s">
         <v>119</v>
       </c>
@@ -3282,13 +3282,13 @@
       <c r="G49" s="75"/>
       <c r="H49" s="56"/>
       <c r="I49" s="56"/>
-      <c r="J49" s="106"/>
+      <c r="J49" s="126"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="150">
+      <c r="A50" s="115">
         <v>48</v>
       </c>
-      <c r="B50" s="112"/>
+      <c r="B50" s="123"/>
       <c r="C50" s="51" t="s">
         <v>121</v>
       </c>
@@ -3298,13 +3298,13 @@
       <c r="G50" s="73"/>
       <c r="H50" s="55"/>
       <c r="I50" s="55"/>
-      <c r="J50" s="102"/>
+      <c r="J50" s="129"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="148">
+      <c r="A51" s="113">
         <v>49</v>
       </c>
-      <c r="B51" s="120" t="s">
+      <c r="B51" s="143" t="s">
         <v>46</v>
       </c>
       <c r="C51" s="59" t="s">
@@ -3322,22 +3322,22 @@
       <c r="G51" s="72">
         <v>1</v>
       </c>
-      <c r="H51" s="126">
+      <c r="H51" s="93">
         <v>43121</v>
       </c>
-      <c r="I51" s="127">
+      <c r="I51" s="94">
         <v>43121</v>
       </c>
-      <c r="J51" s="117">
+      <c r="J51" s="146">
         <v>0.25</v>
       </c>
-      <c r="K51" s="132"/>
+      <c r="K51" s="98"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="149">
+      <c r="A52" s="114">
         <v>50</v>
       </c>
-      <c r="B52" s="121"/>
+      <c r="B52" s="144"/>
       <c r="C52" s="52" t="s">
         <v>117</v>
       </c>
@@ -3347,13 +3347,13 @@
       <c r="G52" s="75"/>
       <c r="H52" s="56"/>
       <c r="I52" s="56"/>
-      <c r="J52" s="106"/>
+      <c r="J52" s="126"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="149">
+      <c r="A53" s="114">
         <v>51</v>
       </c>
-      <c r="B53" s="121"/>
+      <c r="B53" s="144"/>
       <c r="C53" s="52" t="s">
         <v>119</v>
       </c>
@@ -3363,13 +3363,13 @@
       <c r="G53" s="75"/>
       <c r="H53" s="56"/>
       <c r="I53" s="56"/>
-      <c r="J53" s="106"/>
+      <c r="J53" s="126"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="150">
+      <c r="A54" s="115">
         <v>52</v>
       </c>
-      <c r="B54" s="122"/>
+      <c r="B54" s="145"/>
       <c r="C54" s="51" t="s">
         <v>121</v>
       </c>
@@ -3379,181 +3379,181 @@
       <c r="G54" s="73"/>
       <c r="H54" s="55"/>
       <c r="I54" s="55"/>
-      <c r="J54" s="102"/>
-    </row>
-    <row r="55" spans="1:11" s="138" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="148">
+      <c r="J54" s="129"/>
+    </row>
+    <row r="55" spans="1:11" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="113">
         <v>53</v>
       </c>
-      <c r="B55" s="120" t="s">
+      <c r="B55" s="143" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="128" t="s">
+      <c r="C55" s="95" t="s">
         <v>118</v>
       </c>
       <c r="D55" s="90">
         <v>1</v>
       </c>
-      <c r="E55" s="136">
+      <c r="E55" s="102">
         <v>43121</v>
       </c>
-      <c r="F55" s="136">
+      <c r="F55" s="102">
         <v>43121</v>
       </c>
-      <c r="G55" s="129">
-        <v>1</v>
-      </c>
-      <c r="H55" s="136">
+      <c r="G55" s="96">
+        <v>1</v>
+      </c>
+      <c r="H55" s="102">
         <v>43121</v>
       </c>
-      <c r="I55" s="136">
+      <c r="I55" s="102">
         <v>43121</v>
       </c>
-      <c r="J55" s="117">
+      <c r="J55" s="146">
         <v>0.25</v>
       </c>
-      <c r="K55" s="132"/>
-    </row>
-    <row r="56" spans="1:11" s="138" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="149">
+      <c r="K55" s="98"/>
+    </row>
+    <row r="56" spans="1:11" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="114">
         <v>54</v>
       </c>
-      <c r="B56" s="121"/>
-      <c r="C56" s="139" t="s">
+      <c r="B56" s="144"/>
+      <c r="C56" s="105" t="s">
         <v>117</v>
       </c>
       <c r="D56" s="91"/>
-      <c r="E56" s="140"/>
-      <c r="F56" s="141"/>
-      <c r="G56" s="142"/>
-      <c r="H56" s="141"/>
-      <c r="I56" s="141"/>
-      <c r="J56" s="106"/>
-      <c r="K56" s="137"/>
-    </row>
-    <row r="57" spans="1:11" s="138" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="149">
+      <c r="E56" s="106"/>
+      <c r="F56" s="107"/>
+      <c r="G56" s="108"/>
+      <c r="H56" s="107"/>
+      <c r="I56" s="107"/>
+      <c r="J56" s="126"/>
+      <c r="K56" s="103"/>
+    </row>
+    <row r="57" spans="1:11" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="114">
         <v>55</v>
       </c>
-      <c r="B57" s="121"/>
-      <c r="C57" s="139" t="s">
+      <c r="B57" s="144"/>
+      <c r="C57" s="105" t="s">
         <v>119</v>
       </c>
       <c r="D57" s="91"/>
-      <c r="E57" s="140"/>
-      <c r="F57" s="141"/>
-      <c r="G57" s="142"/>
-      <c r="H57" s="141"/>
-      <c r="I57" s="141"/>
-      <c r="J57" s="106"/>
-      <c r="K57" s="137"/>
-    </row>
-    <row r="58" spans="1:11" s="138" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="150">
+      <c r="E57" s="106"/>
+      <c r="F57" s="107"/>
+      <c r="G57" s="108"/>
+      <c r="H57" s="107"/>
+      <c r="I57" s="107"/>
+      <c r="J57" s="126"/>
+      <c r="K57" s="103"/>
+    </row>
+    <row r="58" spans="1:11" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="115">
         <v>56</v>
       </c>
-      <c r="B58" s="122"/>
-      <c r="C58" s="143" t="s">
+      <c r="B58" s="145"/>
+      <c r="C58" s="109" t="s">
         <v>121</v>
       </c>
       <c r="D58" s="92"/>
-      <c r="E58" s="144"/>
-      <c r="F58" s="145"/>
-      <c r="G58" s="146"/>
-      <c r="H58" s="145"/>
-      <c r="I58" s="145"/>
-      <c r="J58" s="102"/>
-      <c r="K58" s="137"/>
-    </row>
-    <row r="59" spans="1:11" s="138" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="148">
+      <c r="E58" s="110"/>
+      <c r="F58" s="111"/>
+      <c r="G58" s="112"/>
+      <c r="H58" s="111"/>
+      <c r="I58" s="111"/>
+      <c r="J58" s="129"/>
+      <c r="K58" s="103"/>
+    </row>
+    <row r="59" spans="1:11" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="113">
         <v>57</v>
       </c>
-      <c r="B59" s="120" t="s">
+      <c r="B59" s="143" t="s">
         <v>145</v>
       </c>
-      <c r="C59" s="128" t="s">
+      <c r="C59" s="95" t="s">
         <v>118</v>
       </c>
       <c r="D59" s="90">
         <v>1</v>
       </c>
-      <c r="E59" s="136">
+      <c r="E59" s="102">
         <v>43121</v>
       </c>
-      <c r="F59" s="136">
+      <c r="F59" s="102">
         <v>43121</v>
       </c>
-      <c r="G59" s="129">
-        <v>1</v>
-      </c>
-      <c r="H59" s="136">
+      <c r="G59" s="96">
+        <v>1</v>
+      </c>
+      <c r="H59" s="102">
         <v>43121</v>
       </c>
-      <c r="I59" s="136">
+      <c r="I59" s="102">
         <v>43121</v>
       </c>
-      <c r="J59" s="117">
+      <c r="J59" s="146">
         <v>0.25</v>
       </c>
-      <c r="K59" s="132"/>
-    </row>
-    <row r="60" spans="1:11" s="138" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="149">
+      <c r="K59" s="98"/>
+    </row>
+    <row r="60" spans="1:11" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="114">
         <v>58</v>
       </c>
-      <c r="B60" s="121"/>
-      <c r="C60" s="139" t="s">
+      <c r="B60" s="144"/>
+      <c r="C60" s="105" t="s">
         <v>117</v>
       </c>
       <c r="D60" s="91"/>
-      <c r="E60" s="140"/>
-      <c r="F60" s="141"/>
-      <c r="G60" s="142"/>
-      <c r="H60" s="141"/>
-      <c r="I60" s="141"/>
-      <c r="J60" s="106"/>
-      <c r="K60" s="137"/>
-    </row>
-    <row r="61" spans="1:11" s="138" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="149">
+      <c r="E60" s="106"/>
+      <c r="F60" s="107"/>
+      <c r="G60" s="108"/>
+      <c r="H60" s="107"/>
+      <c r="I60" s="107"/>
+      <c r="J60" s="126"/>
+      <c r="K60" s="103"/>
+    </row>
+    <row r="61" spans="1:11" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="114">
         <v>59</v>
       </c>
-      <c r="B61" s="121"/>
-      <c r="C61" s="139" t="s">
+      <c r="B61" s="144"/>
+      <c r="C61" s="105" t="s">
         <v>119</v>
       </c>
       <c r="D61" s="91"/>
-      <c r="E61" s="140"/>
-      <c r="F61" s="141"/>
-      <c r="G61" s="142"/>
-      <c r="H61" s="141"/>
-      <c r="I61" s="141"/>
-      <c r="J61" s="106"/>
-      <c r="K61" s="137"/>
-    </row>
-    <row r="62" spans="1:11" s="138" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="150">
+      <c r="E61" s="106"/>
+      <c r="F61" s="107"/>
+      <c r="G61" s="108"/>
+      <c r="H61" s="107"/>
+      <c r="I61" s="107"/>
+      <c r="J61" s="126"/>
+      <c r="K61" s="103"/>
+    </row>
+    <row r="62" spans="1:11" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="115">
         <v>60</v>
       </c>
-      <c r="B62" s="122"/>
-      <c r="C62" s="143" t="s">
+      <c r="B62" s="145"/>
+      <c r="C62" s="109" t="s">
         <v>121</v>
       </c>
       <c r="D62" s="92"/>
-      <c r="E62" s="144"/>
-      <c r="F62" s="145"/>
-      <c r="G62" s="146"/>
-      <c r="H62" s="145"/>
-      <c r="I62" s="145"/>
-      <c r="J62" s="102"/>
-      <c r="K62" s="137"/>
+      <c r="E62" s="110"/>
+      <c r="F62" s="111"/>
+      <c r="G62" s="112"/>
+      <c r="H62" s="111"/>
+      <c r="I62" s="111"/>
+      <c r="J62" s="129"/>
+      <c r="K62" s="103"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="148">
+      <c r="A63" s="113">
         <v>61</v>
       </c>
-      <c r="B63" s="120" t="s">
+      <c r="B63" s="143" t="s">
         <v>61</v>
       </c>
       <c r="C63" s="59" t="s">
@@ -3562,31 +3562,31 @@
       <c r="D63" s="44">
         <v>1</v>
       </c>
-      <c r="E63" s="136">
+      <c r="E63" s="102">
         <v>43121</v>
       </c>
-      <c r="F63" s="136">
+      <c r="F63" s="102">
         <v>43121</v>
       </c>
-      <c r="G63" s="129">
-        <v>1</v>
-      </c>
-      <c r="H63" s="136">
+      <c r="G63" s="96">
+        <v>1</v>
+      </c>
+      <c r="H63" s="102">
         <v>43121</v>
       </c>
-      <c r="I63" s="136">
+      <c r="I63" s="102">
         <v>43121</v>
       </c>
-      <c r="J63" s="117">
+      <c r="J63" s="146">
         <v>0.25</v>
       </c>
-      <c r="K63" s="132"/>
+      <c r="K63" s="98"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="149">
+      <c r="A64" s="114">
         <v>62</v>
       </c>
-      <c r="B64" s="121"/>
+      <c r="B64" s="144"/>
       <c r="C64" s="52" t="s">
         <v>117</v>
       </c>
@@ -3596,13 +3596,13 @@
       <c r="G64" s="75"/>
       <c r="H64" s="56"/>
       <c r="I64" s="56"/>
-      <c r="J64" s="106"/>
+      <c r="J64" s="126"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="149">
+      <c r="A65" s="114">
         <v>63</v>
       </c>
-      <c r="B65" s="121"/>
+      <c r="B65" s="144"/>
       <c r="C65" s="52" t="s">
         <v>119</v>
       </c>
@@ -3612,13 +3612,13 @@
       <c r="G65" s="75"/>
       <c r="H65" s="56"/>
       <c r="I65" s="56"/>
-      <c r="J65" s="106"/>
+      <c r="J65" s="126"/>
     </row>
     <row r="66" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="150">
+      <c r="A66" s="115">
         <v>64</v>
       </c>
-      <c r="B66" s="122"/>
+      <c r="B66" s="145"/>
       <c r="C66" s="51" t="s">
         <v>121</v>
       </c>
@@ -3628,13 +3628,13 @@
       <c r="G66" s="73"/>
       <c r="H66" s="55"/>
       <c r="I66" s="55"/>
-      <c r="J66" s="102"/>
+      <c r="J66" s="129"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="148">
+      <c r="A67" s="113">
         <v>65</v>
       </c>
-      <c r="B67" s="120" t="s">
+      <c r="B67" s="143" t="s">
         <v>85</v>
       </c>
       <c r="C67" s="59" t="s">
@@ -3643,31 +3643,31 @@
       <c r="D67" s="44">
         <v>1</v>
       </c>
-      <c r="E67" s="136">
+      <c r="E67" s="102">
         <v>43121</v>
       </c>
-      <c r="F67" s="136">
+      <c r="F67" s="102">
         <v>43121</v>
       </c>
-      <c r="G67" s="129">
-        <v>1</v>
-      </c>
-      <c r="H67" s="136">
+      <c r="G67" s="96">
+        <v>1</v>
+      </c>
+      <c r="H67" s="102">
         <v>43121</v>
       </c>
-      <c r="I67" s="136">
+      <c r="I67" s="102">
         <v>43121</v>
       </c>
-      <c r="J67" s="117">
+      <c r="J67" s="146">
         <v>0.25</v>
       </c>
-      <c r="K67" s="132"/>
+      <c r="K67" s="98"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="149">
+      <c r="A68" s="114">
         <v>66</v>
       </c>
-      <c r="B68" s="121"/>
+      <c r="B68" s="144"/>
       <c r="C68" s="52" t="s">
         <v>117</v>
       </c>
@@ -3677,13 +3677,13 @@
       <c r="G68" s="75"/>
       <c r="H68" s="56"/>
       <c r="I68" s="56"/>
-      <c r="J68" s="106"/>
+      <c r="J68" s="126"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="149">
+      <c r="A69" s="114">
         <v>67</v>
       </c>
-      <c r="B69" s="121"/>
+      <c r="B69" s="144"/>
       <c r="C69" s="52" t="s">
         <v>119</v>
       </c>
@@ -3693,13 +3693,13 @@
       <c r="G69" s="75"/>
       <c r="H69" s="56"/>
       <c r="I69" s="56"/>
-      <c r="J69" s="106"/>
+      <c r="J69" s="126"/>
     </row>
     <row r="70" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="150">
+      <c r="A70" s="115">
         <v>68</v>
       </c>
-      <c r="B70" s="122"/>
+      <c r="B70" s="145"/>
       <c r="C70" s="51" t="s">
         <v>121</v>
       </c>
@@ -3709,13 +3709,13 @@
       <c r="G70" s="73"/>
       <c r="H70" s="55"/>
       <c r="I70" s="55"/>
-      <c r="J70" s="102"/>
+      <c r="J70" s="129"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="148">
+      <c r="A71" s="113">
         <v>69</v>
       </c>
-      <c r="B71" s="110" t="s">
+      <c r="B71" s="121" t="s">
         <v>62</v>
       </c>
       <c r="C71" s="59" t="s">
@@ -3724,31 +3724,31 @@
       <c r="D71" s="44">
         <v>1</v>
       </c>
-      <c r="E71" s="136">
+      <c r="E71" s="102">
         <v>43121</v>
       </c>
-      <c r="F71" s="136">
+      <c r="F71" s="102">
         <v>43121</v>
       </c>
-      <c r="G71" s="129">
-        <v>1</v>
-      </c>
-      <c r="H71" s="136">
+      <c r="G71" s="96">
+        <v>1</v>
+      </c>
+      <c r="H71" s="102">
         <v>43121</v>
       </c>
-      <c r="I71" s="136">
+      <c r="I71" s="102">
         <v>43121</v>
       </c>
-      <c r="J71" s="117">
+      <c r="J71" s="146">
         <v>0.25</v>
       </c>
-      <c r="K71" s="132"/>
+      <c r="K71" s="98"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="149">
+      <c r="A72" s="114">
         <v>70</v>
       </c>
-      <c r="B72" s="111"/>
+      <c r="B72" s="122"/>
       <c r="C72" s="52" t="s">
         <v>117</v>
       </c>
@@ -3758,13 +3758,13 @@
       <c r="G72" s="75"/>
       <c r="H72" s="56"/>
       <c r="I72" s="56"/>
-      <c r="J72" s="106"/>
+      <c r="J72" s="126"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="149">
+      <c r="A73" s="114">
         <v>71</v>
       </c>
-      <c r="B73" s="111"/>
+      <c r="B73" s="122"/>
       <c r="C73" s="52" t="s">
         <v>119</v>
       </c>
@@ -3774,13 +3774,13 @@
       <c r="G73" s="75"/>
       <c r="H73" s="56"/>
       <c r="I73" s="56"/>
-      <c r="J73" s="106"/>
+      <c r="J73" s="126"/>
     </row>
     <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="150">
+      <c r="A74" s="115">
         <v>72</v>
       </c>
-      <c r="B74" s="112"/>
+      <c r="B74" s="123"/>
       <c r="C74" s="51" t="s">
         <v>121</v>
       </c>
@@ -3790,13 +3790,13 @@
       <c r="G74" s="73"/>
       <c r="H74" s="55"/>
       <c r="I74" s="55"/>
-      <c r="J74" s="102"/>
+      <c r="J74" s="129"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="148">
+      <c r="A75" s="113">
         <v>73</v>
       </c>
-      <c r="B75" s="110" t="s">
+      <c r="B75" s="121" t="s">
         <v>66</v>
       </c>
       <c r="C75" s="59" t="s">
@@ -3805,31 +3805,31 @@
       <c r="D75" s="44">
         <v>1</v>
       </c>
-      <c r="E75" s="136">
+      <c r="E75" s="102">
         <v>43121</v>
       </c>
-      <c r="F75" s="136">
+      <c r="F75" s="102">
         <v>43121</v>
       </c>
-      <c r="G75" s="129">
-        <v>1</v>
-      </c>
-      <c r="H75" s="136">
+      <c r="G75" s="96">
+        <v>1</v>
+      </c>
+      <c r="H75" s="102">
         <v>43121</v>
       </c>
-      <c r="I75" s="136">
+      <c r="I75" s="102">
         <v>43121</v>
       </c>
-      <c r="J75" s="117">
+      <c r="J75" s="146">
         <v>0.25</v>
       </c>
-      <c r="K75" s="132"/>
+      <c r="K75" s="98"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="149">
+      <c r="A76" s="114">
         <v>74</v>
       </c>
-      <c r="B76" s="111"/>
+      <c r="B76" s="122"/>
       <c r="C76" s="52" t="s">
         <v>117</v>
       </c>
@@ -3839,13 +3839,13 @@
       <c r="G76" s="75"/>
       <c r="H76" s="56"/>
       <c r="I76" s="56"/>
-      <c r="J76" s="106"/>
+      <c r="J76" s="126"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="149">
+      <c r="A77" s="114">
         <v>75</v>
       </c>
-      <c r="B77" s="111"/>
+      <c r="B77" s="122"/>
       <c r="C77" s="52" t="s">
         <v>119</v>
       </c>
@@ -3855,13 +3855,13 @@
       <c r="G77" s="75"/>
       <c r="H77" s="56"/>
       <c r="I77" s="56"/>
-      <c r="J77" s="106"/>
+      <c r="J77" s="126"/>
     </row>
     <row r="78" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="150">
+      <c r="A78" s="115">
         <v>76</v>
       </c>
-      <c r="B78" s="112"/>
+      <c r="B78" s="123"/>
       <c r="C78" s="51" t="s">
         <v>121</v>
       </c>
@@ -3871,13 +3871,13 @@
       <c r="G78" s="73"/>
       <c r="H78" s="55"/>
       <c r="I78" s="55"/>
-      <c r="J78" s="102"/>
+      <c r="J78" s="129"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="148">
+      <c r="A79" s="113">
         <v>77</v>
       </c>
-      <c r="B79" s="110" t="s">
+      <c r="B79" s="121" t="s">
         <v>67</v>
       </c>
       <c r="C79" s="59" t="s">
@@ -3886,31 +3886,31 @@
       <c r="D79" s="44">
         <v>1</v>
       </c>
-      <c r="E79" s="136">
+      <c r="E79" s="102">
         <v>43121</v>
       </c>
-      <c r="F79" s="136">
+      <c r="F79" s="102">
         <v>43121</v>
       </c>
-      <c r="G79" s="129">
-        <v>1</v>
-      </c>
-      <c r="H79" s="136">
+      <c r="G79" s="96">
+        <v>1</v>
+      </c>
+      <c r="H79" s="102">
         <v>43121</v>
       </c>
-      <c r="I79" s="136">
+      <c r="I79" s="102">
         <v>43121</v>
       </c>
-      <c r="J79" s="117">
+      <c r="J79" s="146">
         <v>0.25</v>
       </c>
-      <c r="K79" s="132"/>
+      <c r="K79" s="98"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="149">
+      <c r="A80" s="114">
         <v>78</v>
       </c>
-      <c r="B80" s="111"/>
+      <c r="B80" s="122"/>
       <c r="C80" s="52" t="s">
         <v>117</v>
       </c>
@@ -3920,13 +3920,13 @@
       <c r="G80" s="75"/>
       <c r="H80" s="56"/>
       <c r="I80" s="56"/>
-      <c r="J80" s="106"/>
+      <c r="J80" s="126"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="149">
+      <c r="A81" s="114">
         <v>79</v>
       </c>
-      <c r="B81" s="111"/>
+      <c r="B81" s="122"/>
       <c r="C81" s="52" t="s">
         <v>119</v>
       </c>
@@ -3936,13 +3936,13 @@
       <c r="G81" s="75"/>
       <c r="H81" s="56"/>
       <c r="I81" s="56"/>
-      <c r="J81" s="106"/>
+      <c r="J81" s="126"/>
     </row>
     <row r="82" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="150">
+      <c r="A82" s="115">
         <v>80</v>
       </c>
-      <c r="B82" s="112"/>
+      <c r="B82" s="123"/>
       <c r="C82" s="51" t="s">
         <v>121</v>
       </c>
@@ -3952,181 +3952,181 @@
       <c r="G82" s="73"/>
       <c r="H82" s="55"/>
       <c r="I82" s="55"/>
-      <c r="J82" s="102"/>
+      <c r="J82" s="129"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="148">
+      <c r="A83" s="113">
         <v>81</v>
       </c>
-      <c r="B83" s="120" t="s">
+      <c r="B83" s="143" t="s">
         <v>68</v>
       </c>
-      <c r="C83" s="128" t="s">
+      <c r="C83" s="95" t="s">
         <v>118</v>
       </c>
       <c r="D83" s="90">
         <v>1</v>
       </c>
-      <c r="E83" s="136">
+      <c r="E83" s="102">
         <v>43121</v>
       </c>
-      <c r="F83" s="136">
+      <c r="F83" s="102">
         <v>43121</v>
       </c>
-      <c r="G83" s="129">
-        <v>1</v>
-      </c>
-      <c r="H83" s="136">
+      <c r="G83" s="96">
+        <v>1</v>
+      </c>
+      <c r="H83" s="102">
         <v>43121</v>
       </c>
-      <c r="I83" s="136">
+      <c r="I83" s="102">
         <v>43121</v>
       </c>
-      <c r="J83" s="117">
+      <c r="J83" s="146">
         <v>0.25</v>
       </c>
-      <c r="K83" s="132"/>
+      <c r="K83" s="98"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="149">
+      <c r="A84" s="114">
         <v>82</v>
       </c>
-      <c r="B84" s="121"/>
-      <c r="C84" s="139" t="s">
+      <c r="B84" s="144"/>
+      <c r="C84" s="105" t="s">
         <v>117</v>
       </c>
       <c r="D84" s="91"/>
-      <c r="E84" s="141"/>
-      <c r="F84" s="141"/>
-      <c r="G84" s="142"/>
-      <c r="H84" s="141"/>
-      <c r="I84" s="141"/>
-      <c r="J84" s="106"/>
-      <c r="K84" s="137"/>
+      <c r="E84" s="107"/>
+      <c r="F84" s="107"/>
+      <c r="G84" s="108"/>
+      <c r="H84" s="107"/>
+      <c r="I84" s="107"/>
+      <c r="J84" s="126"/>
+      <c r="K84" s="103"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="149">
+      <c r="A85" s="114">
         <v>83</v>
       </c>
-      <c r="B85" s="121"/>
-      <c r="C85" s="139" t="s">
+      <c r="B85" s="144"/>
+      <c r="C85" s="105" t="s">
         <v>119</v>
       </c>
       <c r="D85" s="91"/>
-      <c r="E85" s="141"/>
-      <c r="F85" s="141"/>
-      <c r="G85" s="142"/>
-      <c r="H85" s="141"/>
-      <c r="I85" s="141"/>
-      <c r="J85" s="106"/>
-      <c r="K85" s="137"/>
+      <c r="E85" s="107"/>
+      <c r="F85" s="107"/>
+      <c r="G85" s="108"/>
+      <c r="H85" s="107"/>
+      <c r="I85" s="107"/>
+      <c r="J85" s="126"/>
+      <c r="K85" s="103"/>
     </row>
     <row r="86" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="150">
+      <c r="A86" s="115">
         <v>84</v>
       </c>
-      <c r="B86" s="122"/>
-      <c r="C86" s="143" t="s">
+      <c r="B86" s="145"/>
+      <c r="C86" s="109" t="s">
         <v>121</v>
       </c>
       <c r="D86" s="92"/>
-      <c r="E86" s="145"/>
-      <c r="F86" s="145"/>
-      <c r="G86" s="146"/>
-      <c r="H86" s="145"/>
-      <c r="I86" s="145"/>
-      <c r="J86" s="102"/>
-      <c r="K86" s="137"/>
+      <c r="E86" s="111"/>
+      <c r="F86" s="111"/>
+      <c r="G86" s="112"/>
+      <c r="H86" s="111"/>
+      <c r="I86" s="111"/>
+      <c r="J86" s="129"/>
+      <c r="K86" s="103"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="148">
+      <c r="A87" s="113">
         <v>85</v>
       </c>
-      <c r="B87" s="120" t="s">
+      <c r="B87" s="143" t="s">
         <v>69</v>
       </c>
-      <c r="C87" s="128" t="s">
+      <c r="C87" s="95" t="s">
         <v>118</v>
       </c>
       <c r="D87" s="90">
         <v>1</v>
       </c>
-      <c r="E87" s="151">
+      <c r="E87" s="116">
         <v>43121</v>
       </c>
-      <c r="F87" s="151">
+      <c r="F87" s="116">
         <v>43121</v>
       </c>
-      <c r="G87" s="152">
-        <v>1</v>
-      </c>
-      <c r="H87" s="151">
+      <c r="G87" s="117">
+        <v>1</v>
+      </c>
+      <c r="H87" s="116">
         <v>43121</v>
       </c>
-      <c r="I87" s="151">
+      <c r="I87" s="116">
         <v>43121</v>
       </c>
-      <c r="J87" s="117">
+      <c r="J87" s="146">
         <v>0.25</v>
       </c>
-      <c r="K87" s="132"/>
+      <c r="K87" s="98"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="149">
+      <c r="A88" s="114">
         <v>86</v>
       </c>
-      <c r="B88" s="121"/>
-      <c r="C88" s="139" t="s">
+      <c r="B88" s="144"/>
+      <c r="C88" s="105" t="s">
         <v>117</v>
       </c>
       <c r="D88" s="91"/>
-      <c r="E88" s="141"/>
-      <c r="F88" s="141"/>
-      <c r="G88" s="142"/>
-      <c r="H88" s="141"/>
-      <c r="I88" s="141"/>
-      <c r="J88" s="106"/>
-      <c r="K88" s="137"/>
+      <c r="E88" s="107"/>
+      <c r="F88" s="107"/>
+      <c r="G88" s="108"/>
+      <c r="H88" s="107"/>
+      <c r="I88" s="107"/>
+      <c r="J88" s="126"/>
+      <c r="K88" s="103"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A89" s="149">
+      <c r="A89" s="114">
         <v>87</v>
       </c>
-      <c r="B89" s="121"/>
-      <c r="C89" s="139" t="s">
+      <c r="B89" s="144"/>
+      <c r="C89" s="105" t="s">
         <v>119</v>
       </c>
       <c r="D89" s="91"/>
-      <c r="E89" s="141"/>
-      <c r="F89" s="141"/>
-      <c r="G89" s="142"/>
-      <c r="H89" s="141"/>
-      <c r="I89" s="141"/>
-      <c r="J89" s="106"/>
-      <c r="K89" s="137"/>
+      <c r="E89" s="107"/>
+      <c r="F89" s="107"/>
+      <c r="G89" s="108"/>
+      <c r="H89" s="107"/>
+      <c r="I89" s="107"/>
+      <c r="J89" s="126"/>
+      <c r="K89" s="103"/>
     </row>
     <row r="90" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="150">
+      <c r="A90" s="115">
         <v>88</v>
       </c>
-      <c r="B90" s="122"/>
-      <c r="C90" s="143" t="s">
+      <c r="B90" s="145"/>
+      <c r="C90" s="109" t="s">
         <v>121</v>
       </c>
       <c r="D90" s="92"/>
-      <c r="E90" s="145"/>
-      <c r="F90" s="145"/>
-      <c r="G90" s="146"/>
-      <c r="H90" s="145"/>
-      <c r="I90" s="145"/>
-      <c r="J90" s="102"/>
-      <c r="K90" s="137"/>
+      <c r="E90" s="111"/>
+      <c r="F90" s="111"/>
+      <c r="G90" s="112"/>
+      <c r="H90" s="111"/>
+      <c r="I90" s="111"/>
+      <c r="J90" s="129"/>
+      <c r="K90" s="103"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A91" s="148">
+      <c r="A91" s="113">
         <v>89</v>
       </c>
-      <c r="B91" s="110" t="s">
+      <c r="B91" s="121" t="s">
         <v>56</v>
       </c>
       <c r="C91" s="59" t="s">
@@ -4150,13 +4150,13 @@
       <c r="I91" s="65">
         <v>43125</v>
       </c>
-      <c r="J91" s="106"/>
+      <c r="J91" s="126"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" s="149">
+      <c r="A92" s="114">
         <v>90</v>
       </c>
-      <c r="B92" s="111"/>
+      <c r="B92" s="122"/>
       <c r="C92" s="52" t="s">
         <v>117</v>
       </c>
@@ -4165,13 +4165,13 @@
       <c r="F92" s="56"/>
       <c r="G92" s="75"/>
       <c r="H92" s="56"/>
-      <c r="J92" s="106"/>
+      <c r="J92" s="126"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="149">
+      <c r="A93" s="114">
         <v>91</v>
       </c>
-      <c r="B93" s="111"/>
+      <c r="B93" s="122"/>
       <c r="C93" s="52" t="s">
         <v>119</v>
       </c>
@@ -4180,13 +4180,13 @@
       <c r="F93" s="56"/>
       <c r="G93" s="75"/>
       <c r="H93" s="56"/>
-      <c r="J93" s="106"/>
+      <c r="J93" s="126"/>
     </row>
     <row r="94" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="150">
+      <c r="A94" s="115">
         <v>92</v>
       </c>
-      <c r="B94" s="112"/>
+      <c r="B94" s="123"/>
       <c r="C94" s="51" t="s">
         <v>121</v>
       </c>
@@ -4196,13 +4196,13 @@
       <c r="G94" s="73"/>
       <c r="H94" s="55"/>
       <c r="I94" s="55"/>
-      <c r="J94" s="102"/>
+      <c r="J94" s="129"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A95" s="148">
+      <c r="A95" s="113">
         <v>93</v>
       </c>
-      <c r="B95" s="110" t="s">
+      <c r="B95" s="121" t="s">
         <v>82</v>
       </c>
       <c r="C95" s="59" t="s">
@@ -4226,13 +4226,13 @@
       <c r="I95" s="65">
         <v>43125</v>
       </c>
-      <c r="J95" s="106"/>
+      <c r="J95" s="126"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A96" s="149">
+      <c r="A96" s="114">
         <v>94</v>
       </c>
-      <c r="B96" s="111"/>
+      <c r="B96" s="122"/>
       <c r="C96" s="52" t="s">
         <v>117</v>
       </c>
@@ -4242,13 +4242,13 @@
       <c r="G96" s="75"/>
       <c r="H96" s="56"/>
       <c r="I96" s="56"/>
-      <c r="J96" s="106"/>
+      <c r="J96" s="126"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" s="149">
+      <c r="A97" s="114">
         <v>95</v>
       </c>
-      <c r="B97" s="111"/>
+      <c r="B97" s="122"/>
       <c r="C97" s="52" t="s">
         <v>119</v>
       </c>
@@ -4258,13 +4258,13 @@
       <c r="G97" s="75"/>
       <c r="H97" s="56"/>
       <c r="I97" s="56"/>
-      <c r="J97" s="106"/>
+      <c r="J97" s="126"/>
     </row>
     <row r="98" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="150">
+      <c r="A98" s="115">
         <v>96</v>
       </c>
-      <c r="B98" s="112"/>
+      <c r="B98" s="123"/>
       <c r="C98" s="51" t="s">
         <v>121</v>
       </c>
@@ -4274,13 +4274,13 @@
       <c r="G98" s="73"/>
       <c r="H98" s="55"/>
       <c r="I98" s="55"/>
-      <c r="J98" s="102"/>
+      <c r="J98" s="129"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" s="148">
+      <c r="A99" s="113">
         <v>97</v>
       </c>
-      <c r="B99" s="110" t="s">
+      <c r="B99" s="121" t="s">
         <v>83</v>
       </c>
       <c r="C99" s="59" t="s">
@@ -4304,13 +4304,13 @@
       <c r="I99" s="65">
         <v>43125</v>
       </c>
-      <c r="J99" s="106"/>
+      <c r="J99" s="126"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="149">
+      <c r="A100" s="114">
         <v>98</v>
       </c>
-      <c r="B100" s="111"/>
+      <c r="B100" s="122"/>
       <c r="C100" s="52" t="s">
         <v>117</v>
       </c>
@@ -4320,13 +4320,13 @@
       <c r="G100" s="75"/>
       <c r="H100" s="56"/>
       <c r="I100" s="56"/>
-      <c r="J100" s="106"/>
+      <c r="J100" s="126"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="149">
+      <c r="A101" s="114">
         <v>99</v>
       </c>
-      <c r="B101" s="111"/>
+      <c r="B101" s="122"/>
       <c r="C101" s="52" t="s">
         <v>119</v>
       </c>
@@ -4336,13 +4336,13 @@
       <c r="G101" s="75"/>
       <c r="H101" s="56"/>
       <c r="I101" s="56"/>
-      <c r="J101" s="106"/>
+      <c r="J101" s="126"/>
     </row>
     <row r="102" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="150">
+      <c r="A102" s="115">
         <v>100</v>
       </c>
-      <c r="B102" s="112"/>
+      <c r="B102" s="123"/>
       <c r="C102" s="51" t="s">
         <v>121</v>
       </c>
@@ -4352,13 +4352,13 @@
       <c r="G102" s="73"/>
       <c r="H102" s="55"/>
       <c r="I102" s="55"/>
-      <c r="J102" s="102"/>
+      <c r="J102" s="129"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="148">
+      <c r="A103" s="113">
         <v>101</v>
       </c>
-      <c r="B103" s="120" t="s">
+      <c r="B103" s="143" t="s">
         <v>101</v>
       </c>
       <c r="C103" s="59" t="s">
@@ -4382,13 +4382,13 @@
       <c r="I103" s="65">
         <v>43126</v>
       </c>
-      <c r="J103" s="106"/>
+      <c r="J103" s="126"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="149">
+      <c r="A104" s="114">
         <v>102</v>
       </c>
-      <c r="B104" s="121"/>
+      <c r="B104" s="144"/>
       <c r="C104" s="52" t="s">
         <v>117</v>
       </c>
@@ -4397,13 +4397,13 @@
       <c r="F104" s="56"/>
       <c r="G104" s="75"/>
       <c r="H104" s="56"/>
-      <c r="J104" s="106"/>
+      <c r="J104" s="126"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" s="149">
+      <c r="A105" s="114">
         <v>103</v>
       </c>
-      <c r="B105" s="121"/>
+      <c r="B105" s="144"/>
       <c r="C105" s="52" t="s">
         <v>119</v>
       </c>
@@ -4412,13 +4412,13 @@
       <c r="F105" s="56"/>
       <c r="G105" s="75"/>
       <c r="H105" s="56"/>
-      <c r="J105" s="106"/>
+      <c r="J105" s="126"/>
     </row>
     <row r="106" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="150">
+      <c r="A106" s="115">
         <v>104</v>
       </c>
-      <c r="B106" s="122"/>
+      <c r="B106" s="145"/>
       <c r="C106" s="51" t="s">
         <v>121</v>
       </c>
@@ -4428,13 +4428,13 @@
       <c r="G106" s="73"/>
       <c r="H106" s="55"/>
       <c r="I106" s="55"/>
-      <c r="J106" s="102"/>
+      <c r="J106" s="129"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="148">
+      <c r="A107" s="113">
         <v>105</v>
       </c>
-      <c r="B107" s="120" t="s">
+      <c r="B107" s="143" t="s">
         <v>109</v>
       </c>
       <c r="C107" s="52" t="s">
@@ -4458,33 +4458,33 @@
       <c r="I107" s="65">
         <v>43126</v>
       </c>
-      <c r="J107" s="100"/>
+      <c r="J107" s="125"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" s="149">
+      <c r="A108" s="114">
         <v>106</v>
       </c>
-      <c r="B108" s="121"/>
+      <c r="B108" s="144"/>
       <c r="C108" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="J108" s="106"/>
+      <c r="J108" s="126"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="149">
+      <c r="A109" s="114">
         <v>107</v>
       </c>
-      <c r="B109" s="121"/>
+      <c r="B109" s="144"/>
       <c r="C109" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="J109" s="106"/>
+      <c r="J109" s="126"/>
     </row>
     <row r="110" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="150">
+      <c r="A110" s="115">
         <v>108</v>
       </c>
-      <c r="B110" s="122"/>
+      <c r="B110" s="145"/>
       <c r="C110" s="51" t="s">
         <v>121</v>
       </c>
@@ -4494,13 +4494,13 @@
       <c r="G110" s="73"/>
       <c r="H110" s="55"/>
       <c r="I110" s="55"/>
-      <c r="J110" s="102"/>
+      <c r="J110" s="129"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="148">
+      <c r="A111" s="113">
         <v>109</v>
       </c>
-      <c r="B111" s="120" t="s">
+      <c r="B111" s="143" t="s">
         <v>102</v>
       </c>
       <c r="C111" s="52" t="s">
@@ -4524,33 +4524,33 @@
       <c r="I111" s="65">
         <v>43126</v>
       </c>
-      <c r="J111" s="106"/>
+      <c r="J111" s="126"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="149">
+      <c r="A112" s="114">
         <v>110</v>
       </c>
-      <c r="B112" s="121"/>
+      <c r="B112" s="144"/>
       <c r="C112" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="J112" s="106"/>
+      <c r="J112" s="126"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" s="149">
+      <c r="A113" s="114">
         <v>111</v>
       </c>
-      <c r="B113" s="121"/>
+      <c r="B113" s="144"/>
       <c r="C113" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="J113" s="106"/>
+      <c r="J113" s="126"/>
     </row>
     <row r="114" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="150">
+      <c r="A114" s="115">
         <v>112</v>
       </c>
-      <c r="B114" s="122"/>
+      <c r="B114" s="145"/>
       <c r="C114" s="51" t="s">
         <v>121</v>
       </c>
@@ -4560,13 +4560,13 @@
       <c r="G114" s="73"/>
       <c r="H114" s="55"/>
       <c r="I114" s="55"/>
-      <c r="J114" s="102"/>
+      <c r="J114" s="129"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="148">
+      <c r="A115" s="113">
         <v>113</v>
       </c>
-      <c r="B115" s="120" t="s">
+      <c r="B115" s="143" t="s">
         <v>104</v>
       </c>
       <c r="C115" s="52" t="s">
@@ -4590,33 +4590,33 @@
       <c r="I115" s="65">
         <v>43127</v>
       </c>
-      <c r="J115" s="106"/>
+      <c r="J115" s="126"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="149">
+      <c r="A116" s="114">
         <v>114</v>
       </c>
-      <c r="B116" s="121"/>
+      <c r="B116" s="144"/>
       <c r="C116" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="J116" s="106"/>
+      <c r="J116" s="126"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="149">
+      <c r="A117" s="114">
         <v>115</v>
       </c>
-      <c r="B117" s="121"/>
+      <c r="B117" s="144"/>
       <c r="C117" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="J117" s="106"/>
+      <c r="J117" s="126"/>
     </row>
     <row r="118" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="150">
+      <c r="A118" s="115">
         <v>116</v>
       </c>
-      <c r="B118" s="122"/>
+      <c r="B118" s="145"/>
       <c r="C118" s="51" t="s">
         <v>121</v>
       </c>
@@ -4626,13 +4626,13 @@
       <c r="G118" s="73"/>
       <c r="H118" s="55"/>
       <c r="I118" s="55"/>
-      <c r="J118" s="102"/>
+      <c r="J118" s="129"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" s="148">
+      <c r="A119" s="113">
         <v>117</v>
       </c>
-      <c r="B119" s="110" t="s">
+      <c r="B119" s="121" t="s">
         <v>103</v>
       </c>
       <c r="C119" s="59" t="s">
@@ -4656,13 +4656,13 @@
       <c r="I119" s="65">
         <v>43127</v>
       </c>
-      <c r="J119" s="106"/>
+      <c r="J119" s="126"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="149">
+      <c r="A120" s="114">
         <v>118</v>
       </c>
-      <c r="B120" s="111"/>
+      <c r="B120" s="122"/>
       <c r="C120" s="52" t="s">
         <v>117</v>
       </c>
@@ -4672,13 +4672,13 @@
       <c r="G120" s="75"/>
       <c r="H120" s="56"/>
       <c r="I120" s="56"/>
-      <c r="J120" s="106"/>
+      <c r="J120" s="126"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121" s="149">
+      <c r="A121" s="114">
         <v>119</v>
       </c>
-      <c r="B121" s="111"/>
+      <c r="B121" s="122"/>
       <c r="C121" s="52" t="s">
         <v>119</v>
       </c>
@@ -4688,13 +4688,13 @@
       <c r="G121" s="75"/>
       <c r="H121" s="56"/>
       <c r="I121" s="56"/>
-      <c r="J121" s="106"/>
+      <c r="J121" s="126"/>
     </row>
     <row r="122" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="150">
+      <c r="A122" s="115">
         <v>120</v>
       </c>
-      <c r="B122" s="112"/>
+      <c r="B122" s="123"/>
       <c r="C122" s="51" t="s">
         <v>121</v>
       </c>
@@ -4704,13 +4704,13 @@
       <c r="G122" s="73"/>
       <c r="H122" s="55"/>
       <c r="I122" s="55"/>
-      <c r="J122" s="102"/>
+      <c r="J122" s="129"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" s="148">
+      <c r="A123" s="113">
         <v>121</v>
       </c>
-      <c r="B123" s="110" t="s">
+      <c r="B123" s="121" t="s">
         <v>105</v>
       </c>
       <c r="C123" s="52" t="s">
@@ -4734,33 +4734,33 @@
       <c r="I123" s="65">
         <v>43127</v>
       </c>
-      <c r="J123" s="106"/>
+      <c r="J123" s="126"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A124" s="149">
+      <c r="A124" s="114">
         <v>122</v>
       </c>
-      <c r="B124" s="111"/>
+      <c r="B124" s="122"/>
       <c r="C124" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="J124" s="106"/>
+      <c r="J124" s="126"/>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A125" s="149">
+      <c r="A125" s="114">
         <v>123</v>
       </c>
-      <c r="B125" s="111"/>
+      <c r="B125" s="122"/>
       <c r="C125" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="J125" s="106"/>
+      <c r="J125" s="126"/>
     </row>
     <row r="126" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="150">
+      <c r="A126" s="115">
         <v>124</v>
       </c>
-      <c r="B126" s="112"/>
+      <c r="B126" s="123"/>
       <c r="C126" s="51" t="s">
         <v>121</v>
       </c>
@@ -4770,13 +4770,13 @@
       <c r="G126" s="73"/>
       <c r="H126" s="55"/>
       <c r="I126" s="55"/>
-      <c r="J126" s="102"/>
+      <c r="J126" s="129"/>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A127" s="148">
+      <c r="A127" s="113">
         <v>125</v>
       </c>
-      <c r="B127" s="110" t="s">
+      <c r="B127" s="121" t="s">
         <v>108</v>
       </c>
       <c r="C127" s="52" t="s">
@@ -4800,33 +4800,33 @@
       <c r="I127" s="65">
         <v>43129</v>
       </c>
-      <c r="J127" s="106"/>
+      <c r="J127" s="126"/>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A128" s="149">
+      <c r="A128" s="114">
         <v>126</v>
       </c>
-      <c r="B128" s="111"/>
+      <c r="B128" s="122"/>
       <c r="C128" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="J128" s="106"/>
+      <c r="J128" s="126"/>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A129" s="149">
+      <c r="A129" s="114">
         <v>127</v>
       </c>
-      <c r="B129" s="111"/>
+      <c r="B129" s="122"/>
       <c r="C129" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="J129" s="106"/>
+      <c r="J129" s="126"/>
     </row>
     <row r="130" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="150">
+      <c r="A130" s="115">
         <v>128</v>
       </c>
-      <c r="B130" s="112"/>
+      <c r="B130" s="123"/>
       <c r="C130" s="51" t="s">
         <v>121</v>
       </c>
@@ -4836,13 +4836,13 @@
       <c r="G130" s="73"/>
       <c r="H130" s="55"/>
       <c r="I130" s="55"/>
-      <c r="J130" s="102"/>
+      <c r="J130" s="129"/>
     </row>
     <row r="131" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="148">
+      <c r="A131" s="113">
         <v>129</v>
       </c>
-      <c r="B131" s="110" t="s">
+      <c r="B131" s="121" t="s">
         <v>27</v>
       </c>
       <c r="C131" s="59" t="s">
@@ -4854,14 +4854,14 @@
       <c r="G131" s="57"/>
       <c r="H131" s="70"/>
       <c r="I131" s="70"/>
-      <c r="J131" s="106"/>
-      <c r="K131" s="133"/>
+      <c r="J131" s="126"/>
+      <c r="K131" s="99"/>
     </row>
     <row r="132" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="149">
+      <c r="A132" s="114">
         <v>130</v>
       </c>
-      <c r="B132" s="111"/>
+      <c r="B132" s="122"/>
       <c r="C132" s="52" t="s">
         <v>119</v>
       </c>
@@ -4871,14 +4871,14 @@
       <c r="G132" s="57"/>
       <c r="H132" s="71"/>
       <c r="I132" s="56"/>
-      <c r="J132" s="106"/>
-      <c r="K132" s="133"/>
+      <c r="J132" s="126"/>
+      <c r="K132" s="99"/>
     </row>
     <row r="133" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="149">
+      <c r="A133" s="114">
         <v>131</v>
       </c>
-      <c r="B133" s="111"/>
+      <c r="B133" s="122"/>
       <c r="C133" s="52" t="s">
         <v>117</v>
       </c>
@@ -4888,14 +4888,14 @@
       <c r="G133" s="57"/>
       <c r="H133" s="71"/>
       <c r="I133" s="56"/>
-      <c r="J133" s="106"/>
-      <c r="K133" s="133"/>
+      <c r="J133" s="126"/>
+      <c r="K133" s="99"/>
     </row>
     <row r="134" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="150">
+      <c r="A134" s="115">
         <v>132</v>
       </c>
-      <c r="B134" s="112"/>
+      <c r="B134" s="123"/>
       <c r="C134" s="51" t="s">
         <v>118</v>
       </c>
@@ -4905,13 +4905,13 @@
       <c r="G134" s="73"/>
       <c r="H134" s="69"/>
       <c r="I134" s="55"/>
-      <c r="J134" s="102"/>
+      <c r="J134" s="129"/>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A135" s="148">
+      <c r="A135" s="113">
         <v>133</v>
       </c>
-      <c r="B135" s="120" t="s">
+      <c r="B135" s="143" t="s">
         <v>54</v>
       </c>
       <c r="C135" s="59" t="s">
@@ -4923,16 +4923,16 @@
       <c r="G135" s="74"/>
       <c r="H135" s="65"/>
       <c r="I135" s="65"/>
-      <c r="J135" s="106"/>
+      <c r="J135" s="126"/>
       <c r="L135" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A136" s="149">
+      <c r="A136" s="114">
         <v>134</v>
       </c>
-      <c r="B136" s="121"/>
+      <c r="B136" s="144"/>
       <c r="C136" s="52" t="s">
         <v>117</v>
       </c>
@@ -4942,13 +4942,13 @@
       <c r="G136" s="75"/>
       <c r="H136" s="56"/>
       <c r="I136" s="56"/>
-      <c r="J136" s="106"/>
+      <c r="J136" s="126"/>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A137" s="149">
+      <c r="A137" s="114">
         <v>135</v>
       </c>
-      <c r="B137" s="121"/>
+      <c r="B137" s="144"/>
       <c r="C137" s="52" t="s">
         <v>119</v>
       </c>
@@ -4958,13 +4958,13 @@
       <c r="G137" s="75"/>
       <c r="H137" s="56"/>
       <c r="I137" s="56"/>
-      <c r="J137" s="106"/>
+      <c r="J137" s="126"/>
     </row>
     <row r="138" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="150">
+      <c r="A138" s="115">
         <v>136</v>
       </c>
-      <c r="B138" s="122"/>
+      <c r="B138" s="145"/>
       <c r="C138" s="51" t="s">
         <v>121</v>
       </c>
@@ -4974,13 +4974,13 @@
       <c r="G138" s="73"/>
       <c r="H138" s="55"/>
       <c r="I138" s="55"/>
-      <c r="J138" s="102"/>
+      <c r="J138" s="129"/>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A139" s="148">
+      <c r="A139" s="113">
         <v>137</v>
       </c>
-      <c r="B139" s="110" t="s">
+      <c r="B139" s="121" t="s">
         <v>55</v>
       </c>
       <c r="C139" s="59" t="s">
@@ -4992,16 +4992,16 @@
       <c r="G139" s="74"/>
       <c r="H139" s="65"/>
       <c r="I139" s="65"/>
-      <c r="J139" s="106"/>
+      <c r="J139" s="126"/>
       <c r="L139" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A140" s="149">
+      <c r="A140" s="114">
         <v>138</v>
       </c>
-      <c r="B140" s="111"/>
+      <c r="B140" s="122"/>
       <c r="C140" s="52" t="s">
         <v>117</v>
       </c>
@@ -5011,13 +5011,13 @@
       <c r="G140" s="75"/>
       <c r="H140" s="56"/>
       <c r="I140" s="56"/>
-      <c r="J140" s="106"/>
+      <c r="J140" s="126"/>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A141" s="149">
+      <c r="A141" s="114">
         <v>139</v>
       </c>
-      <c r="B141" s="111"/>
+      <c r="B141" s="122"/>
       <c r="C141" s="52" t="s">
         <v>119</v>
       </c>
@@ -5027,13 +5027,13 @@
       <c r="G141" s="75"/>
       <c r="H141" s="56"/>
       <c r="I141" s="56"/>
-      <c r="J141" s="106"/>
+      <c r="J141" s="126"/>
     </row>
     <row r="142" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="150">
+      <c r="A142" s="115">
         <v>140</v>
       </c>
-      <c r="B142" s="112"/>
+      <c r="B142" s="123"/>
       <c r="C142" s="51" t="s">
         <v>121</v>
       </c>
@@ -5043,13 +5043,13 @@
       <c r="G142" s="73"/>
       <c r="H142" s="55"/>
       <c r="I142" s="55"/>
-      <c r="J142" s="102"/>
+      <c r="J142" s="129"/>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A143" s="148">
+      <c r="A143" s="113">
         <v>141</v>
       </c>
-      <c r="B143" s="123" t="s">
+      <c r="B143" s="149" t="s">
         <v>84</v>
       </c>
       <c r="C143" s="59" t="s">
@@ -5061,13 +5061,13 @@
       <c r="G143" s="74"/>
       <c r="H143" s="65"/>
       <c r="I143" s="65"/>
-      <c r="J143" s="106"/>
+      <c r="J143" s="126"/>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A144" s="149">
+      <c r="A144" s="114">
         <v>142</v>
       </c>
-      <c r="B144" s="124"/>
+      <c r="B144" s="150"/>
       <c r="C144" s="52" t="s">
         <v>117</v>
       </c>
@@ -5077,13 +5077,13 @@
       <c r="G144" s="75"/>
       <c r="H144" s="56"/>
       <c r="I144" s="56"/>
-      <c r="J144" s="106"/>
+      <c r="J144" s="126"/>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A145" s="149">
+      <c r="A145" s="114">
         <v>143</v>
       </c>
-      <c r="B145" s="118" t="s">
+      <c r="B145" s="151" t="s">
         <v>134</v>
       </c>
       <c r="C145" s="52" t="s">
@@ -5095,13 +5095,13 @@
       <c r="G145" s="75"/>
       <c r="H145" s="56"/>
       <c r="I145" s="56"/>
-      <c r="J145" s="106"/>
+      <c r="J145" s="126"/>
     </row>
     <row r="146" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="150">
+      <c r="A146" s="115">
         <v>144</v>
       </c>
-      <c r="B146" s="119"/>
+      <c r="B146" s="152"/>
       <c r="C146" s="51" t="s">
         <v>121</v>
       </c>
@@ -5111,13 +5111,13 @@
       <c r="G146" s="73"/>
       <c r="H146" s="55"/>
       <c r="I146" s="55"/>
-      <c r="J146" s="102"/>
+      <c r="J146" s="129"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A147" s="148">
+      <c r="A147" s="113">
         <v>145</v>
       </c>
-      <c r="B147" s="123" t="s">
+      <c r="B147" s="149" t="s">
         <v>43</v>
       </c>
       <c r="C147" s="59" t="s">
@@ -5129,16 +5129,16 @@
       <c r="G147" s="74"/>
       <c r="H147" s="65"/>
       <c r="I147" s="65"/>
-      <c r="J147" s="106"/>
+      <c r="J147" s="126"/>
       <c r="L147" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A148" s="149">
+      <c r="A148" s="114">
         <v>146</v>
       </c>
-      <c r="B148" s="124"/>
+      <c r="B148" s="150"/>
       <c r="C148" s="52" t="s">
         <v>117</v>
       </c>
@@ -5148,13 +5148,13 @@
       <c r="G148" s="75"/>
       <c r="H148" s="56"/>
       <c r="I148" s="56"/>
-      <c r="J148" s="106"/>
+      <c r="J148" s="126"/>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A149" s="149">
+      <c r="A149" s="114">
         <v>147</v>
       </c>
-      <c r="B149" s="118" t="s">
+      <c r="B149" s="151" t="s">
         <v>134</v>
       </c>
       <c r="C149" s="52" t="s">
@@ -5166,13 +5166,13 @@
       <c r="G149" s="75"/>
       <c r="H149" s="56"/>
       <c r="I149" s="56"/>
-      <c r="J149" s="106"/>
+      <c r="J149" s="126"/>
     </row>
     <row r="150" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="150">
+      <c r="A150" s="115">
         <v>148</v>
       </c>
-      <c r="B150" s="119"/>
+      <c r="B150" s="152"/>
       <c r="C150" s="51" t="s">
         <v>121</v>
       </c>
@@ -5182,13 +5182,13 @@
       <c r="G150" s="73"/>
       <c r="H150" s="55"/>
       <c r="I150" s="55"/>
-      <c r="J150" s="102"/>
+      <c r="J150" s="129"/>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A151" s="148">
+      <c r="A151" s="113">
         <v>149</v>
       </c>
-      <c r="B151" s="110" t="s">
+      <c r="B151" s="121" t="s">
         <v>15</v>
       </c>
       <c r="C151" s="59" t="s">
@@ -5210,13 +5210,13 @@
       <c r="I151" s="65">
         <v>43125</v>
       </c>
-      <c r="J151" s="106"/>
+      <c r="J151" s="126"/>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A152" s="149">
+      <c r="A152" s="114">
         <v>150</v>
       </c>
-      <c r="B152" s="111"/>
+      <c r="B152" s="122"/>
       <c r="C152" s="52" t="s">
         <v>117</v>
       </c>
@@ -5226,13 +5226,13 @@
       <c r="G152" s="75"/>
       <c r="H152" s="56"/>
       <c r="I152" s="56"/>
-      <c r="J152" s="106"/>
+      <c r="J152" s="126"/>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A153" s="149">
+      <c r="A153" s="114">
         <v>151</v>
       </c>
-      <c r="B153" s="111"/>
+      <c r="B153" s="122"/>
       <c r="C153" s="52" t="s">
         <v>119</v>
       </c>
@@ -5242,13 +5242,13 @@
       <c r="G153" s="75"/>
       <c r="H153" s="56"/>
       <c r="I153" s="56"/>
-      <c r="J153" s="106"/>
+      <c r="J153" s="126"/>
     </row>
     <row r="154" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="150">
+      <c r="A154" s="115">
         <v>152</v>
       </c>
-      <c r="B154" s="112"/>
+      <c r="B154" s="123"/>
       <c r="C154" s="51" t="s">
         <v>121</v>
       </c>
@@ -5258,10 +5258,78 @@
       <c r="G154" s="73"/>
       <c r="H154" s="55"/>
       <c r="I154" s="55"/>
-      <c r="J154" s="102"/>
+      <c r="J154" s="129"/>
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="J19:J22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="J15:J18"/>
+    <mergeCell ref="J151:J154"/>
+    <mergeCell ref="J91:J94"/>
+    <mergeCell ref="J95:J98"/>
+    <mergeCell ref="J99:J102"/>
+    <mergeCell ref="B135:B138"/>
+    <mergeCell ref="B139:B142"/>
+    <mergeCell ref="B103:B106"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="B123:B126"/>
+    <mergeCell ref="B127:B130"/>
+    <mergeCell ref="B107:B110"/>
+    <mergeCell ref="J143:J146"/>
+    <mergeCell ref="J131:J134"/>
+    <mergeCell ref="J147:J150"/>
+    <mergeCell ref="J135:J138"/>
+    <mergeCell ref="J139:J142"/>
+    <mergeCell ref="J87:J90"/>
+    <mergeCell ref="J123:J126"/>
+    <mergeCell ref="J127:J130"/>
+    <mergeCell ref="J107:J110"/>
+    <mergeCell ref="B147:B148"/>
+    <mergeCell ref="J103:J106"/>
+    <mergeCell ref="J119:J122"/>
+    <mergeCell ref="J111:J114"/>
+    <mergeCell ref="J115:J118"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="B119:B122"/>
+    <mergeCell ref="B111:B114"/>
+    <mergeCell ref="B115:B118"/>
+    <mergeCell ref="J47:J50"/>
+    <mergeCell ref="J51:J54"/>
+    <mergeCell ref="J55:J58"/>
+    <mergeCell ref="J63:J66"/>
+    <mergeCell ref="B83:B86"/>
+    <mergeCell ref="J67:J70"/>
+    <mergeCell ref="J71:J74"/>
+    <mergeCell ref="J75:J78"/>
+    <mergeCell ref="J79:J82"/>
+    <mergeCell ref="J83:J86"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="B79:B82"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="J27:J30"/>
+    <mergeCell ref="J31:J34"/>
+    <mergeCell ref="J35:J38"/>
+    <mergeCell ref="J39:J42"/>
+    <mergeCell ref="J43:J46"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="B151:B154"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="B99:B102"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B131:B134"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B35:B38"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="B59:B62"/>
     <mergeCell ref="J59:J62"/>
@@ -5278,74 +5346,6 @@
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="B51:B54"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B91:B94"/>
-    <mergeCell ref="B151:B154"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="B87:B90"/>
-    <mergeCell ref="B99:B102"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="B131:B134"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="J27:J30"/>
-    <mergeCell ref="J31:J34"/>
-    <mergeCell ref="J35:J38"/>
-    <mergeCell ref="J39:J42"/>
-    <mergeCell ref="J43:J46"/>
-    <mergeCell ref="J47:J50"/>
-    <mergeCell ref="J51:J54"/>
-    <mergeCell ref="J55:J58"/>
-    <mergeCell ref="J63:J66"/>
-    <mergeCell ref="B83:B86"/>
-    <mergeCell ref="J67:J70"/>
-    <mergeCell ref="J71:J74"/>
-    <mergeCell ref="J75:J78"/>
-    <mergeCell ref="J79:J82"/>
-    <mergeCell ref="J83:J86"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="B79:B82"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="J87:J90"/>
-    <mergeCell ref="J123:J126"/>
-    <mergeCell ref="J127:J130"/>
-    <mergeCell ref="J107:J110"/>
-    <mergeCell ref="B147:B148"/>
-    <mergeCell ref="J103:J106"/>
-    <mergeCell ref="J119:J122"/>
-    <mergeCell ref="J111:J114"/>
-    <mergeCell ref="J115:J118"/>
-    <mergeCell ref="J151:J154"/>
-    <mergeCell ref="J91:J94"/>
-    <mergeCell ref="J95:J98"/>
-    <mergeCell ref="J99:J102"/>
-    <mergeCell ref="B135:B138"/>
-    <mergeCell ref="B139:B142"/>
-    <mergeCell ref="B103:B106"/>
-    <mergeCell ref="B149:B150"/>
-    <mergeCell ref="B123:B126"/>
-    <mergeCell ref="B127:B130"/>
-    <mergeCell ref="B107:B110"/>
-    <mergeCell ref="J143:J146"/>
-    <mergeCell ref="J131:J134"/>
-    <mergeCell ref="J147:J150"/>
-    <mergeCell ref="J135:J138"/>
-    <mergeCell ref="J139:J142"/>
-    <mergeCell ref="B143:B144"/>
-    <mergeCell ref="B145:B146"/>
-    <mergeCell ref="B119:B122"/>
-    <mergeCell ref="B111:B114"/>
-    <mergeCell ref="B115:B118"/>
-    <mergeCell ref="J19:J22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="J23:J26"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="J15:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5368,26 +5368,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="127" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="125" t="s">
+      <c r="D1" s="148" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="125"/>
+      <c r="E1" s="148"/>
       <c r="F1" s="47" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="114"/>
-      <c r="B2" s="114"/>
+      <c r="A2" s="128"/>
+      <c r="B2" s="128"/>
       <c r="C2" s="46" t="s">
         <v>122</v>
       </c>
@@ -5402,7 +5402,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="125" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -5419,7 +5419,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="106"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
@@ -5428,7 +5428,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="106"/>
+      <c r="A5" s="126"/>
       <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
@@ -5437,7 +5437,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="106"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
@@ -5446,7 +5446,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="106"/>
+      <c r="A7" s="126"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
@@ -5455,7 +5455,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="106"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="8" t="s">
         <v>115</v>
       </c>
@@ -5467,7 +5467,7 @@
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="125" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -5475,13 +5475,13 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="106"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="102"/>
+      <c r="A11" s="129"/>
       <c r="B11" s="12" t="s">
         <v>20</v>
       </c>
@@ -5511,7 +5511,7 @@
       <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="125" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="42" t="s">
@@ -5519,13 +5519,13 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="106"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="42" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="102"/>
+      <c r="A16" s="129"/>
       <c r="B16" s="43" t="s">
         <v>32</v>
       </c>
@@ -5535,7 +5535,7 @@
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="100" t="s">
+      <c r="A17" s="125" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -5543,25 +5543,25 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="101"/>
+      <c r="A18" s="138"/>
       <c r="B18" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="101"/>
+      <c r="A19" s="138"/>
       <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="101"/>
+      <c r="A20" s="138"/>
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="102"/>
+      <c r="A21" s="129"/>
       <c r="B21" s="19" t="s">
         <v>40</v>
       </c>
@@ -5607,7 +5607,7 @@
       <c r="F24" s="15"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="93" t="s">
+      <c r="A25" s="134" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -5615,13 +5615,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="94"/>
+      <c r="A26" s="135"/>
       <c r="B26" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="95"/>
+      <c r="A27" s="136"/>
       <c r="B27" s="19" t="s">
         <v>53</v>
       </c>
@@ -5643,7 +5643,7 @@
       <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="93" t="s">
+      <c r="A29" s="134" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -5651,33 +5651,33 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="109"/>
+      <c r="A30" s="137"/>
       <c r="B30" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="109"/>
-      <c r="B31" s="107" t="s">
+      <c r="A31" s="137"/>
+      <c r="B31" s="132" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="109"/>
-      <c r="B32" s="107"/>
+      <c r="A32" s="137"/>
+      <c r="B32" s="132"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="109"/>
-      <c r="B33" s="107" t="s">
+      <c r="A33" s="137"/>
+      <c r="B33" s="132" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="109"/>
-      <c r="B34" s="107"/>
+      <c r="A34" s="137"/>
+      <c r="B34" s="132"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="95"/>
+      <c r="A35" s="136"/>
       <c r="B35" s="9" t="s">
         <v>59</v>
       </c>
@@ -5699,7 +5699,7 @@
       <c r="F36" s="15"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="93" t="s">
+      <c r="A37" s="134" t="s">
         <v>76</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -5707,19 +5707,19 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="94"/>
+      <c r="A38" s="135"/>
       <c r="B38" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="94"/>
+      <c r="A39" s="135"/>
       <c r="B39" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="94"/>
+      <c r="A40" s="135"/>
       <c r="B40" s="3" t="s">
         <v>80</v>
       </c>
@@ -5741,7 +5741,7 @@
       <c r="F41" s="15"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="93" t="s">
+      <c r="A42" s="134" t="s">
         <v>92</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -5749,7 +5749,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="95"/>
+      <c r="A43" s="136"/>
       <c r="B43" s="8" t="s">
         <v>87</v>
       </c>
@@ -5759,7 +5759,7 @@
       <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="93" t="s">
+      <c r="A44" s="134" t="s">
         <v>93</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -5767,25 +5767,25 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="94"/>
+      <c r="A45" s="135"/>
       <c r="B45" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="94"/>
+      <c r="A46" s="135"/>
       <c r="B46" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="94"/>
+      <c r="A47" s="135"/>
       <c r="B47" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="95"/>
+      <c r="A48" s="136"/>
       <c r="B48" s="9" t="s">
         <v>86</v>
       </c>
@@ -5795,7 +5795,7 @@
       <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="93" t="s">
+      <c r="A49" s="134" t="s">
         <v>97</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -5803,13 +5803,13 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="94"/>
+      <c r="A50" s="135"/>
       <c r="B50" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="95"/>
+      <c r="A51" s="136"/>
       <c r="B51" s="8" t="s">
         <v>98</v>
       </c>
@@ -5844,11 +5844,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A42:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="A1:A2"/>
@@ -5859,6 +5854,11 @@
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A42:A43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[DataAccess] Adding and Testing GetGame(Id) task 113
</commit_message>
<xml_diff>
--- a/schedules/Time Estimations.xlsx
+++ b/schedules/Time Estimations.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="149">
   <si>
     <t>Página</t>
   </si>
@@ -471,6 +471,9 @@
   </si>
   <si>
     <t>This depends upon the definition of Prizing Sructures</t>
+  </si>
+  <si>
+    <t>getTeam(Id)</t>
   </si>
 </sst>
 </file>
@@ -521,7 +524,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -604,11 +607,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -862,6 +896,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1029,6 +1090,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1332,37 +1435,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="127" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="127" t="s">
+      <c r="B1" s="136" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="136" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="127" t="s">
+      <c r="D1" s="136" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="127"/>
-      <c r="F1" s="130" t="s">
+      <c r="E1" s="136"/>
+      <c r="F1" s="139" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="128"/>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
+      <c r="A2" s="137"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
       <c r="D2" s="29" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="131"/>
+      <c r="F2" s="140"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="125" t="s">
+      <c r="A3" s="134" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1382,7 +1485,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="126"/>
+      <c r="A4" s="135"/>
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1398,7 +1501,7 @@
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="126"/>
+      <c r="A5" s="135"/>
       <c r="B5" s="6" t="s">
         <v>139</v>
       </c>
@@ -1414,7 +1517,7 @@
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="126"/>
+      <c r="A6" s="135"/>
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
@@ -1430,7 +1533,7 @@
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="126"/>
+      <c r="A7" s="135"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
@@ -1446,7 +1549,7 @@
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="126"/>
+      <c r="A8" s="135"/>
       <c r="B8" s="8" t="s">
         <v>115</v>
       </c>
@@ -1460,7 +1563,7 @@
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="125" t="s">
+      <c r="A9" s="134" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -1469,7 +1572,7 @@
       <c r="C9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="119" t="s">
+      <c r="D9" s="128" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="33">
@@ -1480,27 +1583,27 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="126"/>
+      <c r="A10" s="135"/>
       <c r="B10" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="124"/>
+      <c r="D10" s="133"/>
       <c r="E10" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="129"/>
+      <c r="A11" s="138"/>
       <c r="B11" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="120"/>
+      <c r="D11" s="129"/>
       <c r="E11" s="32" t="s">
         <v>24</v>
       </c>
@@ -1543,47 +1646,47 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="125" t="s">
+      <c r="A14" s="134" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="139" t="s">
+      <c r="C14" s="148" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="118" t="s">
+      <c r="D14" s="127" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="118">
+      <c r="E14" s="127">
         <v>0.5</v>
       </c>
-      <c r="F14" s="121" t="s">
+      <c r="F14" s="130" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="126"/>
+      <c r="A15" s="135"/>
       <c r="B15" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="140"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="119"/>
-      <c r="F15" s="122"/>
+      <c r="C15" s="149"/>
+      <c r="D15" s="128"/>
+      <c r="E15" s="128"/>
+      <c r="F15" s="131"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="129"/>
+      <c r="A16" s="138"/>
       <c r="B16" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="141"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="123"/>
+      <c r="C16" s="150"/>
+      <c r="D16" s="129"/>
+      <c r="E16" s="129"/>
+      <c r="F16" s="132"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="125" t="s">
+      <c r="A17" s="134" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1592,7 +1695,7 @@
       <c r="C17" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="118" t="s">
+      <c r="D17" s="127" t="s">
         <v>34</v>
       </c>
       <c r="E17" s="33">
@@ -1603,53 +1706,53 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="138"/>
+      <c r="A18" s="147"/>
       <c r="B18" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="119"/>
+      <c r="D18" s="128"/>
       <c r="E18" s="33" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="138"/>
+      <c r="A19" s="147"/>
       <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C19" t="s">
         <v>128</v>
       </c>
-      <c r="D19" s="119"/>
+      <c r="D19" s="128"/>
       <c r="E19" s="33">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="138"/>
+      <c r="A20" s="147"/>
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C20" t="s">
         <v>129</v>
       </c>
-      <c r="D20" s="119"/>
+      <c r="D20" s="128"/>
       <c r="E20" s="33">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="129"/>
+      <c r="A21" s="138"/>
       <c r="B21" s="19" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="120"/>
+      <c r="D21" s="129"/>
       <c r="E21" s="32" t="s">
         <v>24</v>
       </c>
@@ -1712,7 +1815,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="134" t="s">
+      <c r="A25" s="143" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1721,7 +1824,7 @@
       <c r="C25" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="118" t="s">
+      <c r="D25" s="127" t="s">
         <v>34</v>
       </c>
       <c r="E25" s="33">
@@ -1732,27 +1835,27 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="135"/>
+      <c r="A26" s="144"/>
       <c r="B26" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="124"/>
+      <c r="D26" s="133"/>
       <c r="E26" s="33">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="136"/>
+      <c r="A27" s="145"/>
       <c r="B27" s="19" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="120"/>
+      <c r="D27" s="129"/>
       <c r="E27" s="32">
         <v>2</v>
       </c>
@@ -1779,7 +1882,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="134" t="s">
+      <c r="A29" s="143" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1796,7 +1899,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="137"/>
+      <c r="A30" s="146"/>
       <c r="B30" s="3" t="s">
         <v>63</v>
       </c>
@@ -1811,14 +1914,14 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="137"/>
-      <c r="B31" s="132" t="s">
+      <c r="A31" s="146"/>
+      <c r="B31" s="141" t="s">
         <v>64</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="124">
+      <c r="D31" s="133">
         <v>3</v>
       </c>
       <c r="E31" s="33">
@@ -1829,25 +1932,25 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="137"/>
-      <c r="B32" s="132"/>
+      <c r="A32" s="146"/>
+      <c r="B32" s="141"/>
       <c r="C32" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="124"/>
+      <c r="D32" s="133"/>
       <c r="E32" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="137"/>
-      <c r="B33" s="132" t="s">
+      <c r="A33" s="146"/>
+      <c r="B33" s="141" t="s">
         <v>65</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="124">
+      <c r="D33" s="133">
         <v>3</v>
       </c>
       <c r="E33" s="33">
@@ -1858,12 +1961,12 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="137"/>
-      <c r="B34" s="132"/>
+      <c r="A34" s="146"/>
+      <c r="B34" s="141"/>
       <c r="C34" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="124"/>
+      <c r="D34" s="133"/>
       <c r="E34" s="33">
         <v>1</v>
       </c>
@@ -1872,7 +1975,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="136"/>
+      <c r="A35" s="145"/>
       <c r="B35" s="9" t="s">
         <v>59</v>
       </c>
@@ -1910,7 +2013,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="134" t="s">
+      <c r="A37" s="143" t="s">
         <v>76</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1930,7 +2033,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="135"/>
+      <c r="A38" s="144"/>
       <c r="B38" s="3" t="s">
         <v>78</v>
       </c>
@@ -1945,7 +2048,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="135"/>
+      <c r="A39" s="144"/>
       <c r="B39" s="3" t="s">
         <v>79</v>
       </c>
@@ -1960,8 +2063,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="135"/>
-      <c r="B40" s="132" t="s">
+      <c r="A40" s="144"/>
+      <c r="B40" s="141" t="s">
         <v>80</v>
       </c>
       <c r="C40" t="s">
@@ -1975,8 +2078,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="136"/>
-      <c r="B41" s="133"/>
+      <c r="A41" s="145"/>
+      <c r="B41" s="142"/>
       <c r="C41" s="9" t="s">
         <v>84</v>
       </c>
@@ -2007,7 +2110,7 @@
       <c r="F42" s="15"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="134" t="s">
+      <c r="A43" s="143" t="s">
         <v>92</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2016,7 +2119,7 @@
       <c r="C43" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="118" t="s">
+      <c r="D43" s="127" t="s">
         <v>34</v>
       </c>
       <c r="E43" s="33">
@@ -2027,14 +2130,14 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="136"/>
+      <c r="A44" s="145"/>
       <c r="B44" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="120"/>
+      <c r="D44" s="129"/>
       <c r="E44" s="32" t="s">
         <v>24</v>
       </c>
@@ -2043,7 +2146,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="134" t="s">
+      <c r="A45" s="143" t="s">
         <v>93</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -2052,7 +2155,7 @@
       <c r="C45" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D45" s="118" t="s">
+      <c r="D45" s="127" t="s">
         <v>34</v>
       </c>
       <c r="E45" s="33">
@@ -2060,56 +2163,56 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="135"/>
+      <c r="A46" s="144"/>
       <c r="B46" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="124"/>
-      <c r="E46" s="124" t="s">
+      <c r="D46" s="133"/>
+      <c r="E46" s="133" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="135"/>
+      <c r="A47" s="144"/>
       <c r="B47" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D47" s="124"/>
-      <c r="E47" s="124"/>
+      <c r="D47" s="133"/>
+      <c r="E47" s="133"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="135"/>
+      <c r="A48" s="144"/>
       <c r="B48" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="124"/>
-      <c r="E48" s="124"/>
+      <c r="D48" s="133"/>
+      <c r="E48" s="133"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="136"/>
+      <c r="A49" s="145"/>
       <c r="B49" s="9" t="s">
         <v>86</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D49" s="120"/>
+      <c r="D49" s="129"/>
       <c r="E49" s="32">
         <v>3</v>
       </c>
       <c r="F49" s="9"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="134" t="s">
+      <c r="A50" s="143" t="s">
         <v>97</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -2118,7 +2221,7 @@
       <c r="C50" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D50" s="118" t="s">
+      <c r="D50" s="127" t="s">
         <v>34</v>
       </c>
       <c r="E50" s="33">
@@ -2126,27 +2229,27 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="135"/>
+      <c r="A51" s="144"/>
       <c r="B51" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D51" s="124"/>
+      <c r="D51" s="133"/>
       <c r="E51" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="136"/>
+      <c r="A52" s="145"/>
       <c r="B52" s="8" t="s">
         <v>98</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D52" s="120"/>
+      <c r="D52" s="129"/>
       <c r="E52" s="32">
         <v>2</v>
       </c>
@@ -2268,8 +2371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F153" sqref="F153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2281,45 +2384,45 @@
     <col min="5" max="6" width="11.42578125" style="50"/>
     <col min="7" max="7" width="13.42578125" style="72" customWidth="1"/>
     <col min="8" max="9" width="11.42578125" style="50"/>
-    <col min="11" max="11" width="21.28515625" style="99" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" style="108" customWidth="1"/>
     <col min="12" max="12" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="156" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="122" t="s">
+      <c r="B1" s="131" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="122" t="s">
+      <c r="C1" s="131" t="s">
         <v>120</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="148" t="s">
+      <c r="E1" s="157" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="148"/>
+      <c r="F1" s="157"/>
       <c r="G1" s="72" t="s">
         <v>124</v>
       </c>
-      <c r="H1" s="148" t="s">
+      <c r="H1" s="157" t="s">
         <v>125</v>
       </c>
-      <c r="I1" s="148"/>
+      <c r="I1" s="157"/>
       <c r="J1" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="K1" s="142" t="s">
+      <c r="K1" s="151" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="147"/>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
+      <c r="A2" s="156"/>
+      <c r="B2" s="132"/>
+      <c r="C2" s="132"/>
       <c r="D2" s="46" t="s">
         <v>122</v>
       </c>
@@ -2341,13 +2444,13 @@
       <c r="J2" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="K2" s="142"/>
+      <c r="K2" s="151"/>
     </row>
     <row r="3" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="113">
-        <v>1</v>
-      </c>
-      <c r="B3" s="121" t="s">
+      <c r="A3" s="122">
+        <v>1</v>
+      </c>
+      <c r="B3" s="130" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="59" t="s">
@@ -2359,16 +2462,16 @@
       <c r="G3" s="74"/>
       <c r="H3" s="60"/>
       <c r="I3" s="60"/>
-      <c r="J3" s="146">
-        <v>1</v>
-      </c>
-      <c r="K3" s="97"/>
+      <c r="J3" s="155">
+        <v>1</v>
+      </c>
+      <c r="K3" s="106"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="114">
+      <c r="A4" s="123">
         <v>2</v>
       </c>
-      <c r="B4" s="122"/>
+      <c r="B4" s="131"/>
       <c r="C4" s="52" t="s">
         <v>117</v>
       </c>
@@ -2378,14 +2481,14 @@
       <c r="G4" s="75"/>
       <c r="H4" s="56"/>
       <c r="I4" s="56"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="98"/>
+      <c r="J4" s="135"/>
+      <c r="K4" s="107"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="114">
+      <c r="A5" s="123">
         <v>3</v>
       </c>
-      <c r="B5" s="122"/>
+      <c r="B5" s="131"/>
       <c r="C5" s="52" t="s">
         <v>119</v>
       </c>
@@ -2395,14 +2498,14 @@
       <c r="G5" s="75"/>
       <c r="H5" s="56"/>
       <c r="I5" s="56"/>
-      <c r="J5" s="126"/>
-      <c r="K5" s="98"/>
+      <c r="J5" s="135"/>
+      <c r="K5" s="107"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="115">
+      <c r="A6" s="124">
         <v>4</v>
       </c>
-      <c r="B6" s="123"/>
+      <c r="B6" s="132"/>
       <c r="C6" s="51" t="s">
         <v>121</v>
       </c>
@@ -2412,14 +2515,14 @@
       <c r="G6" s="73"/>
       <c r="H6" s="55"/>
       <c r="I6" s="55"/>
-      <c r="J6" s="129"/>
-      <c r="K6" s="98"/>
+      <c r="J6" s="138"/>
+      <c r="K6" s="107"/>
     </row>
     <row r="7" spans="1:11" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="113">
+      <c r="A7" s="122">
         <v>5</v>
       </c>
-      <c r="B7" s="121" t="s">
+      <c r="B7" s="130" t="s">
         <v>141</v>
       </c>
       <c r="C7" s="86" t="s">
@@ -2443,16 +2546,16 @@
       <c r="I7" s="61">
         <v>43121</v>
       </c>
-      <c r="J7" s="146">
+      <c r="J7" s="155">
         <v>0.25</v>
       </c>
-      <c r="K7" s="97"/>
+      <c r="K7" s="106"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="114">
+      <c r="A8" s="123">
         <v>6</v>
       </c>
-      <c r="B8" s="122"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="87" t="s">
         <v>117</v>
       </c>
@@ -2462,13 +2565,13 @@
       <c r="G8" s="75"/>
       <c r="H8" s="56"/>
       <c r="I8" s="56"/>
-      <c r="J8" s="126"/>
+      <c r="J8" s="135"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="114">
+      <c r="A9" s="123">
         <v>7</v>
       </c>
-      <c r="B9" s="122"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="87" t="s">
         <v>119</v>
       </c>
@@ -2478,13 +2581,13 @@
       <c r="G9" s="75"/>
       <c r="H9" s="56"/>
       <c r="I9" s="56"/>
-      <c r="J9" s="126"/>
+      <c r="J9" s="135"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="115">
+      <c r="A10" s="124">
         <v>8</v>
       </c>
-      <c r="B10" s="123"/>
+      <c r="B10" s="132"/>
       <c r="C10" s="51" t="s">
         <v>121</v>
       </c>
@@ -2494,13 +2597,13 @@
       <c r="G10" s="73"/>
       <c r="H10" s="55"/>
       <c r="I10" s="55"/>
-      <c r="J10" s="129"/>
+      <c r="J10" s="138"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="113">
+      <c r="A11" s="122">
         <v>9</v>
       </c>
-      <c r="B11" s="121" t="s">
+      <c r="B11" s="130" t="s">
         <v>137</v>
       </c>
       <c r="C11" s="59" t="s">
@@ -2524,16 +2627,16 @@
       <c r="I11" s="65">
         <v>43118</v>
       </c>
-      <c r="J11" s="146">
+      <c r="J11" s="155">
         <v>0.25</v>
       </c>
-      <c r="K11" s="98"/>
+      <c r="K11" s="107"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="114">
+      <c r="A12" s="123">
         <v>10</v>
       </c>
-      <c r="B12" s="122"/>
+      <c r="B12" s="131"/>
       <c r="C12" s="52" t="s">
         <v>117</v>
       </c>
@@ -2542,13 +2645,13 @@
       <c r="F12" s="58"/>
       <c r="H12" s="71"/>
       <c r="I12" s="58"/>
-      <c r="J12" s="126"/>
+      <c r="J12" s="135"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="114">
+      <c r="A13" s="123">
         <v>11</v>
       </c>
-      <c r="B13" s="122"/>
+      <c r="B13" s="131"/>
       <c r="C13" s="52" t="s">
         <v>119</v>
       </c>
@@ -2557,13 +2660,13 @@
       <c r="F13" s="58"/>
       <c r="H13" s="71"/>
       <c r="I13" s="62"/>
-      <c r="J13" s="126"/>
+      <c r="J13" s="135"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="115">
+      <c r="A14" s="124">
         <v>12</v>
       </c>
-      <c r="B14" s="123"/>
+      <c r="B14" s="132"/>
       <c r="C14" s="51" t="s">
         <v>121</v>
       </c>
@@ -2573,13 +2676,13 @@
       <c r="G14" s="73"/>
       <c r="H14" s="69"/>
       <c r="I14" s="63"/>
-      <c r="J14" s="129"/>
+      <c r="J14" s="138"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="113">
+      <c r="A15" s="122">
         <v>13</v>
       </c>
-      <c r="B15" s="121" t="s">
+      <c r="B15" s="130" t="s">
         <v>138</v>
       </c>
       <c r="C15" s="80" t="s">
@@ -2603,16 +2706,16 @@
       <c r="I15" s="65">
         <v>43118</v>
       </c>
-      <c r="J15" s="146">
+      <c r="J15" s="155">
         <v>0.25</v>
       </c>
-      <c r="K15" s="98"/>
+      <c r="K15" s="107"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="114">
+      <c r="A16" s="123">
         <v>14</v>
       </c>
-      <c r="B16" s="122"/>
+      <c r="B16" s="131"/>
       <c r="C16" s="81" t="s">
         <v>117</v>
       </c>
@@ -2621,13 +2724,13 @@
       <c r="F16" s="58"/>
       <c r="H16" s="71"/>
       <c r="I16" s="58"/>
-      <c r="J16" s="126"/>
+      <c r="J16" s="135"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="114">
+      <c r="A17" s="123">
         <v>15</v>
       </c>
-      <c r="B17" s="122"/>
+      <c r="B17" s="131"/>
       <c r="C17" s="81" t="s">
         <v>119</v>
       </c>
@@ -2636,13 +2739,13 @@
       <c r="F17" s="58"/>
       <c r="H17" s="71"/>
       <c r="I17" s="62"/>
-      <c r="J17" s="126"/>
+      <c r="J17" s="135"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="115">
+      <c r="A18" s="124">
         <v>16</v>
       </c>
-      <c r="B18" s="123"/>
+      <c r="B18" s="132"/>
       <c r="C18" s="51" t="s">
         <v>121</v>
       </c>
@@ -2652,13 +2755,13 @@
       <c r="G18" s="73"/>
       <c r="H18" s="69"/>
       <c r="I18" s="63"/>
-      <c r="J18" s="129"/>
+      <c r="J18" s="138"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="113">
+      <c r="A19" s="122">
         <v>17</v>
       </c>
-      <c r="B19" s="121" t="s">
+      <c r="B19" s="130" t="s">
         <v>135</v>
       </c>
       <c r="C19" s="80" t="s">
@@ -2682,16 +2785,16 @@
       <c r="I19" s="65">
         <v>43118</v>
       </c>
-      <c r="J19" s="146">
+      <c r="J19" s="155">
         <v>0.25</v>
       </c>
-      <c r="K19" s="98"/>
+      <c r="K19" s="107"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="114">
+      <c r="A20" s="123">
         <v>18</v>
       </c>
-      <c r="B20" s="122"/>
+      <c r="B20" s="131"/>
       <c r="C20" s="81" t="s">
         <v>117</v>
       </c>
@@ -2700,13 +2803,13 @@
       <c r="F20" s="58"/>
       <c r="H20" s="71"/>
       <c r="I20" s="58"/>
-      <c r="J20" s="126"/>
+      <c r="J20" s="135"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="114">
+      <c r="A21" s="123">
         <v>19</v>
       </c>
-      <c r="B21" s="122"/>
+      <c r="B21" s="131"/>
       <c r="C21" s="81" t="s">
         <v>119</v>
       </c>
@@ -2715,13 +2818,13 @@
       <c r="F21" s="58"/>
       <c r="H21" s="71"/>
       <c r="I21" s="62"/>
-      <c r="J21" s="126"/>
+      <c r="J21" s="135"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="115">
+      <c r="A22" s="124">
         <v>20</v>
       </c>
-      <c r="B22" s="123"/>
+      <c r="B22" s="132"/>
       <c r="C22" s="51" t="s">
         <v>121</v>
       </c>
@@ -2731,13 +2834,13 @@
       <c r="G22" s="73"/>
       <c r="H22" s="69"/>
       <c r="I22" s="63"/>
-      <c r="J22" s="129"/>
+      <c r="J22" s="138"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="113">
+      <c r="A23" s="122">
         <v>21</v>
       </c>
-      <c r="B23" s="121" t="s">
+      <c r="B23" s="130" t="s">
         <v>136</v>
       </c>
       <c r="C23" s="80" t="s">
@@ -2761,16 +2864,16 @@
       <c r="I23" s="65">
         <v>43118</v>
       </c>
-      <c r="J23" s="146">
+      <c r="J23" s="155">
         <v>0.25</v>
       </c>
-      <c r="K23" s="98"/>
+      <c r="K23" s="107"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="114">
+      <c r="A24" s="123">
         <v>22</v>
       </c>
-      <c r="B24" s="122"/>
+      <c r="B24" s="131"/>
       <c r="C24" s="81" t="s">
         <v>117</v>
       </c>
@@ -2779,13 +2882,13 @@
       <c r="F24" s="58"/>
       <c r="H24" s="71"/>
       <c r="I24" s="58"/>
-      <c r="J24" s="126"/>
+      <c r="J24" s="135"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="114">
+      <c r="A25" s="123">
         <v>23</v>
       </c>
-      <c r="B25" s="122"/>
+      <c r="B25" s="131"/>
       <c r="C25" s="81" t="s">
         <v>119</v>
       </c>
@@ -2794,13 +2897,13 @@
       <c r="F25" s="58"/>
       <c r="H25" s="71"/>
       <c r="I25" s="62"/>
-      <c r="J25" s="126"/>
+      <c r="J25" s="135"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="115">
+      <c r="A26" s="124">
         <v>24</v>
       </c>
-      <c r="B26" s="123"/>
+      <c r="B26" s="132"/>
       <c r="C26" s="51" t="s">
         <v>121</v>
       </c>
@@ -2810,13 +2913,13 @@
       <c r="G26" s="73"/>
       <c r="H26" s="69"/>
       <c r="I26" s="63"/>
-      <c r="J26" s="129"/>
+      <c r="J26" s="138"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="113">
+      <c r="A27" s="122">
         <v>25</v>
       </c>
-      <c r="B27" s="121" t="s">
+      <c r="B27" s="130" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="59" t="s">
@@ -2840,16 +2943,16 @@
       <c r="I27" s="65">
         <v>43121</v>
       </c>
-      <c r="J27" s="146">
+      <c r="J27" s="155">
         <v>0.25</v>
       </c>
-      <c r="K27" s="98"/>
+      <c r="K27" s="107"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="114">
+      <c r="A28" s="123">
         <v>26</v>
       </c>
-      <c r="B28" s="122"/>
+      <c r="B28" s="131"/>
       <c r="C28" s="52" t="s">
         <v>117</v>
       </c>
@@ -2858,13 +2961,13 @@
       <c r="F28" s="58"/>
       <c r="H28" s="71"/>
       <c r="I28" s="56"/>
-      <c r="J28" s="126"/>
+      <c r="J28" s="135"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="114">
+      <c r="A29" s="123">
         <v>27</v>
       </c>
-      <c r="B29" s="122"/>
+      <c r="B29" s="131"/>
       <c r="C29" s="52" t="s">
         <v>119</v>
       </c>
@@ -2873,13 +2976,13 @@
       <c r="F29" s="58"/>
       <c r="H29" s="71"/>
       <c r="I29" s="56"/>
-      <c r="J29" s="126"/>
+      <c r="J29" s="135"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="115">
+      <c r="A30" s="124">
         <v>28</v>
       </c>
-      <c r="B30" s="123"/>
+      <c r="B30" s="132"/>
       <c r="C30" s="51" t="s">
         <v>121</v>
       </c>
@@ -2889,13 +2992,13 @@
       <c r="G30" s="73"/>
       <c r="H30" s="69"/>
       <c r="I30" s="55"/>
-      <c r="J30" s="129"/>
+      <c r="J30" s="138"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="113">
+      <c r="A31" s="122">
         <v>29</v>
       </c>
-      <c r="B31" s="121" t="s">
+      <c r="B31" s="130" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="59" t="s">
@@ -2919,16 +3022,16 @@
       <c r="I31" s="65">
         <v>43121</v>
       </c>
-      <c r="J31" s="146">
+      <c r="J31" s="155">
         <v>0.25</v>
       </c>
-      <c r="K31" s="98"/>
+      <c r="K31" s="107"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="114">
+      <c r="A32" s="123">
         <v>30</v>
       </c>
-      <c r="B32" s="122"/>
+      <c r="B32" s="131"/>
       <c r="C32" s="52" t="s">
         <v>117</v>
       </c>
@@ -2937,13 +3040,13 @@
       <c r="F32" s="58"/>
       <c r="H32" s="71"/>
       <c r="I32" s="56"/>
-      <c r="J32" s="126"/>
+      <c r="J32" s="135"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="114">
+      <c r="A33" s="123">
         <v>31</v>
       </c>
-      <c r="B33" s="122"/>
+      <c r="B33" s="131"/>
       <c r="C33" s="52" t="s">
         <v>119</v>
       </c>
@@ -2952,13 +3055,13 @@
       <c r="F33" s="58"/>
       <c r="H33" s="71"/>
       <c r="I33" s="56"/>
-      <c r="J33" s="126"/>
+      <c r="J33" s="135"/>
     </row>
     <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="115">
+      <c r="A34" s="124">
         <v>32</v>
       </c>
-      <c r="B34" s="123"/>
+      <c r="B34" s="132"/>
       <c r="C34" s="51" t="s">
         <v>121</v>
       </c>
@@ -2968,13 +3071,13 @@
       <c r="G34" s="73"/>
       <c r="H34" s="69"/>
       <c r="I34" s="55"/>
-      <c r="J34" s="129"/>
+      <c r="J34" s="138"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="113">
+      <c r="A35" s="122">
         <v>33</v>
       </c>
-      <c r="B35" s="121" t="s">
+      <c r="B35" s="130" t="s">
         <v>14</v>
       </c>
       <c r="C35" s="59" t="s">
@@ -2992,25 +3095,25 @@
       <c r="G35" s="72">
         <v>1</v>
       </c>
-      <c r="H35" s="93">
+      <c r="H35" s="102">
         <v>43121</v>
       </c>
-      <c r="I35" s="94">
+      <c r="I35" s="103">
         <v>43121</v>
       </c>
-      <c r="J35" s="146">
+      <c r="J35" s="155">
         <v>0.25</v>
       </c>
-      <c r="K35" s="98"/>
-      <c r="L35" s="100" t="s">
+      <c r="K35" s="107"/>
+      <c r="L35" s="109" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="114">
+      <c r="A36" s="123">
         <v>34</v>
       </c>
-      <c r="B36" s="122"/>
+      <c r="B36" s="131"/>
       <c r="C36" s="52" t="s">
         <v>117</v>
       </c>
@@ -3019,16 +3122,16 @@
       <c r="F36" s="54"/>
       <c r="H36" s="71"/>
       <c r="I36" s="56"/>
-      <c r="J36" s="126"/>
-      <c r="L36" s="100" t="s">
+      <c r="J36" s="135"/>
+      <c r="L36" s="109" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="114">
+      <c r="A37" s="123">
         <v>35</v>
       </c>
-      <c r="B37" s="122"/>
+      <c r="B37" s="131"/>
       <c r="C37" s="52" t="s">
         <v>119</v>
       </c>
@@ -3037,14 +3140,14 @@
       <c r="F37" s="54"/>
       <c r="H37" s="71"/>
       <c r="I37" s="56"/>
-      <c r="J37" s="126"/>
-      <c r="K37" s="101"/>
+      <c r="J37" s="135"/>
+      <c r="K37" s="110"/>
     </row>
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="115">
+      <c r="A38" s="124">
         <v>36</v>
       </c>
-      <c r="B38" s="123"/>
+      <c r="B38" s="132"/>
       <c r="C38" s="51" t="s">
         <v>121</v>
       </c>
@@ -3054,14 +3157,14 @@
       <c r="G38" s="73"/>
       <c r="H38" s="69"/>
       <c r="I38" s="55"/>
-      <c r="J38" s="129"/>
-      <c r="K38" s="101"/>
+      <c r="J38" s="138"/>
+      <c r="K38" s="110"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="113">
+      <c r="A39" s="122">
         <v>37</v>
       </c>
-      <c r="B39" s="143" t="s">
+      <c r="B39" s="152" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="59" t="s">
@@ -3079,22 +3182,22 @@
       <c r="G39" s="72">
         <v>1</v>
       </c>
-      <c r="H39" s="93">
+      <c r="H39" s="102">
         <v>43121</v>
       </c>
-      <c r="I39" s="94">
+      <c r="I39" s="103">
         <v>43121</v>
       </c>
-      <c r="J39" s="146">
+      <c r="J39" s="155">
         <v>0.25</v>
       </c>
-      <c r="K39" s="98"/>
+      <c r="K39" s="107"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="114">
+      <c r="A40" s="123">
         <v>38</v>
       </c>
-      <c r="B40" s="144"/>
+      <c r="B40" s="153"/>
       <c r="C40" s="52" t="s">
         <v>117</v>
       </c>
@@ -3104,13 +3207,13 @@
       <c r="G40" s="75"/>
       <c r="H40" s="56"/>
       <c r="I40" s="56"/>
-      <c r="J40" s="126"/>
+      <c r="J40" s="135"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="114">
+      <c r="A41" s="123">
         <v>39</v>
       </c>
-      <c r="B41" s="144"/>
+      <c r="B41" s="153"/>
       <c r="C41" s="52" t="s">
         <v>119</v>
       </c>
@@ -3120,13 +3223,13 @@
       <c r="G41" s="75"/>
       <c r="H41" s="56"/>
       <c r="I41" s="56"/>
-      <c r="J41" s="126"/>
+      <c r="J41" s="135"/>
     </row>
     <row r="42" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="115">
+      <c r="A42" s="124">
         <v>40</v>
       </c>
-      <c r="B42" s="145"/>
+      <c r="B42" s="154"/>
       <c r="C42" s="51" t="s">
         <v>121</v>
       </c>
@@ -3136,13 +3239,13 @@
       <c r="G42" s="73"/>
       <c r="H42" s="55"/>
       <c r="I42" s="55"/>
-      <c r="J42" s="129"/>
+      <c r="J42" s="138"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="113">
+      <c r="A43" s="122">
         <v>41</v>
       </c>
-      <c r="B43" s="121" t="s">
+      <c r="B43" s="130" t="s">
         <v>128</v>
       </c>
       <c r="C43" s="59" t="s">
@@ -3160,22 +3263,22 @@
       <c r="G43" s="72">
         <v>1</v>
       </c>
-      <c r="H43" s="93">
+      <c r="H43" s="102">
         <v>43121</v>
       </c>
-      <c r="I43" s="94">
+      <c r="I43" s="103">
         <v>43121</v>
       </c>
-      <c r="J43" s="146">
+      <c r="J43" s="155">
         <v>0.25</v>
       </c>
-      <c r="K43" s="98"/>
+      <c r="K43" s="107"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="114">
+      <c r="A44" s="123">
         <v>42</v>
       </c>
-      <c r="B44" s="122"/>
+      <c r="B44" s="131"/>
       <c r="C44" s="52" t="s">
         <v>117</v>
       </c>
@@ -3185,13 +3288,13 @@
       <c r="G44" s="75"/>
       <c r="H44" s="56"/>
       <c r="I44" s="56"/>
-      <c r="J44" s="126"/>
+      <c r="J44" s="135"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="114">
+      <c r="A45" s="123">
         <v>43</v>
       </c>
-      <c r="B45" s="122"/>
+      <c r="B45" s="131"/>
       <c r="C45" s="52" t="s">
         <v>119</v>
       </c>
@@ -3201,13 +3304,13 @@
       <c r="G45" s="75"/>
       <c r="H45" s="56"/>
       <c r="I45" s="56"/>
-      <c r="J45" s="126"/>
+      <c r="J45" s="135"/>
     </row>
     <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="115">
+      <c r="A46" s="124">
         <v>44</v>
       </c>
-      <c r="B46" s="123"/>
+      <c r="B46" s="132"/>
       <c r="C46" s="51" t="s">
         <v>121</v>
       </c>
@@ -3217,13 +3320,13 @@
       <c r="G46" s="73"/>
       <c r="H46" s="55"/>
       <c r="I46" s="55"/>
-      <c r="J46" s="129"/>
+      <c r="J46" s="138"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="113">
+      <c r="A47" s="122">
         <v>45</v>
       </c>
-      <c r="B47" s="121" t="s">
+      <c r="B47" s="130" t="s">
         <v>129</v>
       </c>
       <c r="C47" s="59" t="s">
@@ -3241,22 +3344,22 @@
       <c r="G47" s="72">
         <v>1</v>
       </c>
-      <c r="H47" s="93">
+      <c r="H47" s="102">
         <v>43121</v>
       </c>
-      <c r="I47" s="94">
+      <c r="I47" s="103">
         <v>43121</v>
       </c>
-      <c r="J47" s="146">
+      <c r="J47" s="155">
         <v>0.25</v>
       </c>
-      <c r="K47" s="98"/>
+      <c r="K47" s="107"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="114">
+      <c r="A48" s="123">
         <v>46</v>
       </c>
-      <c r="B48" s="122"/>
+      <c r="B48" s="131"/>
       <c r="C48" s="52" t="s">
         <v>117</v>
       </c>
@@ -3266,13 +3369,13 @@
       <c r="G48" s="75"/>
       <c r="H48" s="56"/>
       <c r="I48" s="56"/>
-      <c r="J48" s="126"/>
+      <c r="J48" s="135"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="114">
+      <c r="A49" s="123">
         <v>47</v>
       </c>
-      <c r="B49" s="122"/>
+      <c r="B49" s="131"/>
       <c r="C49" s="52" t="s">
         <v>119</v>
       </c>
@@ -3282,13 +3385,13 @@
       <c r="G49" s="75"/>
       <c r="H49" s="56"/>
       <c r="I49" s="56"/>
-      <c r="J49" s="126"/>
+      <c r="J49" s="135"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="115">
+      <c r="A50" s="124">
         <v>48</v>
       </c>
-      <c r="B50" s="123"/>
+      <c r="B50" s="132"/>
       <c r="C50" s="51" t="s">
         <v>121</v>
       </c>
@@ -3298,13 +3401,13 @@
       <c r="G50" s="73"/>
       <c r="H50" s="55"/>
       <c r="I50" s="55"/>
-      <c r="J50" s="129"/>
+      <c r="J50" s="138"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="113">
+      <c r="A51" s="122">
         <v>49</v>
       </c>
-      <c r="B51" s="143" t="s">
+      <c r="B51" s="152" t="s">
         <v>46</v>
       </c>
       <c r="C51" s="59" t="s">
@@ -3322,22 +3425,22 @@
       <c r="G51" s="72">
         <v>1</v>
       </c>
-      <c r="H51" s="93">
+      <c r="H51" s="102">
         <v>43121</v>
       </c>
-      <c r="I51" s="94">
+      <c r="I51" s="103">
         <v>43121</v>
       </c>
-      <c r="J51" s="146">
+      <c r="J51" s="155">
         <v>0.25</v>
       </c>
-      <c r="K51" s="98"/>
+      <c r="K51" s="107"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="114">
+      <c r="A52" s="123">
         <v>50</v>
       </c>
-      <c r="B52" s="144"/>
+      <c r="B52" s="153"/>
       <c r="C52" s="52" t="s">
         <v>117</v>
       </c>
@@ -3347,13 +3450,13 @@
       <c r="G52" s="75"/>
       <c r="H52" s="56"/>
       <c r="I52" s="56"/>
-      <c r="J52" s="126"/>
+      <c r="J52" s="135"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="114">
+      <c r="A53" s="123">
         <v>51</v>
       </c>
-      <c r="B53" s="144"/>
+      <c r="B53" s="153"/>
       <c r="C53" s="52" t="s">
         <v>119</v>
       </c>
@@ -3363,13 +3466,13 @@
       <c r="G53" s="75"/>
       <c r="H53" s="56"/>
       <c r="I53" s="56"/>
-      <c r="J53" s="126"/>
+      <c r="J53" s="135"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="115">
+      <c r="A54" s="124">
         <v>52</v>
       </c>
-      <c r="B54" s="145"/>
+      <c r="B54" s="154"/>
       <c r="C54" s="51" t="s">
         <v>121</v>
       </c>
@@ -3379,181 +3482,181 @@
       <c r="G54" s="73"/>
       <c r="H54" s="55"/>
       <c r="I54" s="55"/>
-      <c r="J54" s="129"/>
-    </row>
-    <row r="55" spans="1:11" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="113">
+      <c r="J54" s="138"/>
+    </row>
+    <row r="55" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="122">
         <v>53</v>
       </c>
-      <c r="B55" s="143" t="s">
+      <c r="B55" s="152" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="95" t="s">
+      <c r="C55" s="104" t="s">
         <v>118</v>
       </c>
       <c r="D55" s="90">
         <v>1</v>
       </c>
-      <c r="E55" s="102">
+      <c r="E55" s="111">
         <v>43121</v>
       </c>
-      <c r="F55" s="102">
+      <c r="F55" s="111">
         <v>43121</v>
       </c>
-      <c r="G55" s="96">
-        <v>1</v>
-      </c>
-      <c r="H55" s="102">
+      <c r="G55" s="105">
+        <v>1</v>
+      </c>
+      <c r="H55" s="111">
         <v>43121</v>
       </c>
-      <c r="I55" s="102">
+      <c r="I55" s="111">
         <v>43121</v>
       </c>
-      <c r="J55" s="146">
+      <c r="J55" s="155">
         <v>0.25</v>
       </c>
-      <c r="K55" s="98"/>
-    </row>
-    <row r="56" spans="1:11" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="114">
+      <c r="K55" s="107"/>
+    </row>
+    <row r="56" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="123">
         <v>54</v>
       </c>
-      <c r="B56" s="144"/>
-      <c r="C56" s="105" t="s">
+      <c r="B56" s="153"/>
+      <c r="C56" s="114" t="s">
         <v>117</v>
       </c>
       <c r="D56" s="91"/>
-      <c r="E56" s="106"/>
-      <c r="F56" s="107"/>
-      <c r="G56" s="108"/>
-      <c r="H56" s="107"/>
-      <c r="I56" s="107"/>
-      <c r="J56" s="126"/>
-      <c r="K56" s="103"/>
-    </row>
-    <row r="57" spans="1:11" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="114">
+      <c r="E56" s="115"/>
+      <c r="F56" s="116"/>
+      <c r="G56" s="117"/>
+      <c r="H56" s="116"/>
+      <c r="I56" s="116"/>
+      <c r="J56" s="135"/>
+      <c r="K56" s="112"/>
+    </row>
+    <row r="57" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="123">
         <v>55</v>
       </c>
-      <c r="B57" s="144"/>
-      <c r="C57" s="105" t="s">
+      <c r="B57" s="153"/>
+      <c r="C57" s="114" t="s">
         <v>119</v>
       </c>
       <c r="D57" s="91"/>
-      <c r="E57" s="106"/>
-      <c r="F57" s="107"/>
-      <c r="G57" s="108"/>
-      <c r="H57" s="107"/>
-      <c r="I57" s="107"/>
-      <c r="J57" s="126"/>
-      <c r="K57" s="103"/>
-    </row>
-    <row r="58" spans="1:11" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="115">
+      <c r="E57" s="115"/>
+      <c r="F57" s="116"/>
+      <c r="G57" s="117"/>
+      <c r="H57" s="116"/>
+      <c r="I57" s="116"/>
+      <c r="J57" s="135"/>
+      <c r="K57" s="112"/>
+    </row>
+    <row r="58" spans="1:11" s="113" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="124">
         <v>56</v>
       </c>
-      <c r="B58" s="145"/>
-      <c r="C58" s="109" t="s">
+      <c r="B58" s="154"/>
+      <c r="C58" s="118" t="s">
         <v>121</v>
       </c>
       <c r="D58" s="92"/>
-      <c r="E58" s="110"/>
-      <c r="F58" s="111"/>
-      <c r="G58" s="112"/>
-      <c r="H58" s="111"/>
-      <c r="I58" s="111"/>
-      <c r="J58" s="129"/>
-      <c r="K58" s="103"/>
-    </row>
-    <row r="59" spans="1:11" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="113">
+      <c r="E58" s="119"/>
+      <c r="F58" s="120"/>
+      <c r="G58" s="121"/>
+      <c r="H58" s="120"/>
+      <c r="I58" s="120"/>
+      <c r="J58" s="138"/>
+      <c r="K58" s="112"/>
+    </row>
+    <row r="59" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="122">
         <v>57</v>
       </c>
-      <c r="B59" s="143" t="s">
+      <c r="B59" s="152" t="s">
         <v>145</v>
       </c>
-      <c r="C59" s="95" t="s">
+      <c r="C59" s="104" t="s">
         <v>118</v>
       </c>
       <c r="D59" s="90">
         <v>1</v>
       </c>
-      <c r="E59" s="102">
+      <c r="E59" s="111">
         <v>43121</v>
       </c>
-      <c r="F59" s="102">
+      <c r="F59" s="111">
         <v>43121</v>
       </c>
-      <c r="G59" s="96">
-        <v>1</v>
-      </c>
-      <c r="H59" s="102">
+      <c r="G59" s="105">
+        <v>1</v>
+      </c>
+      <c r="H59" s="111">
         <v>43121</v>
       </c>
-      <c r="I59" s="102">
+      <c r="I59" s="111">
         <v>43121</v>
       </c>
-      <c r="J59" s="146">
+      <c r="J59" s="155">
         <v>0.25</v>
       </c>
-      <c r="K59" s="98"/>
-    </row>
-    <row r="60" spans="1:11" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="114">
+      <c r="K59" s="107"/>
+    </row>
+    <row r="60" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="123">
         <v>58</v>
       </c>
-      <c r="B60" s="144"/>
-      <c r="C60" s="105" t="s">
+      <c r="B60" s="153"/>
+      <c r="C60" s="114" t="s">
         <v>117</v>
       </c>
       <c r="D60" s="91"/>
-      <c r="E60" s="106"/>
-      <c r="F60" s="107"/>
-      <c r="G60" s="108"/>
-      <c r="H60" s="107"/>
-      <c r="I60" s="107"/>
-      <c r="J60" s="126"/>
-      <c r="K60" s="103"/>
-    </row>
-    <row r="61" spans="1:11" s="104" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="114">
+      <c r="E60" s="115"/>
+      <c r="F60" s="116"/>
+      <c r="G60" s="117"/>
+      <c r="H60" s="116"/>
+      <c r="I60" s="116"/>
+      <c r="J60" s="135"/>
+      <c r="K60" s="112"/>
+    </row>
+    <row r="61" spans="1:11" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="123">
         <v>59</v>
       </c>
-      <c r="B61" s="144"/>
-      <c r="C61" s="105" t="s">
+      <c r="B61" s="153"/>
+      <c r="C61" s="114" t="s">
         <v>119</v>
       </c>
       <c r="D61" s="91"/>
-      <c r="E61" s="106"/>
-      <c r="F61" s="107"/>
-      <c r="G61" s="108"/>
-      <c r="H61" s="107"/>
-      <c r="I61" s="107"/>
-      <c r="J61" s="126"/>
-      <c r="K61" s="103"/>
-    </row>
-    <row r="62" spans="1:11" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="115">
+      <c r="E61" s="115"/>
+      <c r="F61" s="116"/>
+      <c r="G61" s="117"/>
+      <c r="H61" s="116"/>
+      <c r="I61" s="116"/>
+      <c r="J61" s="135"/>
+      <c r="K61" s="112"/>
+    </row>
+    <row r="62" spans="1:11" s="113" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="124">
         <v>60</v>
       </c>
-      <c r="B62" s="145"/>
-      <c r="C62" s="109" t="s">
+      <c r="B62" s="154"/>
+      <c r="C62" s="118" t="s">
         <v>121</v>
       </c>
       <c r="D62" s="92"/>
-      <c r="E62" s="110"/>
-      <c r="F62" s="111"/>
-      <c r="G62" s="112"/>
-      <c r="H62" s="111"/>
-      <c r="I62" s="111"/>
-      <c r="J62" s="129"/>
-      <c r="K62" s="103"/>
+      <c r="E62" s="119"/>
+      <c r="F62" s="120"/>
+      <c r="G62" s="121"/>
+      <c r="H62" s="120"/>
+      <c r="I62" s="120"/>
+      <c r="J62" s="138"/>
+      <c r="K62" s="112"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="113">
+      <c r="A63" s="122">
         <v>61</v>
       </c>
-      <c r="B63" s="143" t="s">
+      <c r="B63" s="152" t="s">
         <v>61</v>
       </c>
       <c r="C63" s="59" t="s">
@@ -3562,31 +3665,31 @@
       <c r="D63" s="44">
         <v>1</v>
       </c>
-      <c r="E63" s="102">
+      <c r="E63" s="111">
         <v>43121</v>
       </c>
-      <c r="F63" s="102">
+      <c r="F63" s="111">
         <v>43121</v>
       </c>
-      <c r="G63" s="96">
-        <v>1</v>
-      </c>
-      <c r="H63" s="102">
+      <c r="G63" s="105">
+        <v>1</v>
+      </c>
+      <c r="H63" s="111">
         <v>43121</v>
       </c>
-      <c r="I63" s="102">
+      <c r="I63" s="111">
         <v>43121</v>
       </c>
-      <c r="J63" s="146">
+      <c r="J63" s="155">
         <v>0.25</v>
       </c>
-      <c r="K63" s="98"/>
+      <c r="K63" s="107"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="114">
+      <c r="A64" s="123">
         <v>62</v>
       </c>
-      <c r="B64" s="144"/>
+      <c r="B64" s="153"/>
       <c r="C64" s="52" t="s">
         <v>117</v>
       </c>
@@ -3596,13 +3699,13 @@
       <c r="G64" s="75"/>
       <c r="H64" s="56"/>
       <c r="I64" s="56"/>
-      <c r="J64" s="126"/>
+      <c r="J64" s="135"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="114">
+      <c r="A65" s="123">
         <v>63</v>
       </c>
-      <c r="B65" s="144"/>
+      <c r="B65" s="153"/>
       <c r="C65" s="52" t="s">
         <v>119</v>
       </c>
@@ -3612,13 +3715,13 @@
       <c r="G65" s="75"/>
       <c r="H65" s="56"/>
       <c r="I65" s="56"/>
-      <c r="J65" s="126"/>
+      <c r="J65" s="135"/>
     </row>
     <row r="66" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="115">
+      <c r="A66" s="124">
         <v>64</v>
       </c>
-      <c r="B66" s="145"/>
+      <c r="B66" s="154"/>
       <c r="C66" s="51" t="s">
         <v>121</v>
       </c>
@@ -3628,13 +3731,13 @@
       <c r="G66" s="73"/>
       <c r="H66" s="55"/>
       <c r="I66" s="55"/>
-      <c r="J66" s="129"/>
+      <c r="J66" s="138"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="113">
+      <c r="A67" s="122">
         <v>65</v>
       </c>
-      <c r="B67" s="143" t="s">
+      <c r="B67" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C67" s="59" t="s">
@@ -3643,31 +3746,31 @@
       <c r="D67" s="44">
         <v>1</v>
       </c>
-      <c r="E67" s="102">
+      <c r="E67" s="111">
         <v>43121</v>
       </c>
-      <c r="F67" s="102">
+      <c r="F67" s="111">
         <v>43121</v>
       </c>
-      <c r="G67" s="96">
-        <v>1</v>
-      </c>
-      <c r="H67" s="102">
+      <c r="G67" s="105">
+        <v>1</v>
+      </c>
+      <c r="H67" s="111">
         <v>43121</v>
       </c>
-      <c r="I67" s="102">
+      <c r="I67" s="111">
         <v>43121</v>
       </c>
-      <c r="J67" s="146">
+      <c r="J67" s="155">
         <v>0.25</v>
       </c>
-      <c r="K67" s="98"/>
+      <c r="K67" s="107"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="114">
+      <c r="A68" s="123">
         <v>66</v>
       </c>
-      <c r="B68" s="144"/>
+      <c r="B68" s="153"/>
       <c r="C68" s="52" t="s">
         <v>117</v>
       </c>
@@ -3677,13 +3780,13 @@
       <c r="G68" s="75"/>
       <c r="H68" s="56"/>
       <c r="I68" s="56"/>
-      <c r="J68" s="126"/>
+      <c r="J68" s="135"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="114">
+      <c r="A69" s="123">
         <v>67</v>
       </c>
-      <c r="B69" s="144"/>
+      <c r="B69" s="153"/>
       <c r="C69" s="52" t="s">
         <v>119</v>
       </c>
@@ -3693,13 +3796,13 @@
       <c r="G69" s="75"/>
       <c r="H69" s="56"/>
       <c r="I69" s="56"/>
-      <c r="J69" s="126"/>
+      <c r="J69" s="135"/>
     </row>
     <row r="70" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="115">
+      <c r="A70" s="124">
         <v>68</v>
       </c>
-      <c r="B70" s="145"/>
+      <c r="B70" s="154"/>
       <c r="C70" s="51" t="s">
         <v>121</v>
       </c>
@@ -3709,13 +3812,13 @@
       <c r="G70" s="73"/>
       <c r="H70" s="55"/>
       <c r="I70" s="55"/>
-      <c r="J70" s="129"/>
+      <c r="J70" s="138"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="113">
+      <c r="A71" s="122">
         <v>69</v>
       </c>
-      <c r="B71" s="121" t="s">
+      <c r="B71" s="130" t="s">
         <v>62</v>
       </c>
       <c r="C71" s="59" t="s">
@@ -3724,31 +3827,31 @@
       <c r="D71" s="44">
         <v>1</v>
       </c>
-      <c r="E71" s="102">
+      <c r="E71" s="111">
         <v>43121</v>
       </c>
-      <c r="F71" s="102">
+      <c r="F71" s="111">
         <v>43121</v>
       </c>
-      <c r="G71" s="96">
-        <v>1</v>
-      </c>
-      <c r="H71" s="102">
+      <c r="G71" s="105">
+        <v>1</v>
+      </c>
+      <c r="H71" s="111">
         <v>43121</v>
       </c>
-      <c r="I71" s="102">
+      <c r="I71" s="111">
         <v>43121</v>
       </c>
-      <c r="J71" s="146">
+      <c r="J71" s="155">
         <v>0.25</v>
       </c>
-      <c r="K71" s="98"/>
+      <c r="K71" s="107"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="114">
+      <c r="A72" s="123">
         <v>70</v>
       </c>
-      <c r="B72" s="122"/>
+      <c r="B72" s="131"/>
       <c r="C72" s="52" t="s">
         <v>117</v>
       </c>
@@ -3758,13 +3861,13 @@
       <c r="G72" s="75"/>
       <c r="H72" s="56"/>
       <c r="I72" s="56"/>
-      <c r="J72" s="126"/>
+      <c r="J72" s="135"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="114">
+      <c r="A73" s="123">
         <v>71</v>
       </c>
-      <c r="B73" s="122"/>
+      <c r="B73" s="131"/>
       <c r="C73" s="52" t="s">
         <v>119</v>
       </c>
@@ -3774,13 +3877,13 @@
       <c r="G73" s="75"/>
       <c r="H73" s="56"/>
       <c r="I73" s="56"/>
-      <c r="J73" s="126"/>
+      <c r="J73" s="135"/>
     </row>
     <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="115">
+      <c r="A74" s="124">
         <v>72</v>
       </c>
-      <c r="B74" s="123"/>
+      <c r="B74" s="132"/>
       <c r="C74" s="51" t="s">
         <v>121</v>
       </c>
@@ -3790,13 +3893,13 @@
       <c r="G74" s="73"/>
       <c r="H74" s="55"/>
       <c r="I74" s="55"/>
-      <c r="J74" s="129"/>
+      <c r="J74" s="138"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="113">
+      <c r="A75" s="122">
         <v>73</v>
       </c>
-      <c r="B75" s="121" t="s">
+      <c r="B75" s="130" t="s">
         <v>66</v>
       </c>
       <c r="C75" s="59" t="s">
@@ -3805,31 +3908,31 @@
       <c r="D75" s="44">
         <v>1</v>
       </c>
-      <c r="E75" s="102">
+      <c r="E75" s="111">
         <v>43121</v>
       </c>
-      <c r="F75" s="102">
+      <c r="F75" s="111">
         <v>43121</v>
       </c>
-      <c r="G75" s="96">
-        <v>1</v>
-      </c>
-      <c r="H75" s="102">
+      <c r="G75" s="105">
+        <v>1</v>
+      </c>
+      <c r="H75" s="111">
         <v>43121</v>
       </c>
-      <c r="I75" s="102">
+      <c r="I75" s="111">
         <v>43121</v>
       </c>
-      <c r="J75" s="146">
+      <c r="J75" s="155">
         <v>0.25</v>
       </c>
-      <c r="K75" s="98"/>
+      <c r="K75" s="107"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="114">
+      <c r="A76" s="123">
         <v>74</v>
       </c>
-      <c r="B76" s="122"/>
+      <c r="B76" s="131"/>
       <c r="C76" s="52" t="s">
         <v>117</v>
       </c>
@@ -3839,13 +3942,13 @@
       <c r="G76" s="75"/>
       <c r="H76" s="56"/>
       <c r="I76" s="56"/>
-      <c r="J76" s="126"/>
+      <c r="J76" s="135"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="114">
+      <c r="A77" s="123">
         <v>75</v>
       </c>
-      <c r="B77" s="122"/>
+      <c r="B77" s="131"/>
       <c r="C77" s="52" t="s">
         <v>119</v>
       </c>
@@ -3855,13 +3958,13 @@
       <c r="G77" s="75"/>
       <c r="H77" s="56"/>
       <c r="I77" s="56"/>
-      <c r="J77" s="126"/>
+      <c r="J77" s="135"/>
     </row>
     <row r="78" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="115">
+      <c r="A78" s="124">
         <v>76</v>
       </c>
-      <c r="B78" s="123"/>
+      <c r="B78" s="132"/>
       <c r="C78" s="51" t="s">
         <v>121</v>
       </c>
@@ -3871,13 +3974,13 @@
       <c r="G78" s="73"/>
       <c r="H78" s="55"/>
       <c r="I78" s="55"/>
-      <c r="J78" s="129"/>
+      <c r="J78" s="138"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="113">
+      <c r="A79" s="122">
         <v>77</v>
       </c>
-      <c r="B79" s="121" t="s">
+      <c r="B79" s="130" t="s">
         <v>67</v>
       </c>
       <c r="C79" s="59" t="s">
@@ -3886,31 +3989,31 @@
       <c r="D79" s="44">
         <v>1</v>
       </c>
-      <c r="E79" s="102">
+      <c r="E79" s="111">
         <v>43121</v>
       </c>
-      <c r="F79" s="102">
+      <c r="F79" s="111">
         <v>43121</v>
       </c>
-      <c r="G79" s="96">
-        <v>1</v>
-      </c>
-      <c r="H79" s="102">
+      <c r="G79" s="105">
+        <v>1</v>
+      </c>
+      <c r="H79" s="111">
         <v>43121</v>
       </c>
-      <c r="I79" s="102">
+      <c r="I79" s="111">
         <v>43121</v>
       </c>
-      <c r="J79" s="146">
+      <c r="J79" s="155">
         <v>0.25</v>
       </c>
-      <c r="K79" s="98"/>
+      <c r="K79" s="107"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="114">
+      <c r="A80" s="123">
         <v>78</v>
       </c>
-      <c r="B80" s="122"/>
+      <c r="B80" s="131"/>
       <c r="C80" s="52" t="s">
         <v>117</v>
       </c>
@@ -3920,13 +4023,13 @@
       <c r="G80" s="75"/>
       <c r="H80" s="56"/>
       <c r="I80" s="56"/>
-      <c r="J80" s="126"/>
+      <c r="J80" s="135"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="114">
+      <c r="A81" s="123">
         <v>79</v>
       </c>
-      <c r="B81" s="122"/>
+      <c r="B81" s="131"/>
       <c r="C81" s="52" t="s">
         <v>119</v>
       </c>
@@ -3936,13 +4039,13 @@
       <c r="G81" s="75"/>
       <c r="H81" s="56"/>
       <c r="I81" s="56"/>
-      <c r="J81" s="126"/>
+      <c r="J81" s="135"/>
     </row>
     <row r="82" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="115">
+      <c r="A82" s="124">
         <v>80</v>
       </c>
-      <c r="B82" s="123"/>
+      <c r="B82" s="132"/>
       <c r="C82" s="51" t="s">
         <v>121</v>
       </c>
@@ -3952,181 +4055,181 @@
       <c r="G82" s="73"/>
       <c r="H82" s="55"/>
       <c r="I82" s="55"/>
-      <c r="J82" s="129"/>
+      <c r="J82" s="138"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="113">
+      <c r="A83" s="122">
         <v>81</v>
       </c>
-      <c r="B83" s="143" t="s">
+      <c r="B83" s="152" t="s">
         <v>68</v>
       </c>
-      <c r="C83" s="95" t="s">
+      <c r="C83" s="104" t="s">
         <v>118</v>
       </c>
       <c r="D83" s="90">
         <v>1</v>
       </c>
-      <c r="E83" s="102">
+      <c r="E83" s="111">
         <v>43121</v>
       </c>
-      <c r="F83" s="102">
+      <c r="F83" s="111">
         <v>43121</v>
       </c>
-      <c r="G83" s="96">
-        <v>1</v>
-      </c>
-      <c r="H83" s="102">
+      <c r="G83" s="105">
+        <v>1</v>
+      </c>
+      <c r="H83" s="111">
         <v>43121</v>
       </c>
-      <c r="I83" s="102">
+      <c r="I83" s="111">
         <v>43121</v>
       </c>
-      <c r="J83" s="146">
+      <c r="J83" s="155">
         <v>0.25</v>
       </c>
-      <c r="K83" s="98"/>
+      <c r="K83" s="107"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="114">
+      <c r="A84" s="123">
         <v>82</v>
       </c>
-      <c r="B84" s="144"/>
-      <c r="C84" s="105" t="s">
+      <c r="B84" s="153"/>
+      <c r="C84" s="114" t="s">
         <v>117</v>
       </c>
       <c r="D84" s="91"/>
-      <c r="E84" s="107"/>
-      <c r="F84" s="107"/>
-      <c r="G84" s="108"/>
-      <c r="H84" s="107"/>
-      <c r="I84" s="107"/>
-      <c r="J84" s="126"/>
-      <c r="K84" s="103"/>
+      <c r="E84" s="116"/>
+      <c r="F84" s="116"/>
+      <c r="G84" s="117"/>
+      <c r="H84" s="116"/>
+      <c r="I84" s="116"/>
+      <c r="J84" s="135"/>
+      <c r="K84" s="112"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="114">
+      <c r="A85" s="123">
         <v>83</v>
       </c>
-      <c r="B85" s="144"/>
-      <c r="C85" s="105" t="s">
+      <c r="B85" s="153"/>
+      <c r="C85" s="114" t="s">
         <v>119</v>
       </c>
       <c r="D85" s="91"/>
-      <c r="E85" s="107"/>
-      <c r="F85" s="107"/>
-      <c r="G85" s="108"/>
-      <c r="H85" s="107"/>
-      <c r="I85" s="107"/>
-      <c r="J85" s="126"/>
-      <c r="K85" s="103"/>
+      <c r="E85" s="116"/>
+      <c r="F85" s="116"/>
+      <c r="G85" s="117"/>
+      <c r="H85" s="116"/>
+      <c r="I85" s="116"/>
+      <c r="J85" s="135"/>
+      <c r="K85" s="112"/>
     </row>
     <row r="86" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="115">
+      <c r="A86" s="124">
         <v>84</v>
       </c>
-      <c r="B86" s="145"/>
-      <c r="C86" s="109" t="s">
+      <c r="B86" s="154"/>
+      <c r="C86" s="118" t="s">
         <v>121</v>
       </c>
       <c r="D86" s="92"/>
-      <c r="E86" s="111"/>
-      <c r="F86" s="111"/>
-      <c r="G86" s="112"/>
-      <c r="H86" s="111"/>
-      <c r="I86" s="111"/>
-      <c r="J86" s="129"/>
-      <c r="K86" s="103"/>
+      <c r="E86" s="120"/>
+      <c r="F86" s="120"/>
+      <c r="G86" s="121"/>
+      <c r="H86" s="120"/>
+      <c r="I86" s="120"/>
+      <c r="J86" s="138"/>
+      <c r="K86" s="112"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="113">
+      <c r="A87" s="122">
         <v>85</v>
       </c>
-      <c r="B87" s="143" t="s">
+      <c r="B87" s="152" t="s">
         <v>69</v>
       </c>
-      <c r="C87" s="95" t="s">
+      <c r="C87" s="104" t="s">
         <v>118</v>
       </c>
       <c r="D87" s="90">
         <v>1</v>
       </c>
-      <c r="E87" s="116">
+      <c r="E87" s="125">
         <v>43121</v>
       </c>
-      <c r="F87" s="116">
+      <c r="F87" s="125">
         <v>43121</v>
       </c>
-      <c r="G87" s="117">
-        <v>1</v>
-      </c>
-      <c r="H87" s="116">
+      <c r="G87" s="126">
+        <v>1</v>
+      </c>
+      <c r="H87" s="125">
         <v>43121</v>
       </c>
-      <c r="I87" s="116">
+      <c r="I87" s="125">
         <v>43121</v>
       </c>
-      <c r="J87" s="146">
+      <c r="J87" s="155">
         <v>0.25</v>
       </c>
-      <c r="K87" s="98"/>
+      <c r="K87" s="107"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="114">
+      <c r="A88" s="123">
         <v>86</v>
       </c>
-      <c r="B88" s="144"/>
-      <c r="C88" s="105" t="s">
+      <c r="B88" s="153"/>
+      <c r="C88" s="114" t="s">
         <v>117</v>
       </c>
       <c r="D88" s="91"/>
-      <c r="E88" s="107"/>
-      <c r="F88" s="107"/>
-      <c r="G88" s="108"/>
-      <c r="H88" s="107"/>
-      <c r="I88" s="107"/>
-      <c r="J88" s="126"/>
-      <c r="K88" s="103"/>
+      <c r="E88" s="116"/>
+      <c r="F88" s="116"/>
+      <c r="G88" s="117"/>
+      <c r="H88" s="116"/>
+      <c r="I88" s="116"/>
+      <c r="J88" s="135"/>
+      <c r="K88" s="112"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A89" s="114">
+      <c r="A89" s="123">
         <v>87</v>
       </c>
-      <c r="B89" s="144"/>
-      <c r="C89" s="105" t="s">
+      <c r="B89" s="153"/>
+      <c r="C89" s="114" t="s">
         <v>119</v>
       </c>
       <c r="D89" s="91"/>
-      <c r="E89" s="107"/>
-      <c r="F89" s="107"/>
-      <c r="G89" s="108"/>
-      <c r="H89" s="107"/>
-      <c r="I89" s="107"/>
-      <c r="J89" s="126"/>
-      <c r="K89" s="103"/>
+      <c r="E89" s="116"/>
+      <c r="F89" s="116"/>
+      <c r="G89" s="117"/>
+      <c r="H89" s="116"/>
+      <c r="I89" s="116"/>
+      <c r="J89" s="135"/>
+      <c r="K89" s="112"/>
     </row>
     <row r="90" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="115">
+      <c r="A90" s="124">
         <v>88</v>
       </c>
-      <c r="B90" s="145"/>
-      <c r="C90" s="109" t="s">
+      <c r="B90" s="154"/>
+      <c r="C90" s="118" t="s">
         <v>121</v>
       </c>
       <c r="D90" s="92"/>
-      <c r="E90" s="111"/>
-      <c r="F90" s="111"/>
-      <c r="G90" s="112"/>
-      <c r="H90" s="111"/>
-      <c r="I90" s="111"/>
-      <c r="J90" s="129"/>
-      <c r="K90" s="103"/>
+      <c r="E90" s="120"/>
+      <c r="F90" s="120"/>
+      <c r="G90" s="121"/>
+      <c r="H90" s="120"/>
+      <c r="I90" s="120"/>
+      <c r="J90" s="138"/>
+      <c r="K90" s="112"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A91" s="113">
+      <c r="A91" s="122">
         <v>89</v>
       </c>
-      <c r="B91" s="121" t="s">
+      <c r="B91" s="130" t="s">
         <v>82</v>
       </c>
       <c r="C91" s="59" t="s">
@@ -4136,27 +4239,28 @@
         <v>1</v>
       </c>
       <c r="E91" s="65">
-        <v>43125</v>
+        <v>43122</v>
       </c>
       <c r="F91" s="65">
-        <v>43125</v>
+        <v>43123</v>
       </c>
       <c r="G91" s="74">
         <v>1</v>
       </c>
       <c r="H91" s="65">
-        <v>43125</v>
+        <v>43123</v>
       </c>
       <c r="I91" s="65">
-        <v>43125</v>
-      </c>
-      <c r="J91" s="126"/>
+        <v>43123</v>
+      </c>
+      <c r="J91" s="135"/>
+      <c r="K91" s="107"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" s="114">
+      <c r="A92" s="123">
         <v>90</v>
       </c>
-      <c r="B92" s="122"/>
+      <c r="B92" s="131"/>
       <c r="C92" s="52" t="s">
         <v>117</v>
       </c>
@@ -4166,13 +4270,13 @@
       <c r="G92" s="75"/>
       <c r="H92" s="56"/>
       <c r="I92" s="56"/>
-      <c r="J92" s="126"/>
+      <c r="J92" s="135"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="114">
+      <c r="A93" s="123">
         <v>91</v>
       </c>
-      <c r="B93" s="122"/>
+      <c r="B93" s="131"/>
       <c r="C93" s="52" t="s">
         <v>119</v>
       </c>
@@ -4182,13 +4286,13 @@
       <c r="G93" s="75"/>
       <c r="H93" s="56"/>
       <c r="I93" s="56"/>
-      <c r="J93" s="126"/>
+      <c r="J93" s="135"/>
     </row>
     <row r="94" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="115">
+      <c r="A94" s="124">
         <v>92</v>
       </c>
-      <c r="B94" s="123"/>
+      <c r="B94" s="132"/>
       <c r="C94" s="51" t="s">
         <v>121</v>
       </c>
@@ -4198,13 +4302,13 @@
       <c r="G94" s="73"/>
       <c r="H94" s="55"/>
       <c r="I94" s="55"/>
-      <c r="J94" s="129"/>
+      <c r="J94" s="138"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A95" s="113">
+      <c r="A95" s="122">
         <v>93</v>
       </c>
-      <c r="B95" s="121" t="s">
+      <c r="B95" s="130" t="s">
         <v>83</v>
       </c>
       <c r="C95" s="59" t="s">
@@ -4214,27 +4318,28 @@
         <v>1</v>
       </c>
       <c r="E95" s="65">
-        <v>43125</v>
+        <v>43123</v>
       </c>
       <c r="F95" s="65">
-        <v>43125</v>
+        <v>43123</v>
       </c>
       <c r="G95" s="74">
         <v>1</v>
       </c>
       <c r="H95" s="65">
-        <v>43125</v>
+        <v>43123</v>
       </c>
       <c r="I95" s="65">
-        <v>43125</v>
-      </c>
-      <c r="J95" s="126"/>
+        <v>43123</v>
+      </c>
+      <c r="J95" s="135"/>
+      <c r="K95" s="107"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A96" s="114">
+      <c r="A96" s="123">
         <v>94</v>
       </c>
-      <c r="B96" s="122"/>
+      <c r="B96" s="131"/>
       <c r="C96" s="52" t="s">
         <v>117</v>
       </c>
@@ -4244,13 +4349,13 @@
       <c r="G96" s="75"/>
       <c r="H96" s="56"/>
       <c r="I96" s="56"/>
-      <c r="J96" s="126"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" s="114">
+      <c r="J96" s="135"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="123">
         <v>95</v>
       </c>
-      <c r="B97" s="122"/>
+      <c r="B97" s="131"/>
       <c r="C97" s="52" t="s">
         <v>119</v>
       </c>
@@ -4260,13 +4365,13 @@
       <c r="G97" s="75"/>
       <c r="H97" s="56"/>
       <c r="I97" s="56"/>
-      <c r="J97" s="126"/>
-    </row>
-    <row r="98" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="115">
+      <c r="J97" s="135"/>
+    </row>
+    <row r="98" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="124">
         <v>96</v>
       </c>
-      <c r="B98" s="123"/>
+      <c r="B98" s="132"/>
       <c r="C98" s="51" t="s">
         <v>121</v>
       </c>
@@ -4276,13 +4381,13 @@
       <c r="G98" s="73"/>
       <c r="H98" s="55"/>
       <c r="I98" s="55"/>
-      <c r="J98" s="129"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" s="113">
+      <c r="J98" s="138"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" s="122">
         <v>97</v>
       </c>
-      <c r="B99" s="143" t="s">
+      <c r="B99" s="152" t="s">
         <v>101</v>
       </c>
       <c r="C99" s="59" t="s">
@@ -4292,27 +4397,28 @@
         <v>1</v>
       </c>
       <c r="E99" s="65">
-        <v>43126</v>
+        <v>43123</v>
       </c>
       <c r="F99" s="65">
-        <v>43126</v>
+        <v>43123</v>
       </c>
       <c r="G99" s="74">
         <v>1</v>
       </c>
       <c r="H99" s="65">
-        <v>43126</v>
+        <v>43123</v>
       </c>
       <c r="I99" s="65">
-        <v>43126</v>
-      </c>
-      <c r="J99" s="126"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="114">
+        <v>43123</v>
+      </c>
+      <c r="J99" s="135"/>
+      <c r="K99" s="107"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" s="123">
         <v>98</v>
       </c>
-      <c r="B100" s="144"/>
+      <c r="B100" s="153"/>
       <c r="C100" s="52" t="s">
         <v>117</v>
       </c>
@@ -4321,13 +4427,13 @@
       <c r="F100" s="56"/>
       <c r="G100" s="75"/>
       <c r="H100" s="56"/>
-      <c r="J100" s="126"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="114">
+      <c r="J100" s="135"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" s="123">
         <v>99</v>
       </c>
-      <c r="B101" s="144"/>
+      <c r="B101" s="153"/>
       <c r="C101" s="52" t="s">
         <v>119</v>
       </c>
@@ -4336,13 +4442,13 @@
       <c r="F101" s="56"/>
       <c r="G101" s="75"/>
       <c r="H101" s="56"/>
-      <c r="J101" s="126"/>
-    </row>
-    <row r="102" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="115">
+      <c r="J101" s="135"/>
+    </row>
+    <row r="102" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="124">
         <v>100</v>
       </c>
-      <c r="B102" s="145"/>
+      <c r="B102" s="154"/>
       <c r="C102" s="51" t="s">
         <v>121</v>
       </c>
@@ -4352,195 +4458,223 @@
       <c r="G102" s="73"/>
       <c r="H102" s="55"/>
       <c r="I102" s="55"/>
-      <c r="J102" s="129"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="113">
+      <c r="J102" s="138"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="162">
         <v>101</v>
       </c>
-      <c r="B103" s="143" t="s">
+      <c r="B103" s="152" t="s">
         <v>109</v>
       </c>
-      <c r="C103" s="52" t="s">
+      <c r="C103" s="114" t="s">
         <v>118</v>
       </c>
-      <c r="D103" s="88">
-        <v>1</v>
-      </c>
-      <c r="E103" s="65">
-        <v>43126</v>
-      </c>
-      <c r="F103" s="65">
-        <v>43126</v>
-      </c>
-      <c r="G103" s="74">
-        <v>1</v>
-      </c>
-      <c r="H103" s="65">
-        <v>43126</v>
-      </c>
-      <c r="I103" s="65">
-        <v>43126</v>
-      </c>
-      <c r="J103" s="125"/>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="114">
+      <c r="D103" s="96">
+        <v>1</v>
+      </c>
+      <c r="E103" s="111">
+        <v>43124</v>
+      </c>
+      <c r="F103" s="111">
+        <v>43124</v>
+      </c>
+      <c r="G103" s="105">
+        <v>1</v>
+      </c>
+      <c r="H103" s="111">
+        <v>43124</v>
+      </c>
+      <c r="I103" s="111">
+        <v>43124</v>
+      </c>
+      <c r="J103" s="148"/>
+      <c r="K103" s="107"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="163">
         <v>102</v>
       </c>
-      <c r="B104" s="144"/>
-      <c r="C104" s="52" t="s">
+      <c r="B104" s="153"/>
+      <c r="C104" s="114" t="s">
         <v>117</v>
       </c>
-      <c r="J104" s="126"/>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" s="114">
+      <c r="D104" s="164"/>
+      <c r="E104" s="165"/>
+      <c r="F104" s="165"/>
+      <c r="G104" s="166"/>
+      <c r="H104" s="165"/>
+      <c r="I104" s="165"/>
+      <c r="J104" s="149"/>
+      <c r="K104" s="112"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" s="163">
         <v>103</v>
       </c>
-      <c r="B105" s="144"/>
-      <c r="C105" s="52" t="s">
+      <c r="B105" s="153"/>
+      <c r="C105" s="114" t="s">
         <v>119</v>
       </c>
-      <c r="J105" s="126"/>
-    </row>
-    <row r="106" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="115">
+      <c r="D105" s="164"/>
+      <c r="E105" s="165"/>
+      <c r="F105" s="165"/>
+      <c r="G105" s="166"/>
+      <c r="H105" s="165"/>
+      <c r="I105" s="165"/>
+      <c r="J105" s="149"/>
+      <c r="K105" s="112"/>
+    </row>
+    <row r="106" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="167">
         <v>104</v>
       </c>
-      <c r="B106" s="145"/>
-      <c r="C106" s="51" t="s">
+      <c r="B106" s="154"/>
+      <c r="C106" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="D106" s="46"/>
-      <c r="E106" s="55"/>
-      <c r="F106" s="55"/>
-      <c r="G106" s="73"/>
-      <c r="H106" s="55"/>
-      <c r="I106" s="55"/>
-      <c r="J106" s="129"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="113">
+      <c r="D106" s="97"/>
+      <c r="E106" s="120"/>
+      <c r="F106" s="120"/>
+      <c r="G106" s="121"/>
+      <c r="H106" s="120"/>
+      <c r="I106" s="120"/>
+      <c r="J106" s="150"/>
+      <c r="K106" s="112"/>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" s="162">
         <v>105</v>
       </c>
-      <c r="B107" s="143" t="s">
-        <v>102</v>
-      </c>
-      <c r="C107" s="52" t="s">
+      <c r="B107" s="152" t="s">
+        <v>148</v>
+      </c>
+      <c r="C107" s="100" t="s">
         <v>118</v>
       </c>
-      <c r="D107" s="88">
+      <c r="D107" s="93">
         <v>1</v>
       </c>
       <c r="E107" s="65">
-        <v>43126</v>
+        <v>43124</v>
       </c>
       <c r="F107" s="65">
-        <v>43126</v>
+        <v>43124</v>
       </c>
       <c r="G107" s="74">
         <v>1</v>
       </c>
       <c r="H107" s="65">
-        <v>43126</v>
+        <v>43124</v>
       </c>
       <c r="I107" s="65">
-        <v>43126</v>
-      </c>
-      <c r="J107" s="126"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" s="114">
+        <v>43124</v>
+      </c>
+      <c r="J107" s="135"/>
+      <c r="K107" s="107"/>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108" s="163">
         <v>106</v>
       </c>
-      <c r="B108" s="144"/>
-      <c r="C108" s="52" t="s">
+      <c r="B108" s="153"/>
+      <c r="C108" s="100" t="s">
         <v>117</v>
       </c>
-      <c r="J108" s="126"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="114">
+      <c r="D108" s="94"/>
+      <c r="E108" s="101"/>
+      <c r="F108" s="101"/>
+      <c r="H108" s="101"/>
+      <c r="I108" s="101"/>
+      <c r="J108" s="135"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109" s="163">
         <v>107</v>
       </c>
-      <c r="B109" s="144"/>
-      <c r="C109" s="52" t="s">
+      <c r="B109" s="153"/>
+      <c r="C109" s="100" t="s">
         <v>119</v>
       </c>
-      <c r="J109" s="126"/>
-    </row>
-    <row r="110" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="115">
+      <c r="D109" s="94"/>
+      <c r="E109" s="101"/>
+      <c r="F109" s="101"/>
+      <c r="H109" s="101"/>
+      <c r="I109" s="101"/>
+      <c r="J109" s="135"/>
+    </row>
+    <row r="110" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="167">
         <v>108</v>
       </c>
-      <c r="B110" s="145"/>
+      <c r="B110" s="154"/>
       <c r="C110" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="D110" s="46"/>
+      <c r="D110" s="95"/>
       <c r="E110" s="55"/>
       <c r="F110" s="55"/>
       <c r="G110" s="73"/>
       <c r="H110" s="55"/>
       <c r="I110" s="55"/>
-      <c r="J110" s="129"/>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="113">
+      <c r="J110" s="138"/>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111" s="162">
         <v>109</v>
       </c>
-      <c r="B111" s="143" t="s">
-        <v>104</v>
+      <c r="B111" s="130" t="s">
+        <v>105</v>
       </c>
       <c r="C111" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D111" s="44">
+      <c r="D111" s="88">
         <v>1</v>
       </c>
       <c r="E111" s="65">
-        <v>43127</v>
+        <v>43125</v>
       </c>
       <c r="F111" s="65">
-        <v>43127</v>
+        <v>43125</v>
       </c>
       <c r="G111" s="74">
         <v>1</v>
       </c>
       <c r="H111" s="65">
-        <v>43127</v>
+        <v>43125</v>
       </c>
       <c r="I111" s="65">
-        <v>43127</v>
-      </c>
-      <c r="J111" s="126"/>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="114">
+        <v>43125</v>
+      </c>
+      <c r="J111" s="135"/>
+      <c r="K111" s="107"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112" s="163">
         <v>110</v>
       </c>
-      <c r="B112" s="144"/>
+      <c r="B112" s="131"/>
       <c r="C112" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="J112" s="126"/>
+      <c r="J112" s="135"/>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A113" s="114">
+      <c r="A113" s="163">
         <v>111</v>
       </c>
-      <c r="B113" s="144"/>
+      <c r="B113" s="131"/>
       <c r="C113" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="J113" s="126"/>
+      <c r="J113" s="135"/>
     </row>
     <row r="114" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="115">
+      <c r="A114" s="167">
         <v>112</v>
       </c>
-      <c r="B114" s="145"/>
+      <c r="B114" s="132"/>
       <c r="C114" s="51" t="s">
         <v>121</v>
       </c>
@@ -4550,75 +4684,64 @@
       <c r="G114" s="73"/>
       <c r="H114" s="55"/>
       <c r="I114" s="55"/>
-      <c r="J114" s="129"/>
+      <c r="J114" s="138"/>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A115" s="113">
+      <c r="A115" s="162">
         <v>113</v>
       </c>
-      <c r="B115" s="121" t="s">
-        <v>103</v>
-      </c>
-      <c r="C115" s="59" t="s">
+      <c r="B115" s="130" t="s">
+        <v>108</v>
+      </c>
+      <c r="C115" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D115" s="88">
+      <c r="D115" s="44">
         <v>1</v>
       </c>
       <c r="E115" s="65">
-        <v>43127</v>
+        <v>43125</v>
       </c>
       <c r="F115" s="65">
-        <v>43127</v>
+        <v>43125</v>
       </c>
       <c r="G115" s="74">
         <v>1</v>
       </c>
       <c r="H115" s="65">
-        <v>43127</v>
+        <v>43125</v>
       </c>
       <c r="I115" s="65">
-        <v>43127</v>
-      </c>
-      <c r="J115" s="126"/>
+        <v>43125</v>
+      </c>
+      <c r="J115" s="135"/>
+      <c r="K115" s="107"/>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A116" s="114">
+      <c r="A116" s="163">
         <v>114</v>
       </c>
-      <c r="B116" s="122"/>
+      <c r="B116" s="131"/>
       <c r="C116" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="D116" s="49"/>
-      <c r="E116" s="56"/>
-      <c r="F116" s="56"/>
-      <c r="G116" s="75"/>
-      <c r="H116" s="56"/>
-      <c r="I116" s="56"/>
-      <c r="J116" s="126"/>
+      <c r="J116" s="135"/>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" s="114">
+      <c r="A117" s="163">
         <v>115</v>
       </c>
-      <c r="B117" s="122"/>
+      <c r="B117" s="131"/>
       <c r="C117" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="D117" s="49"/>
-      <c r="E117" s="56"/>
-      <c r="F117" s="56"/>
-      <c r="G117" s="75"/>
-      <c r="H117" s="56"/>
-      <c r="I117" s="56"/>
-      <c r="J117" s="126"/>
+      <c r="J117" s="135"/>
     </row>
     <row r="118" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="115">
+      <c r="A118" s="167">
         <v>116</v>
       </c>
-      <c r="B118" s="123"/>
+      <c r="B118" s="132"/>
       <c r="C118" s="51" t="s">
         <v>121</v>
       </c>
@@ -4628,63 +4751,67 @@
       <c r="G118" s="73"/>
       <c r="H118" s="55"/>
       <c r="I118" s="55"/>
-      <c r="J118" s="129"/>
+      <c r="J118" s="138"/>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A119" s="113">
+      <c r="A119" s="162">
         <v>117</v>
       </c>
-      <c r="B119" s="121" t="s">
-        <v>105</v>
+      <c r="B119" s="152" t="s">
+        <v>104</v>
       </c>
       <c r="C119" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D119" s="88">
+      <c r="D119" s="44">
         <v>1</v>
       </c>
       <c r="E119" s="65">
-        <v>43127</v>
+        <v>43126</v>
       </c>
       <c r="F119" s="65">
-        <v>43127</v>
+        <v>43126</v>
       </c>
       <c r="G119" s="74">
         <v>1</v>
       </c>
       <c r="H119" s="65">
-        <v>43127</v>
+        <v>43126</v>
       </c>
       <c r="I119" s="65">
-        <v>43127</v>
-      </c>
-      <c r="J119" s="126"/>
+        <v>43126</v>
+      </c>
+      <c r="J119" s="135"/>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A120" s="114">
+      <c r="A120" s="163">
         <v>118</v>
       </c>
-      <c r="B120" s="122"/>
+      <c r="B120" s="153"/>
       <c r="C120" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="J120" s="126"/>
+      <c r="E120" s="101"/>
+      <c r="F120" s="101"/>
+      <c r="H120" s="101"/>
+      <c r="I120" s="101"/>
+      <c r="J120" s="135"/>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A121" s="114">
+      <c r="A121" s="163">
         <v>119</v>
       </c>
-      <c r="B121" s="122"/>
+      <c r="B121" s="153"/>
       <c r="C121" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="J121" s="126"/>
+      <c r="J121" s="135"/>
     </row>
     <row r="122" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="115">
+      <c r="A122" s="167">
         <v>120</v>
       </c>
-      <c r="B122" s="123"/>
+      <c r="B122" s="154"/>
       <c r="C122" s="51" t="s">
         <v>121</v>
       </c>
@@ -4694,63 +4821,75 @@
       <c r="G122" s="73"/>
       <c r="H122" s="55"/>
       <c r="I122" s="55"/>
-      <c r="J122" s="129"/>
+      <c r="J122" s="138"/>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A123" s="113">
+      <c r="A123" s="162">
         <v>121</v>
       </c>
-      <c r="B123" s="121" t="s">
-        <v>108</v>
-      </c>
-      <c r="C123" s="52" t="s">
+      <c r="B123" s="130" t="s">
+        <v>103</v>
+      </c>
+      <c r="C123" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="D123" s="44">
+      <c r="D123" s="88">
         <v>1</v>
       </c>
       <c r="E123" s="65">
-        <v>43129</v>
+        <v>43126</v>
       </c>
       <c r="F123" s="65">
-        <v>43129</v>
+        <v>43126</v>
       </c>
       <c r="G123" s="74">
         <v>1</v>
       </c>
       <c r="H123" s="65">
-        <v>43129</v>
+        <v>43126</v>
       </c>
       <c r="I123" s="65">
-        <v>43129</v>
-      </c>
-      <c r="J123" s="126"/>
+        <v>43126</v>
+      </c>
+      <c r="J123" s="135"/>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A124" s="114">
+      <c r="A124" s="163">
         <v>122</v>
       </c>
-      <c r="B124" s="122"/>
+      <c r="B124" s="131"/>
       <c r="C124" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="J124" s="126"/>
+      <c r="D124" s="49"/>
+      <c r="E124" s="56"/>
+      <c r="F124" s="56"/>
+      <c r="G124" s="75"/>
+      <c r="H124" s="56"/>
+      <c r="I124" s="56"/>
+      <c r="J124" s="135"/>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="114">
+      <c r="A125" s="163">
         <v>123</v>
       </c>
-      <c r="B125" s="122"/>
+      <c r="B125" s="131"/>
       <c r="C125" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="J125" s="126"/>
+      <c r="D125" s="49"/>
+      <c r="E125" s="56"/>
+      <c r="F125" s="56"/>
+      <c r="G125" s="75"/>
+      <c r="H125" s="56"/>
+      <c r="I125" s="56"/>
+      <c r="J125" s="135"/>
     </row>
     <row r="126" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="115">
+      <c r="A126" s="167">
         <v>124</v>
       </c>
-      <c r="B126" s="123"/>
+      <c r="B126" s="132"/>
       <c r="C126" s="51" t="s">
         <v>121</v>
       </c>
@@ -4760,151 +4899,151 @@
       <c r="G126" s="73"/>
       <c r="H126" s="55"/>
       <c r="I126" s="55"/>
-      <c r="J126" s="129"/>
+      <c r="J126" s="138"/>
     </row>
     <row r="127" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="113">
+      <c r="A127" s="162">
         <v>125</v>
       </c>
-      <c r="B127" s="121" t="s">
+      <c r="B127" s="168" t="s">
         <v>27</v>
       </c>
-      <c r="C127" s="59" t="s">
+      <c r="C127" s="99" t="s">
         <v>121</v>
       </c>
-      <c r="D127" s="44"/>
+      <c r="D127" s="93"/>
       <c r="E127" s="65"/>
       <c r="F127" s="65"/>
       <c r="G127" s="57"/>
       <c r="H127" s="70"/>
       <c r="I127" s="70"/>
-      <c r="J127" s="126"/>
-      <c r="K127" s="99"/>
+      <c r="J127" s="171"/>
+      <c r="K127" s="108"/>
     </row>
     <row r="128" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="114">
+      <c r="A128" s="163">
         <v>126</v>
       </c>
-      <c r="B128" s="122"/>
-      <c r="C128" s="52" t="s">
+      <c r="B128" s="169"/>
+      <c r="C128" s="100" t="s">
         <v>119</v>
       </c>
-      <c r="D128" s="49"/>
+      <c r="D128" s="98"/>
       <c r="E128" s="54"/>
       <c r="F128" s="58"/>
       <c r="G128" s="57"/>
       <c r="H128" s="71"/>
       <c r="I128" s="56"/>
-      <c r="J128" s="126"/>
-      <c r="K128" s="99"/>
+      <c r="J128" s="156"/>
+      <c r="K128" s="108"/>
     </row>
     <row r="129" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="114">
+      <c r="A129" s="163">
         <v>127</v>
       </c>
-      <c r="B129" s="122"/>
-      <c r="C129" s="52" t="s">
+      <c r="B129" s="169"/>
+      <c r="C129" s="100" t="s">
         <v>117</v>
       </c>
-      <c r="D129" s="49"/>
+      <c r="D129" s="98"/>
       <c r="E129" s="54"/>
       <c r="F129" s="58"/>
       <c r="G129" s="57"/>
       <c r="H129" s="71"/>
       <c r="I129" s="56"/>
-      <c r="J129" s="126"/>
-      <c r="K129" s="99"/>
+      <c r="J129" s="156"/>
+      <c r="K129" s="108"/>
     </row>
     <row r="130" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="115">
+      <c r="A130" s="167">
         <v>128</v>
       </c>
-      <c r="B130" s="123"/>
+      <c r="B130" s="170"/>
       <c r="C130" s="51" t="s">
         <v>118</v>
       </c>
-      <c r="D130" s="46"/>
+      <c r="D130" s="95"/>
       <c r="E130" s="64"/>
       <c r="F130" s="66"/>
       <c r="G130" s="73"/>
       <c r="H130" s="69"/>
       <c r="I130" s="55"/>
-      <c r="J130" s="129"/>
+      <c r="J130" s="172"/>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A131" s="113">
+      <c r="A131" s="162">
         <v>129</v>
       </c>
-      <c r="B131" s="143" t="s">
+      <c r="B131" s="173" t="s">
         <v>54</v>
       </c>
-      <c r="C131" s="59" t="s">
+      <c r="C131" s="99" t="s">
         <v>118</v>
       </c>
-      <c r="D131" s="44"/>
+      <c r="D131" s="93"/>
       <c r="E131" s="65"/>
       <c r="F131" s="65"/>
       <c r="G131" s="74"/>
       <c r="H131" s="65"/>
       <c r="I131" s="65"/>
-      <c r="J131" s="126"/>
+      <c r="J131" s="171"/>
       <c r="L131" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A132" s="114">
+      <c r="A132" s="163">
         <v>130</v>
       </c>
-      <c r="B132" s="144"/>
-      <c r="C132" s="52" t="s">
+      <c r="B132" s="174"/>
+      <c r="C132" s="100" t="s">
         <v>117</v>
       </c>
-      <c r="D132" s="49"/>
+      <c r="D132" s="98"/>
       <c r="E132" s="56"/>
       <c r="F132" s="56"/>
       <c r="G132" s="75"/>
       <c r="H132" s="56"/>
       <c r="I132" s="56"/>
-      <c r="J132" s="126"/>
+      <c r="J132" s="156"/>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A133" s="114">
+      <c r="A133" s="163">
         <v>131</v>
       </c>
-      <c r="B133" s="144"/>
-      <c r="C133" s="52" t="s">
+      <c r="B133" s="174"/>
+      <c r="C133" s="100" t="s">
         <v>119</v>
       </c>
-      <c r="D133" s="49"/>
+      <c r="D133" s="98"/>
       <c r="E133" s="56"/>
       <c r="F133" s="56"/>
       <c r="G133" s="75"/>
       <c r="H133" s="56"/>
       <c r="I133" s="56"/>
-      <c r="J133" s="126"/>
+      <c r="J133" s="156"/>
     </row>
     <row r="134" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="115">
+      <c r="A134" s="167">
         <v>132</v>
       </c>
-      <c r="B134" s="145"/>
+      <c r="B134" s="175"/>
       <c r="C134" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="D134" s="46"/>
+      <c r="D134" s="95"/>
       <c r="E134" s="55"/>
       <c r="F134" s="55"/>
       <c r="G134" s="73"/>
       <c r="H134" s="55"/>
       <c r="I134" s="55"/>
-      <c r="J134" s="129"/>
+      <c r="J134" s="172"/>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A135" s="113">
+      <c r="A135" s="162">
         <v>133</v>
       </c>
-      <c r="B135" s="121" t="s">
+      <c r="B135" s="130" t="s">
         <v>55</v>
       </c>
       <c r="C135" s="59" t="s">
@@ -4916,16 +5055,16 @@
       <c r="G135" s="74"/>
       <c r="H135" s="65"/>
       <c r="I135" s="65"/>
-      <c r="J135" s="126"/>
+      <c r="J135" s="135"/>
       <c r="L135" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A136" s="114">
+      <c r="A136" s="163">
         <v>134</v>
       </c>
-      <c r="B136" s="122"/>
+      <c r="B136" s="131"/>
       <c r="C136" s="52" t="s">
         <v>117</v>
       </c>
@@ -4935,13 +5074,13 @@
       <c r="G136" s="75"/>
       <c r="H136" s="56"/>
       <c r="I136" s="56"/>
-      <c r="J136" s="126"/>
+      <c r="J136" s="135"/>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A137" s="114">
+      <c r="A137" s="163">
         <v>135</v>
       </c>
-      <c r="B137" s="122"/>
+      <c r="B137" s="131"/>
       <c r="C137" s="52" t="s">
         <v>119</v>
       </c>
@@ -4951,13 +5090,13 @@
       <c r="G137" s="75"/>
       <c r="H137" s="56"/>
       <c r="I137" s="56"/>
-      <c r="J137" s="126"/>
+      <c r="J137" s="135"/>
     </row>
     <row r="138" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="115">
+      <c r="A138" s="167">
         <v>136</v>
       </c>
-      <c r="B138" s="123"/>
+      <c r="B138" s="132"/>
       <c r="C138" s="51" t="s">
         <v>121</v>
       </c>
@@ -4967,13 +5106,13 @@
       <c r="G138" s="73"/>
       <c r="H138" s="55"/>
       <c r="I138" s="55"/>
-      <c r="J138" s="129"/>
+      <c r="J138" s="138"/>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A139" s="113">
+      <c r="A139" s="162">
         <v>137</v>
       </c>
-      <c r="B139" s="149" t="s">
+      <c r="B139" s="158" t="s">
         <v>84</v>
       </c>
       <c r="C139" s="59" t="s">
@@ -4985,13 +5124,13 @@
       <c r="G139" s="74"/>
       <c r="H139" s="65"/>
       <c r="I139" s="65"/>
-      <c r="J139" s="126"/>
+      <c r="J139" s="135"/>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A140" s="114">
+      <c r="A140" s="163">
         <v>138</v>
       </c>
-      <c r="B140" s="150"/>
+      <c r="B140" s="159"/>
       <c r="C140" s="52" t="s">
         <v>117</v>
       </c>
@@ -5001,13 +5140,13 @@
       <c r="G140" s="75"/>
       <c r="H140" s="56"/>
       <c r="I140" s="56"/>
-      <c r="J140" s="126"/>
+      <c r="J140" s="135"/>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A141" s="114">
+      <c r="A141" s="163">
         <v>139</v>
       </c>
-      <c r="B141" s="151" t="s">
+      <c r="B141" s="160" t="s">
         <v>134</v>
       </c>
       <c r="C141" s="52" t="s">
@@ -5019,13 +5158,13 @@
       <c r="G141" s="75"/>
       <c r="H141" s="56"/>
       <c r="I141" s="56"/>
-      <c r="J141" s="126"/>
+      <c r="J141" s="135"/>
     </row>
     <row r="142" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="115">
+      <c r="A142" s="167">
         <v>140</v>
       </c>
-      <c r="B142" s="152"/>
+      <c r="B142" s="161"/>
       <c r="C142" s="51" t="s">
         <v>121</v>
       </c>
@@ -5035,13 +5174,13 @@
       <c r="G142" s="73"/>
       <c r="H142" s="55"/>
       <c r="I142" s="55"/>
-      <c r="J142" s="129"/>
+      <c r="J142" s="138"/>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A143" s="113">
+      <c r="A143" s="162">
         <v>141</v>
       </c>
-      <c r="B143" s="149" t="s">
+      <c r="B143" s="158" t="s">
         <v>43</v>
       </c>
       <c r="C143" s="59" t="s">
@@ -5053,16 +5192,16 @@
       <c r="G143" s="74"/>
       <c r="H143" s="65"/>
       <c r="I143" s="65"/>
-      <c r="J143" s="126"/>
+      <c r="J143" s="135"/>
       <c r="L143" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A144" s="114">
+      <c r="A144" s="163">
         <v>142</v>
       </c>
-      <c r="B144" s="150"/>
+      <c r="B144" s="159"/>
       <c r="C144" s="52" t="s">
         <v>117</v>
       </c>
@@ -5072,13 +5211,13 @@
       <c r="G144" s="75"/>
       <c r="H144" s="56"/>
       <c r="I144" s="56"/>
-      <c r="J144" s="126"/>
+      <c r="J144" s="135"/>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A145" s="114">
+      <c r="A145" s="163">
         <v>143</v>
       </c>
-      <c r="B145" s="151" t="s">
+      <c r="B145" s="160" t="s">
         <v>134</v>
       </c>
       <c r="C145" s="52" t="s">
@@ -5090,13 +5229,13 @@
       <c r="G145" s="75"/>
       <c r="H145" s="56"/>
       <c r="I145" s="56"/>
-      <c r="J145" s="126"/>
+      <c r="J145" s="135"/>
     </row>
     <row r="146" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="115">
+      <c r="A146" s="167">
         <v>144</v>
       </c>
-      <c r="B146" s="152"/>
+      <c r="B146" s="161"/>
       <c r="C146" s="51" t="s">
         <v>121</v>
       </c>
@@ -5106,13 +5245,13 @@
       <c r="G146" s="73"/>
       <c r="H146" s="55"/>
       <c r="I146" s="55"/>
-      <c r="J146" s="129"/>
+      <c r="J146" s="138"/>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A147" s="113">
+      <c r="A147" s="162">
         <v>145</v>
       </c>
-      <c r="B147" s="121" t="s">
+      <c r="B147" s="130" t="s">
         <v>15</v>
       </c>
       <c r="C147" s="59" t="s">
@@ -5134,13 +5273,13 @@
       <c r="I147" s="65">
         <v>43125</v>
       </c>
-      <c r="J147" s="126"/>
+      <c r="J147" s="135"/>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A148" s="114">
+      <c r="A148" s="163">
         <v>146</v>
       </c>
-      <c r="B148" s="122"/>
+      <c r="B148" s="131"/>
       <c r="C148" s="52" t="s">
         <v>117</v>
       </c>
@@ -5150,13 +5289,13 @@
       <c r="G148" s="75"/>
       <c r="H148" s="56"/>
       <c r="I148" s="56"/>
-      <c r="J148" s="126"/>
+      <c r="J148" s="135"/>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A149" s="114">
+      <c r="A149" s="163">
         <v>147</v>
       </c>
-      <c r="B149" s="122"/>
+      <c r="B149" s="131"/>
       <c r="C149" s="52" t="s">
         <v>119</v>
       </c>
@@ -5166,13 +5305,13 @@
       <c r="G149" s="75"/>
       <c r="H149" s="56"/>
       <c r="I149" s="56"/>
-      <c r="J149" s="126"/>
+      <c r="J149" s="135"/>
     </row>
     <row r="150" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="115">
+      <c r="A150" s="167">
         <v>148</v>
       </c>
-      <c r="B150" s="123"/>
+      <c r="B150" s="132"/>
       <c r="C150" s="51" t="s">
         <v>121</v>
       </c>
@@ -5182,7 +5321,7 @@
       <c r="G150" s="73"/>
       <c r="H150" s="55"/>
       <c r="I150" s="55"/>
-      <c r="J150" s="129"/>
+      <c r="J150" s="138"/>
     </row>
   </sheetData>
   <mergeCells count="82">
@@ -5198,8 +5337,8 @@
     <mergeCell ref="B135:B138"/>
     <mergeCell ref="B99:B102"/>
     <mergeCell ref="B145:B146"/>
-    <mergeCell ref="B119:B122"/>
-    <mergeCell ref="B123:B126"/>
+    <mergeCell ref="B111:B114"/>
+    <mergeCell ref="B115:B118"/>
     <mergeCell ref="B103:B106"/>
     <mergeCell ref="J139:J142"/>
     <mergeCell ref="J127:J130"/>
@@ -5207,19 +5346,19 @@
     <mergeCell ref="J131:J134"/>
     <mergeCell ref="J135:J138"/>
     <mergeCell ref="J87:J90"/>
-    <mergeCell ref="J119:J122"/>
-    <mergeCell ref="J123:J126"/>
+    <mergeCell ref="J111:J114"/>
+    <mergeCell ref="J115:J118"/>
     <mergeCell ref="J103:J106"/>
     <mergeCell ref="B143:B144"/>
     <mergeCell ref="J99:J102"/>
-    <mergeCell ref="J115:J118"/>
+    <mergeCell ref="J123:J126"/>
     <mergeCell ref="J107:J110"/>
-    <mergeCell ref="J111:J114"/>
+    <mergeCell ref="J119:J122"/>
     <mergeCell ref="B139:B140"/>
     <mergeCell ref="B141:B142"/>
-    <mergeCell ref="B115:B118"/>
+    <mergeCell ref="B123:B126"/>
     <mergeCell ref="B107:B110"/>
-    <mergeCell ref="B111:B114"/>
+    <mergeCell ref="B119:B122"/>
     <mergeCell ref="J47:J50"/>
     <mergeCell ref="J51:J54"/>
     <mergeCell ref="J55:J58"/>
@@ -5290,26 +5429,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="136" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="148" t="s">
+      <c r="D1" s="157" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="148"/>
+      <c r="E1" s="157"/>
       <c r="F1" s="47" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="128"/>
-      <c r="B2" s="128"/>
+      <c r="A2" s="137"/>
+      <c r="B2" s="137"/>
       <c r="C2" s="46" t="s">
         <v>122</v>
       </c>
@@ -5324,7 +5463,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="125" t="s">
+      <c r="A3" s="134" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -5341,7 +5480,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="126"/>
+      <c r="A4" s="135"/>
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
@@ -5350,7 +5489,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="126"/>
+      <c r="A5" s="135"/>
       <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
@@ -5359,7 +5498,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="126"/>
+      <c r="A6" s="135"/>
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
@@ -5368,7 +5507,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="126"/>
+      <c r="A7" s="135"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
@@ -5377,7 +5516,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="126"/>
+      <c r="A8" s="135"/>
       <c r="B8" s="8" t="s">
         <v>115</v>
       </c>
@@ -5389,7 +5528,7 @@
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="125" t="s">
+      <c r="A9" s="134" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -5397,13 +5536,13 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="126"/>
+      <c r="A10" s="135"/>
       <c r="B10" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="129"/>
+      <c r="A11" s="138"/>
       <c r="B11" s="12" t="s">
         <v>20</v>
       </c>
@@ -5433,7 +5572,7 @@
       <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="125" t="s">
+      <c r="A14" s="134" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="42" t="s">
@@ -5441,13 +5580,13 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="126"/>
+      <c r="A15" s="135"/>
       <c r="B15" s="42" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="129"/>
+      <c r="A16" s="138"/>
       <c r="B16" s="43" t="s">
         <v>32</v>
       </c>
@@ -5457,7 +5596,7 @@
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="125" t="s">
+      <c r="A17" s="134" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -5465,25 +5604,25 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="138"/>
+      <c r="A18" s="147"/>
       <c r="B18" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="138"/>
+      <c r="A19" s="147"/>
       <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="138"/>
+      <c r="A20" s="147"/>
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="129"/>
+      <c r="A21" s="138"/>
       <c r="B21" s="19" t="s">
         <v>40</v>
       </c>
@@ -5529,7 +5668,7 @@
       <c r="F24" s="15"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="134" t="s">
+      <c r="A25" s="143" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -5537,13 +5676,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="135"/>
+      <c r="A26" s="144"/>
       <c r="B26" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="136"/>
+      <c r="A27" s="145"/>
       <c r="B27" s="19" t="s">
         <v>53</v>
       </c>
@@ -5565,7 +5704,7 @@
       <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="134" t="s">
+      <c r="A29" s="143" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -5573,33 +5712,33 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="137"/>
+      <c r="A30" s="146"/>
       <c r="B30" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="137"/>
-      <c r="B31" s="132" t="s">
+      <c r="A31" s="146"/>
+      <c r="B31" s="141" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="137"/>
-      <c r="B32" s="132"/>
+      <c r="A32" s="146"/>
+      <c r="B32" s="141"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="137"/>
-      <c r="B33" s="132" t="s">
+      <c r="A33" s="146"/>
+      <c r="B33" s="141" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="137"/>
-      <c r="B34" s="132"/>
+      <c r="A34" s="146"/>
+      <c r="B34" s="141"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="136"/>
+      <c r="A35" s="145"/>
       <c r="B35" s="9" t="s">
         <v>59</v>
       </c>
@@ -5621,7 +5760,7 @@
       <c r="F36" s="15"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="134" t="s">
+      <c r="A37" s="143" t="s">
         <v>76</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -5629,19 +5768,19 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="135"/>
+      <c r="A38" s="144"/>
       <c r="B38" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="135"/>
+      <c r="A39" s="144"/>
       <c r="B39" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="135"/>
+      <c r="A40" s="144"/>
       <c r="B40" s="3" t="s">
         <v>80</v>
       </c>
@@ -5663,7 +5802,7 @@
       <c r="F41" s="15"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="134" t="s">
+      <c r="A42" s="143" t="s">
         <v>92</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -5671,7 +5810,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="136"/>
+      <c r="A43" s="145"/>
       <c r="B43" s="8" t="s">
         <v>87</v>
       </c>
@@ -5681,7 +5820,7 @@
       <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="134" t="s">
+      <c r="A44" s="143" t="s">
         <v>93</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -5689,25 +5828,25 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="135"/>
+      <c r="A45" s="144"/>
       <c r="B45" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="135"/>
+      <c r="A46" s="144"/>
       <c r="B46" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="135"/>
+      <c r="A47" s="144"/>
       <c r="B47" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="136"/>
+      <c r="A48" s="145"/>
       <c r="B48" s="9" t="s">
         <v>86</v>
       </c>
@@ -5717,7 +5856,7 @@
       <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="134" t="s">
+      <c r="A49" s="143" t="s">
         <v>97</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -5725,13 +5864,13 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="135"/>
+      <c r="A50" s="144"/>
       <c r="B50" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="136"/>
+      <c r="A51" s="145"/>
       <c r="B51" s="8" t="s">
         <v>98</v>
       </c>

</xml_diff>